<commit_message>
Added microenvironment assay to MCDS2ISA_DB script, updated relationships xlsx to accomodate change
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621BC8E3-05E8-4765-AF80-6C172E1C2476}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE53F8E-C709-4735-859E-C0DF130325E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
-    <sheet name="Assays" sheetId="3" r:id="rId2"/>
-    <sheet name="ISA-Tab to MCDS-DCL" sheetId="2" r:id="rId3"/>
+    <sheet name="A_Microenvironment" sheetId="4" r:id="rId2"/>
+    <sheet name="Assays" sheetId="3" r:id="rId3"/>
+    <sheet name="ISA-Tab to MCDS-DCL" sheetId="2" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
+  <definedNames>
+    <definedName name="B">A_Microenvironment!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="240">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -416,54 +417,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>/MultiCellDS/cell_line/metadata/MultiCellDB/ID</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/MultiCellDB/name</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/description</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/citation/text</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/citation/notes</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/data_origins/data_origin/citation/PMID, /MultiCellDS/cell_line/metadata/data_analysis/citation/PMID</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/data_origins/data_origin/citation/DOI, /MultiCellDS/cell_line/metadata/data_analysis/citation/DOI</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/family-name</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/given-names</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/email</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/url</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/phenotype_dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/MultiCellDS/cell_line/phenotype_dataset/microenvironment </t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/phenotype_dataset/microenvironment/domain/variables/variable(s) [attr. (name).(type)]</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/creator/orcid-identifier/family-name, /MultiCellDS/cell_line/metadata/curation/curator/orcid-identifier/family-name, /MultiCellDS/cell_line/metadata/curation/last_modified_by/orcid-identifier/family-name, /MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/family-name</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/creator/orcid-identifier/given-names, /MultiCellDS/cell_line/metadata/curation/curator/orcid-identifier/given-names, /MultiCellDS/cell_line/metadata/curation/last_modified_by/orcid-identifier/given-names, /MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/given-names</t>
-  </si>
-  <si>
     <t>Text Entry</t>
   </si>
   <si>
@@ -488,9 +441,6 @@
     <t>current_contact</t>
   </si>
   <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/creator/orcid-identifier/email, /MultiCellDS/cell_line/metadata/curation/curator/orcid-identifier/email, /MultiCellDS/cell_line/metadata/curation/last_modified_by/orcid-identifier/email, /MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/email</t>
-  </si>
-  <si>
     <t>Multiples for xPath</t>
   </si>
   <si>
@@ -500,39 +450,9 @@
     <t>organization-name &amp; department-name</t>
   </si>
   <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/organization-name &amp; /MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/department-name</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/creator/orcid-identifier/organization-name &amp; /MultiCellDS/cell_line/metadata/curation/creator/orcid-identifier/department-name, /MultiCellDS/cell_line/metadata/curation/curator/orcid-identifier/organization-name &amp; /MultiCellDS/cell_line/metadata/curation/curator/orcid-identifier/department-name, /MultiCellDS/cell_line/metadata/curation/last_modified_by/orcid-identifier/organization-name &amp; /MultiCellDS/cell_line/metadata/curation/last_modified_by/orcid-identifier/department-name, /MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/organization-name &amp; /MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/department-name</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/creator/orcid-identifier/family-name**, /MultiCellDS/cell_line/metadata/curation/curator/orcid-identifier/family-name**, /MultiCellDS/cell_line/metadata/curation/last_modified_by/orcid-identifier/family-name**, /MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/family-name**</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/family-name**</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/rights/license</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/rights/license/licenseDocument</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/rights/license/licenseDocument/name</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/rights/license/licenseDocument/URL</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>licenseDocument</t>
-  </si>
-  <si>
-    <t>license</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -542,42 +462,21 @@
     <t>url</t>
   </si>
   <si>
-    <t>/MultiCellDS/cell_line/metadata/curation/creator/orcid-identifier/url, /MultiCellDS/cell_line/metadata/curation/curator/orcid-identifier/url, /MultiCellDS/cell_line/metadata/curation/last_modified_by/orcid-identifier/url, /MultiCellDS/cell_line/metadata/curation/current_contact/orcid-identifier/url</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>text</t>
   </si>
   <si>
-    <t xml:space="preserve">/MultiCellDS/cell_line/metadata/data_origins/data_origin/citation/DOI, /MultiCellDS/cell_line/metadata/data_analysis/citation/DOI, </t>
-  </si>
-  <si>
     <t>Comment[notes]</t>
   </si>
   <si>
-    <t>/MultiCellDS/cell_line/metadata/notes</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/cell_origin/custom/company/name</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/citation, /MultiCellDS/cell_line/metadata/citation/text</t>
-  </si>
-  <si>
     <t>citation</t>
   </si>
   <si>
     <t>Comment[Cell Line Citation Notes]</t>
   </si>
   <si>
-    <t>Comment[License]</t>
-  </si>
-  <si>
-    <t>Comment[License Document]</t>
-  </si>
-  <si>
     <t>Comment[License Name]</t>
   </si>
   <si>
@@ -590,21 +489,12 @@
     <t>Comment[Study PMCID]</t>
   </si>
   <si>
-    <t>/MultiCellDS/cell_line/metadata/data_origins/data_origin/citation/PMCID, /MultiCellDS/cell_line/metadata/data_analysis/citation/PMCID</t>
-  </si>
-  <si>
-    <t>/MultiCellDS/cell_line/metadata/data_origins/data_origin/citation</t>
-  </si>
-  <si>
     <t>Comment[Study Data URL]</t>
   </si>
   <si>
     <t>PMCID</t>
   </si>
   <si>
-    <t>/MultiCellDS/cell_line/metadata/data_origins/data_origin/citation/URL, /MultiCellDS/cell_line/metadata/data_analysis/URL, /MultiCellDS/cell_line/metadata/data_analysis/citation/URL</t>
-  </si>
-  <si>
     <t>Sample Name</t>
   </si>
   <si>
@@ -632,9 +522,6 @@
     <t>cell_part[name]</t>
   </si>
   <si>
-    <t>/MultiCellDS/cell_line/phenotype_dataset[@Keywords]</t>
-  </si>
-  <si>
     <t>Cell_Microenvironment</t>
   </si>
   <si>
@@ -680,10 +567,199 @@
     <t>Assay name, variable name, or No</t>
   </si>
   <si>
-    <t>Multiple - 94</t>
-  </si>
-  <si>
     <t>Parameter Value[oxygen.concentration]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/MultiCellDB/ID</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/MultiCellDB/name</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/notes</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/description</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/citation/notes</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/citation/text</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/rights/license/LicenseDocument/name</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/rights/license/LicenseDocument/URL</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/data_origins/data_origin/citation/DOI, cell_line/metadata/data_analysis/citation/DOI</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/citation, cell_line/metadata/citation/text</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/family-name</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/given-names</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/email</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/url</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/organization-name &amp; cell_line/metadata/curation/current_contact/orcid-identifier/department-name</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/family-name**</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/data_origins/data_origin/citation/PMID, cell_line/metadata/data_analysis/citation/PMID</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/data_origins/data_origin/citation</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/data_origins/data_origin/citation/PMCID, cell_line/metadata/data_analysis/citation/PMCID</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/data_origins/data_origin/citation/URL, cell_line/metadata/data_analysis/URL, cell_line/metadata/data_analysis/citation/URL</t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset[@Keywords]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/custom/company/name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_line/phenotype_dataset/microenvironment </t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset/microenvironment/domain/variables/variable(s) [attr. (name).(type)]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/family-name, cell_line/metadata/curation/curator/orcid-identifier/family-name, cell_line/metadata/curation/creator/orcid-identifier/family-name,  cell_line/metadata/curation/last_modified_by/orcid-identifier/family-name</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/given-names, cell_line/metadata/curation/curator/orcid-identifier/given-names, cell_line/metadata/curation/creator/orcid-identifier/given-names, cell_line/metadata/curation/last_modified_by/orcid-identifier/given-names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_line/metadata/curation/current_contact/orcid-identifier/email, cell_line/metadata/curation/curator/orcid-identifier/email, cell_line/metadata/curation/creator/orcid-identifier/email,  cell_line/metadata/curation/last_modified_by/orcid-identifier/email </t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/url, cell_line/metadata/curation/curator/orcid-identifier/url, cell_line/metadata/curation/creator/orcid-identifier/url,  cell_line/metadata/curation/last_modified_by/orcid-identifier/url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_line/metadata/curation/current_contact/orcid-identifier/family-name**, cell_line/metadata/curation/curator/orcid-identifier/family-name**, cell_line/metadata/curation/creator/orcid-identifier/family-name**,  cell_line/metadata/curation/last_modified_by/orcid-identifier/family-name** </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_line/metadata/curation/current_contact/orcid-identifier/organization-name" - "cell_line/metadata/curation/current_contact/orcid-identifier/department-name, cell_line/metadata/curation/curator/orcid-identifier/organization-name" - "cell_line/metadata/curation/curator/orcid-identifier/department-name, cell_line/metadata/curation/creator/orcid-identifier/organization-name" - "cell_line/metadata/curation/creator/orcid-identifier/department-name,  cell_line/metadata/curation/last_modified_by/orcid-identifier/organization-name" - "cell_line/metadata/curation/last_modified_by/orcid-identifier/department-name </t>
+  </si>
+  <si>
+    <t>Multiple - Study Person Last Name</t>
+  </si>
+  <si>
+    <t>/material_amount[@max]</t>
+  </si>
+  <si>
+    <t>/material_amount[@min]</t>
+  </si>
+  <si>
+    <t>/material_amount[@range]</t>
+  </si>
+  <si>
+    <t>/material_amount[@standard_deviation]</t>
+  </si>
+  <si>
+    <t>/material_amount[@uncertainty]</t>
+  </si>
+  <si>
+    <t>[@ChEBI_ID]</t>
+  </si>
+  <si>
+    <t>[@GO_ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Surface Variable MeSH ID]</t>
+  </si>
+  <si>
+    <t>domain/experimental_condition/surface_variable[@MeSH_ID]</t>
+  </si>
+  <si>
+    <t>[@MeSH_ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Surface Variable ChEBI ID]</t>
+  </si>
+  <si>
+    <t>domain/experimental_condition/surface_variable[@ChEBI_ID]</t>
+  </si>
+  <si>
+    <t>[@PR_ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Surface Variable Name]</t>
+  </si>
+  <si>
+    <t>domain/experimental_condition/surface_variable[@name]</t>
+  </si>
+  <si>
+    <t>[@UniProt_ID]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Experiment Dimensionality]</t>
+  </si>
+  <si>
+    <t>domain/experimental_condition/dimensionality</t>
+  </si>
+  <si>
+    <t>/material_amount[@units]</t>
+  </si>
+  <si>
+    <t>Characteristic[Experiment System]</t>
+  </si>
+  <si>
+    <t>domain/experimental_condition/system</t>
+  </si>
+  <si>
+    <t>/material_amount[@measurement_type]</t>
+  </si>
+  <si>
+    <t>Temperature Units</t>
+  </si>
+  <si>
+    <t>domain/variables/physical_parameter_set/conditions/temperature[@units]</t>
+  </si>
+  <si>
+    <t>[@type]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Temperature]</t>
+  </si>
+  <si>
+    <t>domain/variables/physical_parameter_set/conditions/temperature</t>
+  </si>
+  <si>
+    <t>[@units]</t>
+  </si>
+  <si>
+    <t>After the script finds each named variable within the microenvironment field, each microenvironment variable element will be searched for at the xPaths at which the named variables were found. The microenvironment condition element gives xPaths outside of the /variables/variable pathway to search. ISA Condition Entities is the corresponding name used in the Microenvironment Assay .txt file for the values found at the adjacent Condition xPaths</t>
+  </si>
+  <si>
+    <t>ISA Condition Entities</t>
+  </si>
+  <si>
+    <t>Microenvironment Condition xPaths</t>
+  </si>
+  <si>
+    <t>Microenvironment Variable xPaths</t>
+  </si>
+  <si>
+    <t>Column Explanation</t>
   </si>
 </sst>
 </file>
@@ -730,7 +806,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -755,8 +831,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -784,11 +866,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -816,6 +970,37 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,42 +1073,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Parent + dup xPath removed"/>
-      <sheetName val="Assay Information"/>
-      <sheetName val="A_MicroEnvironment"/>
-      <sheetName val="Use in ISA files"/>
-      <sheetName val="All Elem + Attr"/>
-      <sheetName val="Entities in discrete files"/>
-      <sheetName val="Both Elem + Attr"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>/MultiCellDS/cell_line/phenotype_dataset/microenvironment/domain/variables/variable[@units]</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>/MultiCellDS/cell_line/phenotype_dataset/microenvironment/domain/variables/variable[@ChEBI_ID]</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1223,18 +1372,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FA11B-2D6D-4A50-A5F1-7D079DCC0D36}">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E89" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="55.28515625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="54.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="48" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" style="2" customWidth="1"/>
     <col min="6" max="7" width="98.7109375" style="5" customWidth="1"/>
     <col min="8" max="8" width="14" style="5" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
@@ -1244,7 +1394,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1262,7 +1412,7 @@
         <v>106</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>113</v>
@@ -1306,13 +1456,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>114</v>
@@ -1336,13 +1486,13 @@
         <v>3</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>114</v>
@@ -1366,13 +1516,13 @@
         <v>3</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>114</v>
@@ -1396,13 +1546,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>114</v>
@@ -1446,11 +1596,11 @@
       <c r="E8" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>125</v>
+      <c r="F8" t="s">
+        <v>176</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>115</v>
@@ -1471,13 +1621,13 @@
         <v>3</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>126</v>
+        <v>136</v>
+      </c>
+      <c r="F9" t="s">
+        <v>177</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>115</v>
@@ -1498,13 +1648,13 @@
         <v>3</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>127</v>
+        <v>138</v>
+      </c>
+      <c r="F10" t="s">
+        <v>179</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>115</v>
@@ -1556,7 +1706,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
@@ -1565,13 +1715,13 @@
         <v>3</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>172</v>
+        <v>137</v>
+      </c>
+      <c r="F13" t="s">
+        <v>178</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1580,7 +1730,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
@@ -1589,13 +1739,13 @@
         <v>3</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="F14" t="s">
+        <v>181</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>115</v>
@@ -1610,7 +1760,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -1619,13 +1769,13 @@
         <v>3</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>129</v>
+        <v>137</v>
+      </c>
+      <c r="F15" t="s">
+        <v>180</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>115</v>
@@ -1640,7 +1790,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -1649,16 +1799,16 @@
         <v>3</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>157</v>
+        <v>136</v>
+      </c>
+      <c r="F16" t="s">
+        <v>182</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1667,7 +1817,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -1676,16 +1826,16 @@
         <v>3</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>158</v>
+        <v>124</v>
+      </c>
+      <c r="F17" t="s">
+        <v>183</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1693,27 +1843,19 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>179</v>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>168</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -1721,7 +1863,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>180</v>
+        <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -1730,16 +1872,14 @@
         <v>3</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>160</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F19" s="6"/>
       <c r="G19" s="5" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>168</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,19 +1887,27 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>16</v>
+      <c r="B20" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -1767,7 +1915,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -1775,15 +1923,11 @@
       <c r="D21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="E21" s="4"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="5" t="s">
-        <v>146</v>
-      </c>
+      <c r="G21" s="6"/>
       <c r="H21" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1791,8 +1935,8 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>18</v>
+      <c r="B22" s="20" t="s">
+        <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -1801,16 +1945,16 @@
         <v>3</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>146</v>
+        <v>185</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1819,7 +1963,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -1831,7 +1975,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1839,8 +1983,8 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="20" t="s">
-        <v>20</v>
+      <c r="B24" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -1848,17 +1992,11 @@
       <c r="D24" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>146</v>
-      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1867,7 +2005,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -1887,21 +2025,19 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>22</v>
+      <c r="B26" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6" t="s">
-        <v>117</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -1909,7 +2045,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>4</v>
@@ -1917,11 +2053,17 @@
       <c r="D27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
+      <c r="E27" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="H27" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1929,19 +2071,27 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>24</v>
+      <c r="B28" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -1949,7 +2099,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>4</v>
@@ -1957,17 +2107,13 @@
       <c r="D29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1976,7 +2122,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -1985,13 +2131,13 @@
         <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>133</v>
+        <v>188</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>115</v>
@@ -2003,7 +2149,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -2014,7 +2160,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>116</v>
@@ -2026,7 +2172,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>4</v>
@@ -2034,17 +2180,13 @@
       <c r="D32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>134</v>
-      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="6"/>
       <c r="G32" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2053,7 +2195,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>4</v>
@@ -2061,14 +2203,21 @@
       <c r="D33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="6"/>
+      <c r="E33" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>189</v>
+      </c>
       <c r="G33" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>116</v>
       </c>
+      <c r="I33" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -2076,7 +2225,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>4</v>
@@ -2084,13 +2233,20 @@
       <c r="D34" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="6"/>
+      <c r="E34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>190</v>
+      </c>
       <c r="G34" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2099,7 +2255,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -2108,20 +2264,17 @@
         <v>3</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>135</v>
+        <v>191</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="I35" s="4" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -2129,7 +2282,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -2137,20 +2290,13 @@
       <c r="D36" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>153</v>
-      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="6"/>
       <c r="G36" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2159,7 +2305,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -2167,104 +2313,104 @@
       <c r="D37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>146</v>
-      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
       <c r="H37" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="B38" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6" t="s">
-        <v>146</v>
-      </c>
+      <c r="D38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="17"/>
       <c r="H38" s="6" t="s">
         <v>116</v>
       </c>
+      <c r="I38"/>
+      <c r="J38"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>35</v>
+      <c r="B39" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="17"/>
+      <c r="B40" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="H40" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="I40"/>
-      <c r="J40"/>
+        <v>115</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>37</v>
+      <c r="B41" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41" s="14"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -2272,7 +2418,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>104</v>
@@ -2282,10 +2428,10 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6" t="s">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>115</v>
@@ -2297,7 +2443,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>104</v>
@@ -2306,14 +2452,10 @@
         <v>3</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>146</v>
-      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
       <c r="H43" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -2322,7 +2464,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>104</v>
@@ -2331,14 +2473,10 @@
         <v>3</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>146</v>
-      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
       <c r="H44" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2347,7 +2485,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>104</v>
@@ -2359,7 +2497,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2368,7 +2506,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>104</v>
@@ -2389,7 +2527,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>104</v>
@@ -2401,7 +2539,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -2409,21 +2547,19 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>41</v>
+      <c r="B48" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6" t="s">
-        <v>116</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E48" s="14"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
@@ -2431,7 +2567,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>104</v>
@@ -2451,19 +2587,21 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>46</v>
+      <c r="B50" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="14"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E50" s="4"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
@@ -2471,7 +2609,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>104</v>
@@ -2491,21 +2629,19 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>48</v>
+      <c r="B52" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E52" s="4"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6" t="s">
-        <v>116</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E52" s="14"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
@@ -2513,7 +2649,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>104</v>
@@ -2521,11 +2657,17 @@
       <c r="D53" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
+      <c r="E53" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="H53" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -2533,19 +2675,27 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>50</v>
+      <c r="B54" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E54" s="14"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H54" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
@@ -2553,7 +2703,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>104</v>
@@ -2561,16 +2711,8 @@
       <c r="D55" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H55" s="6" t="s">
+      <c r="E55" s="4"/>
+      <c r="H55" s="5" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2580,7 +2722,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>104</v>
@@ -2589,13 +2731,13 @@
         <v>3</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>131</v>
+        <v>143</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>193</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>115</v>
@@ -2607,7 +2749,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>104</v>
@@ -2616,7 +2758,9 @@
         <v>3</v>
       </c>
       <c r="E57" s="4"/>
-      <c r="H57" s="5" t="s">
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2626,7 +2770,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>104</v>
@@ -2634,15 +2778,9 @@
       <c r="D58" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>146</v>
-      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
       <c r="H58" s="6" t="s">
         <v>115</v>
       </c>
@@ -2653,7 +2791,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>104</v>
@@ -2674,7 +2812,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>56</v>
+        <v>148</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>104</v>
@@ -2682,12 +2820,16 @@
       <c r="D60" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E60" s="4"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="E60" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F60" t="s">
+        <v>194</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H60" s="6"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
@@ -2695,7 +2837,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>57</v>
+        <v>149</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>104</v>
@@ -2703,36 +2845,34 @@
       <c r="D61" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="E61" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="H61" s="6"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>182</v>
+      <c r="B62" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F62" t="s">
-        <v>183</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>147</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
       <c r="H62" s="6"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2741,7 +2881,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>185</v>
+        <v>59</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>104</v>
@@ -2749,35 +2889,35 @@
       <c r="D63" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E63" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="H63" s="6"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>58</v>
+      <c r="B64" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E64" s="14"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16"/>
-      <c r="H64" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E64" s="4"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
@@ -2785,7 +2925,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>104</v>
@@ -2794,12 +2934,8 @@
         <v>3</v>
       </c>
       <c r="E65" s="4"/>
-      <c r="F65" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G65" s="6"/>
-      <c r="H65" s="6" t="s">
-        <v>114</v>
+      <c r="H65" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2808,7 +2944,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>104</v>
@@ -2829,7 +2965,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>104</v>
@@ -2838,30 +2974,31 @@
         <v>3</v>
       </c>
       <c r="E67" s="4"/>
-      <c r="H67" s="5" t="s">
-        <v>118</v>
+      <c r="F67" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <f t="shared" ref="A68:A106" si="1">A67+1</f>
+        <f t="shared" ref="A68:A104" si="1">A67+1</f>
         <v>67</v>
       </c>
-      <c r="B68" s="4" t="s">
-        <v>62</v>
+      <c r="B68" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E68" s="4"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6" t="s">
-        <v>118</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E68" s="14"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
@@ -2869,21 +3006,17 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E69" s="4"/>
-      <c r="F69" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6" t="s">
-        <v>119</v>
+      <c r="H69" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2891,18 +3024,19 @@
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>64</v>
+      <c r="B70" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>103</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E70" s="14"/>
-      <c r="F70" s="15"/>
-      <c r="G70" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="E70" s="4"/>
+      <c r="H70" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
@@ -2910,7 +3044,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>103</v>
@@ -2919,6 +3053,8 @@
         <v>3</v>
       </c>
       <c r="E71" s="4"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
       <c r="H71" s="5" t="s">
         <v>120</v>
       </c>
@@ -2929,7 +3065,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>103</v>
@@ -2938,6 +3074,8 @@
         <v>3</v>
       </c>
       <c r="E72" s="4"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
       <c r="H72" s="5" t="s">
         <v>120</v>
       </c>
@@ -2948,7 +3086,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>103</v>
@@ -2957,8 +3095,6 @@
         <v>3</v>
       </c>
       <c r="E73" s="4"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
       <c r="H73" s="5" t="s">
         <v>120</v>
       </c>
@@ -2969,7 +3105,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>103</v>
@@ -2990,7 +3126,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>103</v>
@@ -2999,6 +3135,8 @@
         <v>3</v>
       </c>
       <c r="E75" s="4"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
       <c r="H75" s="5" t="s">
         <v>120</v>
       </c>
@@ -3009,7 +3147,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>103</v>
@@ -3017,9 +3155,15 @@
       <c r="D76" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E76" s="4"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
+      <c r="E76" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="H76" s="5" t="s">
         <v>120</v>
       </c>
@@ -3029,21 +3173,19 @@
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>70</v>
+      <c r="B77" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E77" s="4"/>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
-      <c r="H77" s="5" t="s">
-        <v>120</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E77" s="14"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
@@ -3051,25 +3193,21 @@
         <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E78" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F78" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>120</v>
+      <c r="E78" s="4"/>
+      <c r="F78" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -3077,19 +3215,23 @@
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>73</v>
+      <c r="B79" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E79" s="14"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="16"/>
-      <c r="H79" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E79" s="4"/>
+      <c r="F79" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
@@ -3097,7 +3239,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>104</v>
@@ -3106,12 +3248,10 @@
         <v>3</v>
       </c>
       <c r="E80" s="4"/>
-      <c r="F80" s="6" t="s">
-        <v>137</v>
-      </c>
+      <c r="F80" s="6"/>
       <c r="G80" s="6"/>
       <c r="H80" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -3120,7 +3260,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>104</v>
@@ -3129,9 +3269,7 @@
         <v>3</v>
       </c>
       <c r="E81" s="4"/>
-      <c r="F81" s="6" t="s">
-        <v>138</v>
-      </c>
+      <c r="F81" s="6"/>
       <c r="G81" s="6"/>
       <c r="H81" s="6" t="s">
         <v>116</v>
@@ -3143,7 +3281,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>104</v>
@@ -3164,7 +3302,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>104</v>
@@ -3185,7 +3323,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>104</v>
@@ -3206,7 +3344,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>104</v>
@@ -3218,7 +3356,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -3227,7 +3365,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>104</v>
@@ -3248,7 +3386,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>104</v>
@@ -3257,10 +3395,8 @@
         <v>3</v>
       </c>
       <c r="E87" s="4"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
       <c r="H87" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -3269,7 +3405,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>104</v>
@@ -3290,7 +3426,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>104</v>
@@ -3299,6 +3435,8 @@
         <v>3</v>
       </c>
       <c r="E89" s="4"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
       <c r="H89" s="6" t="s">
         <v>116</v>
       </c>
@@ -3309,7 +3447,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>104</v>
@@ -3330,7 +3468,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>104</v>
@@ -3339,8 +3477,6 @@
         <v>3</v>
       </c>
       <c r="E91" s="4"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="6"/>
       <c r="H91" s="6" t="s">
         <v>116</v>
       </c>
@@ -3350,21 +3486,18 @@
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>86</v>
+      <c r="B92" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E92" s="4"/>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6" t="s">
-        <v>116</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E92" s="14"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="15"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
@@ -3372,7 +3505,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>104</v>
@@ -3381,8 +3514,14 @@
         <v>3</v>
       </c>
       <c r="E93" s="4"/>
+      <c r="F93" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="H93" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -3390,18 +3529,25 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="B94" s="3" t="s">
-        <v>88</v>
+      <c r="B94" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E94" s="14"/>
-      <c r="F94" s="15"/>
-      <c r="G94" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="E94" s="4"/>
+      <c r="F94" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H94" s="6" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
@@ -3409,7 +3555,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>104</v>
@@ -3418,14 +3564,12 @@
         <v>3</v>
       </c>
       <c r="E95" s="4"/>
-      <c r="F95" s="6" t="s">
-        <v>139</v>
-      </c>
+      <c r="F95" s="6"/>
       <c r="G95" s="5" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="H95" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -3434,7 +3578,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>104</v>
@@ -3444,10 +3588,10 @@
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="6" t="s">
-        <v>140</v>
+        <v>202</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="H96" s="6" t="s">
         <v>115</v>
@@ -3459,7 +3603,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>104</v>
@@ -3470,7 +3614,7 @@
       <c r="E97" s="4"/>
       <c r="F97" s="6"/>
       <c r="G97" s="5" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>116</v>
@@ -3482,7 +3626,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>104</v>
@@ -3491,14 +3635,11 @@
         <v>3</v>
       </c>
       <c r="E98" s="4"/>
-      <c r="F98" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="G98" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="H98" s="6" t="s">
-        <v>115</v>
+        <v>206</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -3507,7 +3648,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>104</v>
@@ -3516,11 +3657,13 @@
         <v>3</v>
       </c>
       <c r="E99" s="4"/>
-      <c r="F99" s="6"/>
+      <c r="F99" s="6" t="s">
+        <v>203</v>
+      </c>
       <c r="G99" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="H99" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H99" s="5" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3530,7 +3673,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>104</v>
@@ -3539,11 +3682,14 @@
         <v>3</v>
       </c>
       <c r="E100" s="4"/>
+      <c r="F100" s="6" t="s">
+        <v>205</v>
+      </c>
       <c r="G100" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="H100" s="5" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="H100" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -3552,7 +3698,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>104</v>
@@ -3562,10 +3708,10 @@
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="6" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>116</v>
@@ -3577,7 +3723,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>104</v>
@@ -3586,14 +3732,11 @@
         <v>3</v>
       </c>
       <c r="E102" s="4"/>
-      <c r="F102" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="G102" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="H102" s="6" t="s">
-        <v>115</v>
+        <v>206</v>
+      </c>
+      <c r="H102" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -3602,7 +3745,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>104</v>
@@ -3611,11 +3754,8 @@
         <v>3</v>
       </c>
       <c r="E103" s="4"/>
-      <c r="F103" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="G103" s="5" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>116</v>
@@ -3626,108 +3766,64 @@
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E104" s="4"/>
+      <c r="B104" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E104" s="7"/>
+      <c r="F104" s="10"/>
       <c r="G104" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="H104" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H104" s="12" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
-        <f t="shared" si="1"/>
-        <v>104</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E105" s="4"/>
-      <c r="G105" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="H105" s="5" t="s">
-        <v>116</v>
+      <c r="C105" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E106" s="7"/>
-      <c r="F106" s="10"/>
-      <c r="G106" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="H106" s="12" t="s">
-        <v>116</v>
+      <c r="B106" s="22" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C107" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>2</v>
+      <c r="B107" s="22" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B108" s="22" t="s">
-        <v>198</v>
+      <c r="B108" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="22" t="s">
-        <v>199</v>
+      <c r="B109" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B112" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="2" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:G1 E7:G34 H1:H44 E45:H1048576">
+  <conditionalFormatting sqref="E1:G1 E7:G32 H1:H42 E43:H1048576">
     <cfRule type="expression" dxfId="7" priority="13">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
@@ -3737,12 +3833,12 @@
       <formula>"$C2 = 'Header'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:G2 I36 F3:G6 E36:G44">
+  <conditionalFormatting sqref="E2:G2 I34 F3:G6 E34:G42">
     <cfRule type="expression" dxfId="5" priority="9">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E35:F35">
+  <conditionalFormatting sqref="E33:F33">
     <cfRule type="expression" dxfId="4" priority="8">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
@@ -3752,12 +3848,12 @@
       <formula>"$C2 = 'Header'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
+  <conditionalFormatting sqref="I33">
     <cfRule type="expression" dxfId="2" priority="5">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
+  <conditionalFormatting sqref="G33">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
@@ -3768,11 +3864,188 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27473039-7BF5-41BD-AAFA-F14B86FDFC50}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="23"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="G10" s="27"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="C11" s="23"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="23"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" s="23"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="23"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25"/>
+      <c r="B15" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="23"/>
+    </row>
+    <row r="30" ht="111.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9E7900-7483-405A-A875-85DCA0D23C39}">
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3788,80 +4061,80 @@
   <sheetData>
     <row r="1" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>207</v>
+        <v>169</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>210</v>
+        <v>172</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="F2" t="s">
-        <v>206</v>
-      </c>
-      <c r="L2" t="str">
-        <f>REPLACE([1]A_MicroEnvironment!A2,1,LEN([1]A_MicroEnvironment!A9), "")</f>
-        <v/>
+        <v>168</v>
+      </c>
+      <c r="L2" t="e">
+        <f>REPLACE(A_Microenvironment!#REF!,1,LEN(A_Microenvironment!#REF!), "")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="E3" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="F3" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="F4" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="J4" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3875,45 +4148,45 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="F7" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3921,180 +4194,180 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="22" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="E11" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="F11" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="21" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="C15" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="E15" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="F15" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="21" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="D18" s="22"/>
       <c r="E18" s="22" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="F19" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="21" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>192</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="E23" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="F23" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4108,11 +4381,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3E76D3-6A9A-4827-BA9C-4B17098CC9CF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added cell death and cell cycle assay writing to script function
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE53F8E-C709-4735-859E-C0DF130325E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17786D0F-FE39-4D74-9555-F74E62BBBF19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
     <sheet name="A_Microenvironment" sheetId="4" r:id="rId2"/>
-    <sheet name="Assays" sheetId="3" r:id="rId3"/>
-    <sheet name="ISA-Tab to MCDS-DCL" sheetId="2" r:id="rId4"/>
+    <sheet name="A_CellCycle" sheetId="5" r:id="rId3"/>
+    <sheet name="A_CellDeath" sheetId="6" r:id="rId4"/>
+    <sheet name="Assays" sheetId="3" r:id="rId5"/>
+    <sheet name="ISA-Tab to MCDS-DCL" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="B">A_Microenvironment!#REF!</definedName>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="301">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -760,6 +762,189 @@
   </si>
   <si>
     <t>Column Explanation</t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset/phenotype/cell_cycle/cell_cycle_phase[@ID]</t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset/phenotype/cell_cycle[@ID]</t>
+  </si>
+  <si>
+    <t>/birth_rate</t>
+  </si>
+  <si>
+    <t>/birth_rate[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/birth_rate[@units]</t>
+  </si>
+  <si>
+    <t>/cell_cycle_arrest/condition</t>
+  </si>
+  <si>
+    <t>/cell_cycle_arrest/condition[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/cell_cycle_arrest/condition[@standard_error_of_the_mean]</t>
+  </si>
+  <si>
+    <t>/cell_cycle_arrest/condition[@type]</t>
+  </si>
+  <si>
+    <t>/cell_cycle_arrest/condition[@units]</t>
+  </si>
+  <si>
+    <t>/death_rate</t>
+  </si>
+  <si>
+    <t>/death_rate[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/death_rate[@type]</t>
+  </si>
+  <si>
+    <t>/death_rate[@units]</t>
+  </si>
+  <si>
+    <t>/duration</t>
+  </si>
+  <si>
+    <t>/duration[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/duration[@units]</t>
+  </si>
+  <si>
+    <t>/net_birth_rate</t>
+  </si>
+  <si>
+    <t>/net_birth_rate[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/net_birth_rate[@standard_error_of_the_mean]</t>
+  </si>
+  <si>
+    <t>/net_birth_rate[@units]</t>
+  </si>
+  <si>
+    <t>[@ID]</t>
+  </si>
+  <si>
+    <t>Cell Cycle Phase xPaths</t>
+  </si>
+  <si>
+    <t>Parameter Value[Birth Rate]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Death Rate]</t>
+  </si>
+  <si>
+    <t>Characteristic[Death Type]</t>
+  </si>
+  <si>
+    <t>Cell Cycle Phase ISA Entities</t>
+  </si>
+  <si>
+    <t>Parameter Value[Cell Cycle Arrest Condition]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Duration]</t>
+  </si>
+  <si>
+    <t>Characteristic[Birth Rate - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Characteristic[Death Rate - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Characteristic[Net Birth Rate - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Cell Cycle Arrest Condition - Units</t>
+  </si>
+  <si>
+    <t>Duration - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Cell Cycle Arrest Condition - Type]</t>
+  </si>
+  <si>
+    <t>Characteristic[Cell Cycle Arrest Condition - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Cell Cycle Arrest Condition - Standard Error of Mean]</t>
+  </si>
+  <si>
+    <t>Death Rate - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Death Rate - Type]</t>
+  </si>
+  <si>
+    <t>Birth Rate - Units</t>
+  </si>
+  <si>
+    <t>Net Birth Rate - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Duration - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Net Birth Rate]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Net Birth Rate - Standard Error of Mean]</t>
+  </si>
+  <si>
+    <t>Unused paths</t>
+  </si>
+  <si>
+    <t>/custom/velocity</t>
+  </si>
+  <si>
+    <t>/custom/velocity[@units]</t>
+  </si>
+  <si>
+    <t>/summary_elements/population_doubling_time</t>
+  </si>
+  <si>
+    <t>/summary_elements/population_doubling_time[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/summary_elements/population_doubling_time[@units]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Cell Cycle Velocity]</t>
+  </si>
+  <si>
+    <t>Cell Cycle Velocity - Units</t>
+  </si>
+  <si>
+    <t>Parameter Value[Population Doubling Time]</t>
+  </si>
+  <si>
+    <t>Population Doubling Time - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Population Doubling Time - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Cell Cycle Summary ISA Entities</t>
+  </si>
+  <si>
+    <t>Cell Cycle Summary xPaths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell Cycle Phase ISA Entities + xPaths are contained under cell_cycle_phase tag; </t>
+  </si>
+  <si>
+    <t>Cell Death ISA Entities</t>
+  </si>
+  <si>
+    <t>Base xPath: cell_line/phenotype_dataset/phenotype/cell_death</t>
+  </si>
+  <si>
+    <t>Cell Death xPaths</t>
   </si>
 </sst>
 </file>
@@ -806,7 +991,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,12 +1018,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -938,11 +1135,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -970,36 +1267,67 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1374,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FA11B-2D6D-4A50-A5F1-7D079DCC0D36}">
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A75" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3867,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27473039-7BF5-41BD-AAFA-F14B86FDFC50}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3880,155 +4208,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="F1" s="30"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="39" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="43" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="35" t="s">
         <v>233</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="36" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="36" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="24" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="43" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="36" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" s="24" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="36" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="36" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="40"/>
+      <c r="B7" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="36" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="24" t="s">
+      <c r="A8" s="40"/>
+      <c r="B8" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="36" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="24" t="s">
+      <c r="A9" s="40"/>
+      <c r="B9" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="37"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="G10" s="27"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="37"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="24" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="43" t="s">
         <v>211</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="40"/>
+      <c r="B12" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="40"/>
+      <c r="B13" s="43" t="s">
         <v>209</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="24" t="s">
+      <c r="A14" s="40"/>
+      <c r="B14" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="41"/>
+      <c r="B15" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="37"/>
     </row>
     <row r="30" ht="111.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -4041,11 +4376,390 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACDCEEC-2455-41F7-B48E-7900618A1490}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>290</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="47"/>
+      <c r="B3" s="27" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="G3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="47"/>
+      <c r="B4" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>287</v>
+      </c>
+      <c r="G4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="47"/>
+      <c r="B5" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>249</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" s="32"/>
+      <c r="E7" s="31"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" s="32"/>
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="D9" s="32"/>
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="47"/>
+      <c r="B10" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="47"/>
+      <c r="B11" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="47"/>
+      <c r="B12" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="31"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="47"/>
+      <c r="B13" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>251</v>
+      </c>
+      <c r="D13" s="32"/>
+      <c r="E13" s="31"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="31"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="47"/>
+      <c r="B15" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="31"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="47"/>
+      <c r="B16" s="27" t="s">
+        <v>281</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="D16" s="32"/>
+      <c r="E16" s="31"/>
+      <c r="G16" t="str">
+        <f>REPLACE(F16,1,$H$14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="47"/>
+      <c r="B17" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="31"/>
+      <c r="G17" t="str">
+        <f>REPLACE(F17,1,$H$14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="47"/>
+      <c r="B18" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="32"/>
+      <c r="E18" s="31"/>
+      <c r="G18" t="str">
+        <f>REPLACE(F18,1,$H$14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="31"/>
+      <c r="G19" t="str">
+        <f>REPLACE(F19,1,$H$14,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="48"/>
+      <c r="B20" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="32"/>
+      <c r="E20" s="31"/>
+      <c r="G20" t="str">
+        <f>REPLACE(F20,1,$H$14,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC37ADF-8EEC-40F8-B778-8DF21953A6C4}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>273</v>
+      </c>
+      <c r="C4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H8" t="str">
+        <f t="shared" ref="H5:H8" si="0">REPLACE(G8,1,$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9E7900-7483-405A-A875-85DCA0D23C39}">
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4381,7 +5095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3E76D3-6A9A-4827-BA9C-4B17098CC9CF}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added mechanics, geometrical properties, and motility assay writing to script function
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17786D0F-FE39-4D74-9555-F74E62BBBF19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAF168B-14C0-4D9A-AC8E-16FE120FDCCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
     <sheet name="A_Microenvironment" sheetId="4" r:id="rId2"/>
     <sheet name="A_CellCycle" sheetId="5" r:id="rId3"/>
     <sheet name="A_CellDeath" sheetId="6" r:id="rId4"/>
-    <sheet name="Assays" sheetId="3" r:id="rId5"/>
-    <sheet name="ISA-Tab to MCDS-DCL" sheetId="2" r:id="rId6"/>
+    <sheet name="A_Mechanics" sheetId="7" r:id="rId5"/>
+    <sheet name="A_GeometricalProperties" sheetId="9" r:id="rId6"/>
+    <sheet name="A_Motility" sheetId="8" r:id="rId7"/>
+    <sheet name="ISA-Tab to MCDS-DCL" sheetId="2" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="B">A_Microenvironment!#REF!</definedName>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="389">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -500,30 +502,9 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>Assay Entity</t>
-  </si>
-  <si>
-    <t>xPath</t>
-  </si>
-  <si>
-    <t>phenotype_dataset[keywords]</t>
-  </si>
-  <si>
-    <t>MCDS entity</t>
-  </si>
-  <si>
-    <t>Cell ID?</t>
-  </si>
-  <si>
     <t>Cell Part</t>
   </si>
   <si>
-    <t>Conditions</t>
-  </si>
-  <si>
-    <t>cell_part[name]</t>
-  </si>
-  <si>
     <t>Cell_Microenvironment</t>
   </si>
   <si>
@@ -542,36 +523,12 @@
     <t>Cell_Geometrics</t>
   </si>
   <si>
-    <t>cell_line/phenotype_dataset[@ID]</t>
-  </si>
-  <si>
     <t>cell_line/phenotype_dataset[@keywords]</t>
   </si>
   <si>
-    <t>phenotype_dataset[ID]</t>
-  </si>
-  <si>
-    <t>Protocol REF</t>
-  </si>
-  <si>
     <t>Assay Name</t>
   </si>
   <si>
-    <t>Characteristic[phenotype_dataset_ID]</t>
-  </si>
-  <si>
-    <t>Cell ID</t>
-  </si>
-  <si>
-    <t>In /"assay"/?</t>
-  </si>
-  <si>
-    <t>Assay name, variable name, or No</t>
-  </si>
-  <si>
-    <t>Parameter Value[oxygen.concentration]</t>
-  </si>
-  <si>
     <t>cell_line/metadata/MultiCellDB/ID</t>
   </si>
   <si>
@@ -833,6 +790,9 @@
     <t>Cell Cycle Phase xPaths</t>
   </si>
   <si>
+    <t>Sample name</t>
+  </si>
+  <si>
     <t>Parameter Value[Birth Rate]</t>
   </si>
   <si>
@@ -945,6 +905,312 @@
   </si>
   <si>
     <t>Cell Death xPaths</t>
+  </si>
+  <si>
+    <t>Cell Mechanics ISA Entities</t>
+  </si>
+  <si>
+    <t>Cell Mechanics xPaths</t>
+  </si>
+  <si>
+    <t>/maximum_cell_deformation</t>
+  </si>
+  <si>
+    <t>/maximum_cell_deformation[@units]</t>
+  </si>
+  <si>
+    <t>/maximum_cell_deformation[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/maximum_cell_deformation[@range]</t>
+  </si>
+  <si>
+    <t>/poisson_ratio</t>
+  </si>
+  <si>
+    <t>/poisson_ratio[@units]</t>
+  </si>
+  <si>
+    <t>/poisson_ratio[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/youngs_modulus</t>
+  </si>
+  <si>
+    <t>/youngs_modulus[@units]</t>
+  </si>
+  <si>
+    <t>/youngs_modulus[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/youngs_modulus[@standard_deviation]</t>
+  </si>
+  <si>
+    <t>/youngs_modulus[@uncertainty]</t>
+  </si>
+  <si>
+    <t>Maximum Cell Deformation - Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Maximum Cell Deformation - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Maximum Cell Deformation - Range]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Young's Modulus]</t>
+  </si>
+  <si>
+    <t>Young's Modulus - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Young's Modulus - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Young's Modulus - Standard Deviation]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Young's Modulus - Uncertainty]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Maximum Cell Deformation]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Poisson Ratio]</t>
+  </si>
+  <si>
+    <t>Poisson Ratio - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Poisson Ratio - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Mechanics Explanation</t>
+  </si>
+  <si>
+    <t>Check for existence of base element</t>
+  </si>
+  <si>
+    <t>Remove from list of paths</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>/areas/total_surface_area</t>
+  </si>
+  <si>
+    <t>/cross_section/areas/total_area</t>
+  </si>
+  <si>
+    <t>/lengths/major_axis</t>
+  </si>
+  <si>
+    <t>/lengths/minor_axis</t>
+  </si>
+  <si>
+    <t>/lengths/radius</t>
+  </si>
+  <si>
+    <t>/volumes/total_volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>measurement_type</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>uncertainty</t>
+  </si>
+  <si>
+    <t>Base path(s)</t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset/phenotype/geometrical_properties/</t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset/cell_part/cell_part/phenotype/geometrical_properties/</t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset/cell_part/phenotype/geometrical_properties/</t>
+  </si>
+  <si>
+    <t>Cell Geometrical Properties xPaths</t>
+  </si>
+  <si>
+    <t>Cell Geometrical Properties Attributes</t>
+  </si>
+  <si>
+    <t>Cell Geometrical Properties ISA Measurement Name</t>
+  </si>
+  <si>
+    <t>Cell Geometrical Properties ISA Entity Beginning</t>
+  </si>
+  <si>
+    <t>Cell Geometrical Properties ISA Entity Tail</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Major Axis</t>
+  </si>
+  <si>
+    <t>Minor Axis</t>
+  </si>
+  <si>
+    <t>Total Surface Area</t>
+  </si>
+  <si>
+    <t>Cross Section Total Area</t>
+  </si>
+  <si>
+    <t>Total Volume</t>
+  </si>
+  <si>
+    <t>Parameter Value[</t>
+  </si>
+  <si>
+    <t>Characteristic[</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Measurement - Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Measurement Type]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Measurement - Maximum]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Measurement - Minimum]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Measurement - Range]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Measurement - Uncertainty]</t>
+  </si>
+  <si>
+    <t>Add to dictionary?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from </t>
+  </si>
+  <si>
+    <t>From parent</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parameter </t>
+  </si>
+  <si>
+    <t>Rows:</t>
+  </si>
+  <si>
+    <t>One per elem (each cell_part)</t>
+  </si>
+  <si>
+    <t>Need to determine param/attrib for writing</t>
+  </si>
+  <si>
+    <t>attribute order in xlsx dictates order in doc</t>
+  </si>
+  <si>
+    <t>First two columns are used to find "measurement" elements under geometrical_properties elements. Attributes is used to find attributes. ISA header = beginning + measurement + tail</t>
+  </si>
+  <si>
+    <t>elem.tag</t>
+  </si>
+  <si>
+    <t>base paths</t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset/phenotype/motility/restricted/</t>
+  </si>
+  <si>
+    <t>cell_line/phenotype_dataset/phenotype/motility/unrestricted/</t>
+  </si>
+  <si>
+    <t>differentiated in file by Motility Type</t>
+  </si>
+  <si>
+    <t>/diffusion_coefficient</t>
+  </si>
+  <si>
+    <t>/mean_speed</t>
+  </si>
+  <si>
+    <t>/persistence</t>
+  </si>
+  <si>
+    <t>/timescale</t>
+  </si>
+  <si>
+    <t>/restriction/surface_variable[@name]</t>
+  </si>
+  <si>
+    <t>number_obs</t>
+  </si>
+  <si>
+    <t>standard_deviation</t>
+  </si>
+  <si>
+    <t>Characteristic[Motility Type]</t>
+  </si>
+  <si>
+    <t>Characteristic[Restriction Surface Name]</t>
+  </si>
+  <si>
+    <t>Cell Motility ISA Measurement Name</t>
+  </si>
+  <si>
+    <t>Cell Motility xPaths</t>
+  </si>
+  <si>
+    <t>Cell Motility Attributes</t>
+  </si>
+  <si>
+    <t>Cell Motility ISA Entity Beginning</t>
+  </si>
+  <si>
+    <t>Diffusion Coefficient</t>
+  </si>
+  <si>
+    <t>Mean Speed</t>
+  </si>
+  <si>
+    <t>Persistence</t>
+  </si>
+  <si>
+    <t>Timescale</t>
+  </si>
+  <si>
+    <t>Cell Motility ISA Entity Tail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Standard Deviation]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Number of Observations]</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1235,11 +1501,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1329,18 +1604,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -1925,7 +2205,7 @@
         <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>130</v>
@@ -1952,7 +2232,7 @@
         <v>136</v>
       </c>
       <c r="F9" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>130</v>
@@ -1979,7 +2259,7 @@
         <v>138</v>
       </c>
       <c r="F10" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>130</v>
@@ -2046,7 +2326,7 @@
         <v>137</v>
       </c>
       <c r="F13" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>130</v>
@@ -2070,7 +2350,7 @@
         <v>141</v>
       </c>
       <c r="F14" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>130</v>
@@ -2100,7 +2380,7 @@
         <v>137</v>
       </c>
       <c r="F15" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>130</v>
@@ -2130,7 +2410,7 @@
         <v>136</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>130</v>
@@ -2157,7 +2437,7 @@
         <v>124</v>
       </c>
       <c r="F17" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>130</v>
@@ -2228,7 +2508,7 @@
         <v>111</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>130</v>
@@ -2276,7 +2556,7 @@
         <v>143</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>130</v>
@@ -2385,7 +2665,7 @@
         <v>122</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>130</v>
@@ -2412,7 +2692,7 @@
         <v>123</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>130</v>
@@ -2462,7 +2742,7 @@
         <v>112</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>130</v>
@@ -2535,7 +2815,7 @@
         <v>139</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>130</v>
@@ -2565,7 +2845,7 @@
         <v>135</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>130</v>
@@ -2595,7 +2875,7 @@
         <v>132</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>130</v>
@@ -2706,7 +2986,7 @@
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>130</v>
@@ -2731,7 +3011,7 @@
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>130</v>
@@ -2756,7 +3036,7 @@
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>130</v>
@@ -2989,7 +3269,7 @@
         <v>110</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>130</v>
@@ -3016,7 +3296,7 @@
         <v>111</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>130</v>
@@ -3062,7 +3342,7 @@
         <v>143</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>130</v>
@@ -3152,7 +3432,7 @@
         <v>150</v>
       </c>
       <c r="F60" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="G60" s="6" t="s">
         <v>130</v>
@@ -3177,7 +3457,7 @@
         <v>124</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="G61" s="6" t="s">
         <v>130</v>
@@ -3219,7 +3499,7 @@
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="6" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="6" t="s">
@@ -3303,7 +3583,7 @@
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="6" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="6" t="s">
@@ -3487,7 +3767,7 @@
         <v>136</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="G76" s="6" t="s">
         <v>130</v>
@@ -3531,7 +3811,7 @@
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="6" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="G78" s="6"/>
       <c r="H78" s="6" t="s">
@@ -3554,7 +3834,7 @@
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="6" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="G79" s="6"/>
       <c r="H79" s="6" t="s">
@@ -3843,7 +4123,7 @@
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="6" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>131</v>
@@ -3868,7 +4148,7 @@
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="6" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>131</v>
@@ -3894,7 +4174,7 @@
       <c r="E95" s="4"/>
       <c r="F95" s="6"/>
       <c r="G95" s="5" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>116</v>
@@ -3916,7 +4196,7 @@
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="6" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>131</v>
@@ -3942,7 +4222,7 @@
       <c r="E97" s="4"/>
       <c r="F97" s="6"/>
       <c r="G97" s="5" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>116</v>
@@ -3964,7 +4244,7 @@
       </c>
       <c r="E98" s="4"/>
       <c r="G98" s="5" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H98" s="5" t="s">
         <v>116</v>
@@ -3986,7 +4266,7 @@
       </c>
       <c r="E99" s="4"/>
       <c r="F99" s="6" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="G99" s="5" t="s">
         <v>131</v>
@@ -4011,7 +4291,7 @@
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="6" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>131</v>
@@ -4036,7 +4316,7 @@
       </c>
       <c r="E101" s="4"/>
       <c r="F101" s="6" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="G101" s="5" t="s">
         <v>131</v>
@@ -4061,7 +4341,7 @@
       </c>
       <c r="E102" s="4"/>
       <c r="G102" s="5" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H102" s="5" t="s">
         <v>116</v>
@@ -4083,7 +4363,7 @@
       </c>
       <c r="E103" s="4"/>
       <c r="G103" s="5" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>116</v>
@@ -4106,7 +4386,7 @@
       <c r="E104" s="7"/>
       <c r="F104" s="10"/>
       <c r="G104" s="5" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H104" s="12" t="s">
         <v>116</v>
@@ -4122,67 +4402,67 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B106" s="22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B107" s="22" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:G1 E7:G32 H1:H42 E43:H1048576">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="6" priority="13">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G2">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>"$C2 = 'Header'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:G2 I34 F3:G6 E34:G42">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33:F33">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>"$C2 = 'Header'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G33">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4196,7 +4476,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4209,109 +4489,109 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="40"/>
       <c r="B3" s="43" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
       <c r="B4" s="43" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="40"/>
       <c r="B5" s="43" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="40"/>
       <c r="B6" s="43" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="40"/>
       <c r="B7" s="43" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="40"/>
       <c r="B8" s="43" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="40"/>
       <c r="B9" s="43" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="37"/>
@@ -4319,7 +4599,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="40"/>
       <c r="B10" s="43" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="37"/>
@@ -4328,7 +4608,7 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="43" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="37"/>
@@ -4336,7 +4616,7 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="43" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="37"/>
@@ -4344,7 +4624,7 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="43" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="37"/>
@@ -4352,7 +4632,7 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="43" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="37"/>
@@ -4360,7 +4640,7 @@
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41"/>
       <c r="B15" s="43" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C15" s="32"/>
       <c r="D15" s="37"/>
@@ -4395,114 +4675,114 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="E1" s="46" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="B3" s="27" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="G3" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="27" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="G4" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="27" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="27" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="27" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="31"/>
@@ -4510,10 +4790,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="47"/>
       <c r="B8" s="27" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="D8" s="32"/>
       <c r="E8" s="31"/>
@@ -4521,10 +4801,10 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="27" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="31"/>
@@ -4532,10 +4812,10 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="27" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="31"/>
@@ -4543,10 +4823,10 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="27" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="31"/>
@@ -4554,10 +4834,10 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="27" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="31"/>
@@ -4565,10 +4845,10 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="27" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="31"/>
@@ -4576,10 +4856,10 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="27" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="31"/>
@@ -4587,10 +4867,10 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="27" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="D15" s="32"/>
       <c r="E15" s="31"/>
@@ -4598,10 +4878,10 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="27" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="D16" s="32"/>
       <c r="E16" s="31"/>
@@ -4613,10 +4893,10 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="27" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="D17" s="32"/>
       <c r="E17" s="31"/>
@@ -4628,10 +4908,10 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="27" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="31"/>
@@ -4643,10 +4923,10 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="27" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="31"/>
@@ -4658,10 +4938,10 @@
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="48"/>
       <c r="B20" s="27" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="D20" s="32"/>
       <c r="E20" s="31"/>
@@ -4683,8 +4963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC37ADF-8EEC-40F8-B778-8DF21953A6C4}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4696,51 +4976,51 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="G2" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="C3" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="G3" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="C4" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="C5" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4755,347 +5035,527 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9E7900-7483-405A-A875-85DCA0D23C39}">
-  <dimension ref="A1:L24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098C817-F491-46B8-ACCD-892895410AE2}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>306</v>
+      </c>
+      <c r="C10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>308</v>
+      </c>
+      <c r="C12" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>309</v>
+      </c>
+      <c r="C13" t="s">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9108F335-02AF-4487-9ECF-FF27706B5F2B}">
+  <dimension ref="A1:R12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>335</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>337</v>
+      </c>
+      <c r="F1" s="49" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>363</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>339</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>322</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50" t="s">
+        <v>347</v>
+      </c>
+      <c r="I2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="51" t="s">
+        <v>340</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>325</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>346</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>348</v>
+      </c>
+      <c r="I3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="54"/>
+      <c r="B4" s="51" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>321</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>327</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>349</v>
+      </c>
+      <c r="I4" t="s">
+        <v>353</v>
+      </c>
+      <c r="R4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="51" t="s">
+        <v>342</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>318</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>328</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>350</v>
+      </c>
+      <c r="R5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="51" t="s">
+        <v>343</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>351</v>
+      </c>
+      <c r="I6" s="50" t="s">
+        <v>151</v>
+      </c>
+      <c r="J6" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="K6" s="50" t="s">
+        <v>356</v>
+      </c>
+      <c r="L6" s="50" t="s">
+        <v>357</v>
+      </c>
+      <c r="M6" s="50" t="s">
+        <v>358</v>
+      </c>
+      <c r="N6" s="50" t="s">
+        <v>357</v>
+      </c>
+      <c r="O6" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F2" t="s">
-        <v>168</v>
-      </c>
-      <c r="L2" t="e">
-        <f>REPLACE(A_Microenvironment!#REF!,1,LEN(A_Microenvironment!#REF!), "")</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C7" t="s">
-        <v>156</v>
-      </c>
-      <c r="E7" t="s">
-        <v>154</v>
-      </c>
-      <c r="F7" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" t="s">
-        <v>156</v>
-      </c>
-      <c r="E11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C15" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" t="s">
-        <v>154</v>
-      </c>
-      <c r="F15" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C19" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" t="s">
-        <v>154</v>
-      </c>
-      <c r="F19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="C23" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" t="s">
-        <v>154</v>
-      </c>
-      <c r="F23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
-        <v>153</v>
+      <c r="R6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="51" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>323</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>329</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>352</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>355</v>
+      </c>
+      <c r="J7" t="s">
+        <v>354</v>
+      </c>
+      <c r="R7" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>359</v>
+      </c>
+      <c r="J9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B5:G5">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>"$C2 = ""Header"""</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D15C30-4CE2-4FE6-8ED7-DB2C8418632F}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>380</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>381</v>
+      </c>
+      <c r="F1" s="49" t="s">
+        <v>386</v>
+      </c>
+      <c r="H1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>363</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>382</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>369</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50" t="s">
+        <v>302</v>
+      </c>
+      <c r="H2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="54"/>
+      <c r="B3" s="51" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>325</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>346</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>348</v>
+      </c>
+      <c r="H3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="54"/>
+      <c r="B4" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>371</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>374</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>388</v>
+      </c>
+      <c r="H4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="54"/>
+      <c r="B5" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>375</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>345</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="54"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="H6" t="s">
+        <v>248</v>
+      </c>
+      <c r="I6" t="s">
+        <v>376</v>
+      </c>
+      <c r="J6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="I7" t="s">
+        <v>364</v>
+      </c>
+      <c r="J7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3E76D3-6A9A-4827-BA9C-4B17098CC9CF}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Completed PKPD Assay, created study file, updated excel relationship file
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAF168B-14C0-4D9A-AC8E-16FE120FDCCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5DCBC4-3F8C-4035-AF98-494A314C4C71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,11 @@
     <sheet name="A_Mechanics" sheetId="7" r:id="rId5"/>
     <sheet name="A_GeometricalProperties" sheetId="9" r:id="rId6"/>
     <sheet name="A_Motility" sheetId="8" r:id="rId7"/>
-    <sheet name="ISA-Tab to MCDS-DCL" sheetId="2" r:id="rId8"/>
+    <sheet name="A_S_PKPD" sheetId="11" r:id="rId8"/>
+    <sheet name="A_TransportProcesses" sheetId="12" r:id="rId9"/>
+    <sheet name="A_ClinicalStain" sheetId="13" r:id="rId10"/>
+    <sheet name="Study" sheetId="10" r:id="rId11"/>
+    <sheet name="ISA-Tab to MCDS-DCL" sheetId="2" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="B">A_Microenvironment!#REF!</definedName>
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="549">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -1211,6 +1215,486 @@
   </si>
   <si>
     <t xml:space="preserve"> - Number of Observations]</t>
+  </si>
+  <si>
+    <t>Characteristic[Restriction Surface MeSH ID]</t>
+  </si>
+  <si>
+    <t>/restriction/surface_variable[@MeSH ID]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/BTO_ID</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/CLO_ID</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/disease</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/morphology</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/organ</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/patient_derived</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/patient_derived[@patient_ID]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/species</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/cell_origin/strain</t>
+  </si>
+  <si>
+    <t>Custom/clinical</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/alive_patient</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/age_at_diagnosis</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/age_at_diagnosis[@measurement_type]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/age_at_diagnosis[@units]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/d_over_rho</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/d_over_rho[@measurement_type]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/d_over_rho[@units]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/overall_survival</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/overall_survival[@measurement_type]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/overall_survival[@units]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/rho_over_d</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/rho_over_d[@max]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/rho_over_d[@measurement_type]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/rho_over_d[@min]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/rho_over_d[@std]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/rho_over_d[@units]</t>
+  </si>
+  <si>
+    <t>stain</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain</t>
+  </si>
+  <si>
+    <t>cytoplasmic_stain</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/cytoplasmic_stain</t>
+  </si>
+  <si>
+    <t>membrane_stain</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/membrane_stain</t>
+  </si>
+  <si>
+    <t>nuclear_stain</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/nuclear_stain</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/source</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/target</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain[@ID]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain[@name]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_grade</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_type</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain</t>
+  </si>
+  <si>
+    <t>positive_fraction</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain/positive_fraction</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain/positive_fraction[@measurement_type]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain/positive_fraction[@units]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain[@ID]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain[@name]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Each element is in 172 distinct files</t>
+  </si>
+  <si>
+    <t>Therapy measurement set</t>
+  </si>
+  <si>
+    <t>Therapy - is this for each or single?</t>
+  </si>
+  <si>
+    <t>Repeats: Drug - descriptions</t>
+  </si>
+  <si>
+    <t>Drug description</t>
+  </si>
+  <si>
+    <t>Put drug info in study file?</t>
+  </si>
+  <si>
+    <t>Drugs - ID and info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pharamacodynamics - therapy measurement set, each therapy can be different </t>
+  </si>
+  <si>
+    <t>Organize by therapy measurement set, have repeating columns for drug?</t>
+  </si>
+  <si>
+    <t>ChEBI_ID</t>
+  </si>
+  <si>
+    <t>MeSH_ID</t>
+  </si>
+  <si>
+    <t>PR_ID</t>
+  </si>
+  <si>
+    <t>UniProt_ID</t>
+  </si>
+  <si>
+    <t>Export Rate</t>
+  </si>
+  <si>
+    <t>Import Rate</t>
+  </si>
+  <si>
+    <t>Saturation Density</t>
+  </si>
+  <si>
+    <t>Export Rate per Unit Surface Area</t>
+  </si>
+  <si>
+    <t>Import Rate per Unit Surface Area</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Characteristic[Variable ChEBI ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Variable MeSH ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Variable PR ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Variable UniProt ID]</t>
+  </si>
+  <si>
+    <t>First two columns are used to find variables for transport processes, remaining columns are used to find measurements under each variable</t>
+  </si>
+  <si>
+    <t>Transport Processes ISA Entity Beginning</t>
+  </si>
+  <si>
+    <t>Transport Processes ISA Entity Tail</t>
+  </si>
+  <si>
+    <t>Transport Processes ISA Variable Headers</t>
+  </si>
+  <si>
+    <t>Transport Processes Variable Attributes</t>
+  </si>
+  <si>
+    <t>Transport Processes ISA Measurement Name</t>
+  </si>
+  <si>
+    <t>Transport Processes Variable Measurements</t>
+  </si>
+  <si>
+    <t>Transport Processes Variable Measurement Attributes</t>
+  </si>
+  <si>
+    <t>/export_rate</t>
+  </si>
+  <si>
+    <t>/export_rate_per_unit_surface_area</t>
+  </si>
+  <si>
+    <t>/import_rate</t>
+  </si>
+  <si>
+    <t>/import_rate_per_unit_surface_area</t>
+  </si>
+  <si>
+    <t>/saturation_density</t>
+  </si>
+  <si>
+    <t>DrugBank_ID</t>
+  </si>
+  <si>
+    <t>Drug Name</t>
+  </si>
+  <si>
+    <t>Characteristic[Drug ChEBI ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Drug DrugBank ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Drug MeSH ID]</t>
+  </si>
+  <si>
+    <t>PKPD Drug ISA Headers</t>
+  </si>
+  <si>
+    <t>PKPD Drug Attributes</t>
+  </si>
+  <si>
+    <t>Use ID to match</t>
+  </si>
+  <si>
+    <t>Measurement Set #</t>
+  </si>
+  <si>
+    <t>Measurement Set ID</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>PKPD PD Headers</t>
+  </si>
+  <si>
+    <t>PKPD PD xPaths</t>
+  </si>
+  <si>
+    <t>Drug Dose - Units</t>
+  </si>
+  <si>
+    <t>Parameter Value[Drug Dose]</t>
+  </si>
+  <si>
+    <t>Characteristic[Drug Dose Measurement Type]</t>
+  </si>
+  <si>
+    <t>Parameter Value[IC50]</t>
+  </si>
+  <si>
+    <t>IC50 - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[IC50 Measurement Type]</t>
+  </si>
+  <si>
+    <t>Drug</t>
+  </si>
+  <si>
+    <t>/dose[@type]</t>
+  </si>
+  <si>
+    <t>/dose[@units]</t>
+  </si>
+  <si>
+    <t>/dose</t>
+  </si>
+  <si>
+    <t>/response/custom/IC_50</t>
+  </si>
+  <si>
+    <t>/response/custom/IC_50[@units]</t>
+  </si>
+  <si>
+    <t>/response/custom/IC_50[@measurement_type]</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>measurement</t>
+  </si>
+  <si>
+    <t>Cell Line Label</t>
+  </si>
+  <si>
+    <t>Study ISA Header</t>
+  </si>
+  <si>
+    <t>Study xPath</t>
+  </si>
+  <si>
+    <t>cell_line[@label]</t>
+  </si>
+  <si>
+    <t>MultiCellDB Name</t>
+  </si>
+  <si>
+    <t>match the ID to data?</t>
+  </si>
+  <si>
+    <t>As of now, this data exists for every custom/clinical</t>
+  </si>
+  <si>
+    <t>Sample base</t>
+  </si>
+  <si>
+    <t>Stain Name</t>
+  </si>
+  <si>
+    <t>Characteristic[Cytoplasmic Stain]</t>
+  </si>
+  <si>
+    <t>Characteristic[Stain Target]</t>
+  </si>
+  <si>
+    <t>Characteristic[Stain Source]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Stain Positive Fraction]</t>
+  </si>
+  <si>
+    <t>Characteristic[Cell Origin Company]</t>
+  </si>
+  <si>
+    <t>Characteristic[Cell Disease]</t>
+  </si>
+  <si>
+    <t>Cell BTO ID</t>
+  </si>
+  <si>
+    <t>Cell CLO ID</t>
+  </si>
+  <si>
+    <t>Characteristic[Morphology]</t>
+  </si>
+  <si>
+    <t>Characteristic[Organ]</t>
+  </si>
+  <si>
+    <t>Characteristic[Species]</t>
+  </si>
+  <si>
+    <t>Characteristic[Strain]</t>
+  </si>
+  <si>
+    <t>Characteristic[Patient Derived]</t>
+  </si>
+  <si>
+    <t>Characteristic[Patient ID]</t>
+  </si>
+  <si>
+    <t>Characteristic[Alive Patient]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Patient Age at Diagnosis]</t>
+  </si>
+  <si>
+    <t>Patient Age at Diagnosis - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Patient Age at Diagnosis Measurement Type]</t>
+  </si>
+  <si>
+    <t>Characteristic[Pathology Type]</t>
+  </si>
+  <si>
+    <t>Characteristic[Pathology Grade]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Overall Survival]</t>
+  </si>
+  <si>
+    <t>Overall Survival - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Overall Survival - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Characteristic[D/Rho - Measurement Type]</t>
+  </si>
+  <si>
+    <t>D/Rho - Units</t>
+  </si>
+  <si>
+    <t>Parameter Value[D/Rho]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Rho/D]</t>
+  </si>
+  <si>
+    <t>Rho/D - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Rho/D - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Rho/D - Maximum]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Rho/D - Minimum]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Rho/D - Standard Deviation]</t>
+  </si>
+  <si>
+    <t>In I file: is this needed?</t>
+  </si>
+  <si>
+    <t>Need to match Stain ID's</t>
+  </si>
+  <si>
+    <t>ID# is properly ordered - therefore, can write in order</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1574,15 +2058,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1598,22 +2073,53 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1982,7 +2488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FA11B-2D6D-4A50-A5F1-7D079DCC0D36}">
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
@@ -4471,6 +4977,479 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A97BD1D-99EF-49BC-B0C5-86FC67BB4019}">
+  <dimension ref="A1:T20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B3" t="s">
+        <v>422</v>
+      </c>
+      <c r="M3" t="s">
+        <v>512</v>
+      </c>
+      <c r="N3" t="s">
+        <v>513</v>
+      </c>
+      <c r="O3" t="s">
+        <v>514</v>
+      </c>
+      <c r="P3" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>514</v>
+      </c>
+      <c r="R3" t="s">
+        <v>515</v>
+      </c>
+      <c r="S3" t="s">
+        <v>516</v>
+      </c>
+      <c r="T3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B4" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>427</v>
+      </c>
+      <c r="B6" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" t="s">
+        <v>429</v>
+      </c>
+      <c r="M7" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>430</v>
+      </c>
+      <c r="M8" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>417</v>
+      </c>
+      <c r="B10" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>434</v>
+      </c>
+      <c r="B11" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B12" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B13" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>511</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF94A00-A6D2-49B1-9C65-88878417CF76}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="97.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
+        <v>546</v>
+      </c>
+      <c r="E3" t="s">
+        <v>440</v>
+      </c>
+      <c r="F3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>520</v>
+      </c>
+      <c r="B4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>521</v>
+      </c>
+      <c r="B5" t="s">
+        <v>392</v>
+      </c>
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>522</v>
+      </c>
+      <c r="B6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>524</v>
+      </c>
+      <c r="B7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>525</v>
+      </c>
+      <c r="B8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>523</v>
+      </c>
+      <c r="B9" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>519</v>
+      </c>
+      <c r="B10" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>518</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>526</v>
+      </c>
+      <c r="B12" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>527</v>
+      </c>
+      <c r="B13" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>528</v>
+      </c>
+      <c r="B14" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>529</v>
+      </c>
+      <c r="B15" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>530</v>
+      </c>
+      <c r="B16" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>531</v>
+      </c>
+      <c r="B17" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>532</v>
+      </c>
+      <c r="B18" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>533</v>
+      </c>
+      <c r="B19" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>534</v>
+      </c>
+      <c r="B20" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>535</v>
+      </c>
+      <c r="B21" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>536</v>
+      </c>
+      <c r="B22" t="s">
+        <v>409</v>
+      </c>
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>539</v>
+      </c>
+      <c r="B23" t="s">
+        <v>405</v>
+      </c>
+      <c r="C23" s="19"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>538</v>
+      </c>
+      <c r="B24" t="s">
+        <v>407</v>
+      </c>
+      <c r="C24" s="18"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>537</v>
+      </c>
+      <c r="B25" t="s">
+        <v>406</v>
+      </c>
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>540</v>
+      </c>
+      <c r="B26" t="s">
+        <v>411</v>
+      </c>
+      <c r="C26" s="18"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>541</v>
+      </c>
+      <c r="B27" t="s">
+        <v>416</v>
+      </c>
+      <c r="C27" s="19"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>542</v>
+      </c>
+      <c r="B28" t="s">
+        <v>413</v>
+      </c>
+      <c r="C28" s="18"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>543</v>
+      </c>
+      <c r="B29" t="s">
+        <v>412</v>
+      </c>
+      <c r="C29" s="19"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>544</v>
+      </c>
+      <c r="B30" t="s">
+        <v>414</v>
+      </c>
+      <c r="C30" s="18"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>545</v>
+      </c>
+      <c r="B31" t="s">
+        <v>415</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3E76D3-6A9A-4827-BA9C-4B17098CC9CF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27473039-7BF5-41BD-AAFA-F14B86FDFC50}">
   <dimension ref="A1:G30"/>
@@ -4491,7 +5470,7 @@
       <c r="A1" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="39" t="s">
         <v>223</v>
       </c>
       <c r="C1" s="33" t="s">
@@ -4503,10 +5482,10 @@
       <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="40" t="s">
         <v>219</v>
       </c>
       <c r="C2" s="35" t="s">
@@ -4517,8 +5496,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="43" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="40" t="s">
         <v>216</v>
       </c>
       <c r="C3" s="35" t="s">
@@ -4529,8 +5508,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="43" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="40" t="s">
         <v>213</v>
       </c>
       <c r="C4" s="35" t="s">
@@ -4541,8 +5520,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="43" t="s">
+      <c r="A5" s="49"/>
+      <c r="B5" s="40" t="s">
         <v>210</v>
       </c>
       <c r="C5" s="35" t="s">
@@ -4553,8 +5532,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="43" t="s">
+      <c r="A6" s="49"/>
+      <c r="B6" s="40" t="s">
         <v>207</v>
       </c>
       <c r="C6" s="35" t="s">
@@ -4565,8 +5544,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="40" t="s">
         <v>204</v>
       </c>
       <c r="C7" s="35" t="s">
@@ -4577,8 +5556,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="43" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="40" t="s">
         <v>201</v>
       </c>
       <c r="C8" s="35" t="s">
@@ -4589,16 +5568,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="43" t="s">
+      <c r="A9" s="49"/>
+      <c r="B9" s="40" t="s">
         <v>198</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="37"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="43" t="s">
+      <c r="A10" s="49"/>
+      <c r="B10" s="40" t="s">
         <v>197</v>
       </c>
       <c r="C10" s="32"/>
@@ -4606,40 +5585,40 @@
       <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="43" t="s">
+      <c r="A11" s="49"/>
+      <c r="B11" s="40" t="s">
         <v>196</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="37"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="43" t="s">
+      <c r="A12" s="49"/>
+      <c r="B12" s="40" t="s">
         <v>195</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="43" t="s">
+      <c r="A13" s="49"/>
+      <c r="B13" s="40" t="s">
         <v>194</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="43" t="s">
+      <c r="A14" s="49"/>
+      <c r="B14" s="40" t="s">
         <v>193</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="40" t="s">
         <v>192</v>
       </c>
       <c r="C15" s="32"/>
@@ -4674,7 +5653,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="41" t="s">
         <v>224</v>
       </c>
       <c r="B1" s="25" t="s">
@@ -4683,15 +5662,15 @@
       <c r="C1" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>281</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="43" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="51" t="s">
         <v>283</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -4711,7 +5690,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="47"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="27" t="s">
         <v>265</v>
       </c>
@@ -4729,7 +5708,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="47"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="27" t="s">
         <v>255</v>
       </c>
@@ -4747,7 +5726,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="47"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="27" t="s">
         <v>253</v>
       </c>
@@ -4762,7 +5741,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="27" t="s">
         <v>258</v>
       </c>
@@ -4777,7 +5756,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="27" t="s">
         <v>260</v>
       </c>
@@ -4788,7 +5767,7 @@
       <c r="E7" s="31"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="27" t="s">
         <v>261</v>
       </c>
@@ -4799,7 +5778,7 @@
       <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="27" t="s">
         <v>262</v>
       </c>
@@ -4810,7 +5789,7 @@
       <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="27" t="s">
         <v>250</v>
       </c>
@@ -4821,7 +5800,7 @@
       <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="27" t="s">
         <v>263</v>
       </c>
@@ -4832,7 +5811,7 @@
       <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="47"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="27" t="s">
         <v>264</v>
       </c>
@@ -4843,7 +5822,7 @@
       <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="47"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="27" t="s">
         <v>256</v>
       </c>
@@ -4854,7 +5833,7 @@
       <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="27" t="s">
         <v>254</v>
       </c>
@@ -4865,7 +5844,7 @@
       <c r="E14" s="31"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="27" t="s">
         <v>259</v>
       </c>
@@ -4876,7 +5855,7 @@
       <c r="E15" s="31"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="47"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="27" t="s">
         <v>267</v>
       </c>
@@ -4891,7 +5870,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="27" t="s">
         <v>268</v>
       </c>
@@ -4906,7 +5885,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="27" t="s">
         <v>266</v>
       </c>
@@ -4921,7 +5900,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="27" t="s">
         <v>257</v>
       </c>
@@ -4936,7 +5915,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
+      <c r="A20" s="52"/>
       <c r="B20" s="27" t="s">
         <v>269</v>
       </c>
@@ -4975,7 +5954,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="41" t="s">
         <v>224</v>
       </c>
       <c r="B1" s="25" t="s">
@@ -5025,7 +6004,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H8" t="str">
-        <f t="shared" ref="H5:H8" si="0">REPLACE(G8,1,$C$11,"")</f>
+        <f t="shared" ref="H8" si="0">REPLACE(G8,1,$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -5050,7 +6029,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="41" t="s">
         <v>314</v>
       </c>
       <c r="B1" s="25" t="s">
@@ -5167,7 +6146,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5181,7 +6160,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="47" t="s">
         <v>224</v>
       </c>
       <c r="B1" s="25" t="s">
@@ -5190,13 +6169,13 @@
       <c r="C1" s="26" t="s">
         <v>334</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="44" t="s">
         <v>335</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="44" t="s">
         <v>337</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="44" t="s">
         <v>338</v>
       </c>
     </row>
@@ -5204,17 +6183,17 @@
       <c r="A2" s="53" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="46" t="s">
         <v>322</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="45" t="s">
         <v>317</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="45" t="s">
         <v>347</v>
       </c>
       <c r="I2" t="s">
@@ -5223,19 +6202,19 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="54"/>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="46" t="s">
         <v>340</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="46" t="s">
         <v>320</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="45" t="s">
         <v>325</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="45" t="s">
         <v>346</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="45" t="s">
         <v>348</v>
       </c>
       <c r="I3" t="s">
@@ -5244,19 +6223,19 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="54"/>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="46" t="s">
         <v>341</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="46" t="s">
         <v>321</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="45" t="s">
         <v>327</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="45" t="s">
         <v>345</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="45" t="s">
         <v>349</v>
       </c>
       <c r="I4" t="s">
@@ -5268,19 +6247,19 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="54"/>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="46" t="s">
         <v>318</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="45" t="s">
         <v>328</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="45" t="s">
         <v>345</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="45" t="s">
         <v>350</v>
       </c>
       <c r="R5" t="s">
@@ -5289,40 +6268,40 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="46" t="s">
         <v>343</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="46" t="s">
         <v>319</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="45" t="s">
         <v>326</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="45" t="s">
         <v>345</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="45" t="s">
         <v>351</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="I6" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="J6" s="50" t="s">
+      <c r="J6" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="K6" s="50" t="s">
+      <c r="K6" s="45" t="s">
         <v>356</v>
       </c>
-      <c r="L6" s="50" t="s">
+      <c r="L6" s="45" t="s">
         <v>357</v>
       </c>
-      <c r="M6" s="50" t="s">
+      <c r="M6" s="45" t="s">
         <v>358</v>
       </c>
-      <c r="N6" s="50" t="s">
+      <c r="N6" s="45" t="s">
         <v>357</v>
       </c>
-      <c r="O6" s="50" t="s">
+      <c r="O6" s="45" t="s">
         <v>160</v>
       </c>
       <c r="R6" t="s">
@@ -5331,22 +6310,22 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="46" t="s">
         <v>344</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="45" t="s">
         <v>329</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="45" t="s">
         <v>345</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="45" t="s">
         <v>352</v>
       </c>
-      <c r="I7" s="50" t="s">
+      <c r="I7" s="45" t="s">
         <v>355</v>
       </c>
       <c r="J7" t="s">
@@ -5396,10 +6375,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D15C30-4CE2-4FE6-8ED7-DB2C8418632F}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5412,8 +6391,8 @@
     <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>224</v>
       </c>
       <c r="B1" s="25" t="s">
@@ -5422,101 +6401,101 @@
       <c r="C1" s="26" t="s">
         <v>379</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="44" t="s">
         <v>380</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="44" t="s">
         <v>381</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="44" t="s">
         <v>386</v>
       </c>
       <c r="H1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>363</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="46" t="s">
         <v>382</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="46" t="s">
         <v>369</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="45" t="s">
         <v>317</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="45" t="s">
         <v>302</v>
       </c>
       <c r="H2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="54"/>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="46" t="s">
         <v>383</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="46" t="s">
         <v>370</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="45" t="s">
         <v>325</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="45" t="s">
         <v>346</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="45" t="s">
         <v>348</v>
       </c>
       <c r="H3" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="54"/>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="46" t="s">
         <v>384</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="46" t="s">
         <v>371</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="45" t="s">
         <v>374</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="45" t="s">
         <v>345</v>
       </c>
-      <c r="F4" s="50" t="s">
+      <c r="F4" s="45" t="s">
         <v>388</v>
       </c>
       <c r="H4" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="54"/>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="46" t="s">
         <v>385</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="46" t="s">
         <v>372</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="45" t="s">
         <v>375</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="45" t="s">
         <v>345</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="45" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="54"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -5532,8 +6511,11 @@
       <c r="J6" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="54"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -5545,6 +6527,9 @@
       </c>
       <c r="J7" t="s">
         <v>373</v>
+      </c>
+      <c r="K7" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -5556,29 +6541,569 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3E76D3-6A9A-4827-BA9C-4B17098CC9CF}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396B2822-99EC-42E4-91AF-250489E95AB3}">
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>483</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>488</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>489</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>491</v>
+      </c>
+      <c r="D2" t="s">
+        <v>499</v>
+      </c>
+      <c r="E2" t="s">
+        <v>496</v>
+      </c>
+      <c r="G2" t="s">
+        <v>484</v>
+      </c>
+      <c r="J2" t="s">
+        <v>487</v>
+      </c>
+      <c r="K2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B3" t="s">
+        <v>450</v>
+      </c>
+      <c r="C3" t="s">
+        <v>490</v>
+      </c>
+      <c r="D3" t="s">
+        <v>498</v>
+      </c>
+      <c r="E3" t="s">
+        <v>496</v>
+      </c>
+      <c r="J3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B4" t="s">
+        <v>477</v>
+      </c>
+      <c r="C4" t="s">
+        <v>492</v>
+      </c>
+      <c r="D4" t="s">
+        <v>497</v>
+      </c>
+      <c r="E4" t="s">
+        <v>496</v>
+      </c>
+      <c r="G4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B5" t="s">
+        <v>451</v>
+      </c>
+      <c r="C5" t="s">
+        <v>493</v>
+      </c>
+      <c r="D5" t="s">
+        <v>500</v>
+      </c>
+      <c r="E5" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>494</v>
+      </c>
+      <c r="D6" t="s">
+        <v>501</v>
+      </c>
+      <c r="E6" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>495</v>
+      </c>
+      <c r="D7" t="s">
+        <v>502</v>
+      </c>
+      <c r="E7" t="s">
+        <v>504</v>
+      </c>
+      <c r="G7" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>449</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE00531-8080-48DE-8FA5-708A543CF7FA}">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>467</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>468</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>469</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>470</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>471</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="57" t="s">
+        <v>464</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>459</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>454</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>472</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>317</v>
+      </c>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="58"/>
+      <c r="B3" s="46" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>450</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>457</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>473</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>325</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>346</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="46" t="s">
+        <v>461</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>451</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>455</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="46" t="s">
+        <v>462</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>452</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>458</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>475</v>
+      </c>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="46" t="s">
+        <v>463</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>453</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>456</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>476</v>
+      </c>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="61"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="61"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="61"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="61"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="61"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="61"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="61"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="61"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="61"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="61"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="61"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="61"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="61"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="61"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="61"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="61"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A2:A6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100935E4B14CAE0794BBA76749019BEDAFD" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e8f083d54fb8f98c28d609697373e77">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c1e63f73-2b16-46a0-94d9-b08dde3039d7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3c9a3a28a489059020da38f7a939b45" ns2:_="">
     <xsd:import namespace="c1e63f73-2b16-46a0-94d9-b08dde3039d7"/>
@@ -5710,6 +7235,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5717,14 +7251,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61B3F181-E7E1-4FBA-8814-FA691E66D479}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0CBCE95-0DDE-458E-A141-8F35E0758221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5738,6 +7264,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61B3F181-E7E1-4FBA-8814-FA691E66D479}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Created Clinical Stain assay, created function to remove empty comments from I file, added option to write files to user directed file path, updated excel relationship file
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5DCBC4-3F8C-4035-AF98-494A314C4C71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709B9EA4-0C81-42B7-8263-9DBAA1F2D9B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="538">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -1301,75 +1301,12 @@
     <t>cell_line/metadata/custom/clinical/diagnosis/clinical_correlates/rho_over_d[@units]</t>
   </si>
   <si>
-    <t>stain</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain</t>
-  </si>
-  <si>
-    <t>cytoplasmic_stain</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/cytoplasmic_stain</t>
-  </si>
-  <si>
-    <t>membrane_stain</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/membrane_stain</t>
-  </si>
-  <si>
-    <t>nuclear_stain</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/nuclear_stain</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/source</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain/target</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain[@ID]</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_definitions/stain[@name]</t>
-  </si>
-  <si>
     <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_grade</t>
   </si>
   <si>
     <t>cell_line/metadata/custom/clinical/diagnosis/pathology/pathology_type</t>
   </si>
   <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain</t>
-  </si>
-  <si>
-    <t>positive_fraction</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain/positive_fraction</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain/positive_fraction[@measurement_type]</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain/positive_fraction[@units]</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain[@ID]</t>
-  </si>
-  <si>
-    <t>cell_line/metadata/custom/clinical/diagnosis/pathology/stain[@name]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -1580,18 +1517,6 @@
     <t>MultiCellDB Name</t>
   </si>
   <si>
-    <t>match the ID to data?</t>
-  </si>
-  <si>
-    <t>As of now, this data exists for every custom/clinical</t>
-  </si>
-  <si>
-    <t>Sample base</t>
-  </si>
-  <si>
-    <t>Stain Name</t>
-  </si>
-  <si>
     <t>Characteristic[Cytoplasmic Stain]</t>
   </si>
   <si>
@@ -1601,9 +1526,6 @@
     <t>Characteristic[Stain Source]</t>
   </si>
   <si>
-    <t>Parameter Value[Stain Positive Fraction]</t>
-  </si>
-  <si>
     <t>Characteristic[Cell Origin Company]</t>
   </si>
   <si>
@@ -1691,10 +1613,55 @@
     <t>In I file: is this needed?</t>
   </si>
   <si>
-    <t>Need to match Stain ID's</t>
-  </si>
-  <si>
-    <t>ID# is properly ordered - therefore, can write in order</t>
+    <t>Clinical Stain Properties xPaths</t>
+  </si>
+  <si>
+    <t>Clinical Stain Properties ISA Headers</t>
+  </si>
+  <si>
+    <t>/cytoplasmic_stain</t>
+  </si>
+  <si>
+    <t>/membrane_stain</t>
+  </si>
+  <si>
+    <t>/nuclear_stain</t>
+  </si>
+  <si>
+    <t>/source</t>
+  </si>
+  <si>
+    <t>/target</t>
+  </si>
+  <si>
+    <t>Clinical Stain Measurements ISA Header</t>
+  </si>
+  <si>
+    <t>/positive_fraction</t>
+  </si>
+  <si>
+    <t>/positive_fraction[@measurement_type]</t>
+  </si>
+  <si>
+    <t>/positive_fraction[@units]</t>
+  </si>
+  <si>
+    <t>Characteristic[Membrane Stain]</t>
+  </si>
+  <si>
+    <t>Characteristic[Nuclear Stain]</t>
+  </si>
+  <si>
+    <t>Parameter Value[Positive Fraction]</t>
+  </si>
+  <si>
+    <t>Positive Fraction - Units</t>
+  </si>
+  <si>
+    <t>Characteristic[Positive Fraction - Measurement Type]</t>
+  </si>
+  <si>
+    <t>Clinical Stain Measurements xPaths</t>
   </si>
 </sst>
 </file>
@@ -2488,8 +2455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FA11B-2D6D-4A50-A5F1-7D079DCC0D36}">
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4979,168 +4946,95 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A97BD1D-99EF-49BC-B0C5-86FC67BB4019}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>417</v>
-      </c>
-      <c r="B1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>522</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>528</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>419</v>
+        <v>489</v>
       </c>
       <c r="B2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+      <c r="C2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>421</v>
+        <v>532</v>
       </c>
       <c r="B3" t="s">
-        <v>422</v>
-      </c>
-      <c r="M3" t="s">
-        <v>512</v>
-      </c>
-      <c r="N3" t="s">
-        <v>513</v>
-      </c>
-      <c r="O3" t="s">
-        <v>514</v>
-      </c>
-      <c r="P3" t="s">
-        <v>514</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>514</v>
-      </c>
-      <c r="R3" t="s">
-        <v>515</v>
-      </c>
-      <c r="S3" t="s">
-        <v>516</v>
-      </c>
-      <c r="T3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+      <c r="C3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D3" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>423</v>
+        <v>533</v>
       </c>
       <c r="B4" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+      <c r="C4" t="s">
+        <v>536</v>
+      </c>
+      <c r="D4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>425</v>
+        <v>491</v>
       </c>
       <c r="B5" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>427</v>
+        <v>490</v>
       </c>
       <c r="B6" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" t="s">
-        <v>429</v>
-      </c>
-      <c r="M7" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>430</v>
-      </c>
-      <c r="M8" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>417</v>
-      </c>
-      <c r="B10" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>434</v>
-      </c>
-      <c r="B11" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>325</v>
-      </c>
-      <c r="B12" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>317</v>
-      </c>
-      <c r="B13" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B15" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>511</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5149,7 +5043,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5161,40 +5055,40 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="B2" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
       <c r="B3" t="s">
         <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>546</v>
+        <v>520</v>
       </c>
       <c r="E3" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
       <c r="F3" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>520</v>
+        <v>494</v>
       </c>
       <c r="B4" t="s">
         <v>391</v>
@@ -5202,7 +5096,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>521</v>
+        <v>495</v>
       </c>
       <c r="B5" t="s">
         <v>392</v>
@@ -5213,7 +5107,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>522</v>
+        <v>496</v>
       </c>
       <c r="B6" t="s">
         <v>394</v>
@@ -5224,7 +5118,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>524</v>
+        <v>498</v>
       </c>
       <c r="B7" t="s">
         <v>398</v>
@@ -5232,7 +5126,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>525</v>
+        <v>499</v>
       </c>
       <c r="B8" t="s">
         <v>399</v>
@@ -5240,7 +5134,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>523</v>
+        <v>497</v>
       </c>
       <c r="B9" t="s">
         <v>395</v>
@@ -5248,7 +5142,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>519</v>
+        <v>493</v>
       </c>
       <c r="B10" t="s">
         <v>393</v>
@@ -5256,7 +5150,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>518</v>
+        <v>492</v>
       </c>
       <c r="B11" t="s">
         <v>182</v>
@@ -5264,7 +5158,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>526</v>
+        <v>500</v>
       </c>
       <c r="B12" t="s">
         <v>396</v>
@@ -5272,7 +5166,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>527</v>
+        <v>501</v>
       </c>
       <c r="B13" t="s">
         <v>397</v>
@@ -5280,7 +5174,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>528</v>
+        <v>502</v>
       </c>
       <c r="B14" t="s">
         <v>401</v>
@@ -5288,7 +5182,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>529</v>
+        <v>503</v>
       </c>
       <c r="B15" t="s">
         <v>402</v>
@@ -5296,7 +5190,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>530</v>
+        <v>504</v>
       </c>
       <c r="B16" t="s">
         <v>404</v>
@@ -5304,7 +5198,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>531</v>
+        <v>505</v>
       </c>
       <c r="B17" t="s">
         <v>403</v>
@@ -5312,23 +5206,23 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>532</v>
+        <v>506</v>
       </c>
       <c r="B18" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>533</v>
+        <v>507</v>
       </c>
       <c r="B19" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>534</v>
+        <v>508</v>
       </c>
       <c r="B20" t="s">
         <v>408</v>
@@ -5336,7 +5230,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>535</v>
+        <v>509</v>
       </c>
       <c r="B21" t="s">
         <v>410</v>
@@ -5344,7 +5238,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>536</v>
+        <v>510</v>
       </c>
       <c r="B22" t="s">
         <v>409</v>
@@ -5353,7 +5247,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>539</v>
+        <v>513</v>
       </c>
       <c r="B23" t="s">
         <v>405</v>
@@ -5362,7 +5256,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>538</v>
+        <v>512</v>
       </c>
       <c r="B24" t="s">
         <v>407</v>
@@ -5371,7 +5265,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>537</v>
+        <v>511</v>
       </c>
       <c r="B25" t="s">
         <v>406</v>
@@ -5380,7 +5274,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
       <c r="B26" t="s">
         <v>411</v>
@@ -5389,7 +5283,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>541</v>
+        <v>515</v>
       </c>
       <c r="B27" t="s">
         <v>416</v>
@@ -5398,7 +5292,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>542</v>
+        <v>516</v>
       </c>
       <c r="B28" t="s">
         <v>413</v>
@@ -5407,7 +5301,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>543</v>
+        <v>517</v>
       </c>
       <c r="B29" t="s">
         <v>412</v>
@@ -5416,7 +5310,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>544</v>
+        <v>518</v>
       </c>
       <c r="B30" t="s">
         <v>414</v>
@@ -5425,7 +5319,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>545</v>
+        <v>519</v>
       </c>
       <c r="B31" t="s">
         <v>415</v>
@@ -6558,165 +6452,165 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>468</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>482</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>483</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>488</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>489</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="B2" t="s">
         <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="D2" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
       <c r="E2" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="G2" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="J2" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="K2" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="B3" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="C3" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
       <c r="D3" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="E3" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="J3" t="s">
         <v>151</v>
       </c>
       <c r="K3" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="B4" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="C4" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="D4" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="E4" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="G4" t="s">
-        <v>445</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
       <c r="B5" t="s">
-        <v>451</v>
+        <v>430</v>
       </c>
       <c r="C5" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="D5" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
       <c r="E5" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
       <c r="D6" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="E6" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="D7" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="E7" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
       <c r="G7" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -6750,42 +6644,42 @@
         <v>224</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
       <c r="C1" s="60" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
       <c r="H1" s="44" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>459</v>
+        <v>438</v>
       </c>
       <c r="C2" s="46" t="s">
         <v>136</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>454</v>
+        <v>433</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="F2" s="45" t="s">
         <v>317</v>
@@ -6798,16 +6692,16 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="58"/>
       <c r="B3" s="46" t="s">
-        <v>460</v>
+        <v>439</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="F3" s="45" t="s">
         <v>325</v>
@@ -6822,16 +6716,16 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="58"/>
       <c r="B4" s="46" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>451</v>
+        <v>430</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>455</v>
+        <v>434</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="F4" s="45"/>
       <c r="G4" s="45"/>
@@ -6840,16 +6734,16 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="46" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>458</v>
+        <v>437</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="F5" s="45"/>
       <c r="G5" s="45"/>
@@ -6858,16 +6752,16 @@
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="58"/>
       <c r="B6" s="46" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>456</v>
+        <v>435</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="F6" s="45"/>
       <c r="G6" s="45"/>

</xml_diff>

<commit_message>
Passes ISA validation (for a few examples anyways). Added protocols, parameter components to I file. Changed to writing assays with dataframes
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08383C4D-BC85-4DE4-A61D-BE2CA7DC2F82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E81280D-92C8-40DE-B279-842708DE846A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="11" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="604">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -1602,15 +1602,6 @@
     <t>study</t>
   </si>
   <si>
-    <t>submission</t>
-  </si>
-  <si>
-    <t>grant</t>
-  </si>
-  <si>
-    <t>funding</t>
-  </si>
-  <si>
     <t>design</t>
   </si>
   <si>
@@ -1656,9 +1647,6 @@
     <t>phenotype_factors</t>
   </si>
   <si>
-    <t>phenotype_factor_type</t>
-  </si>
-  <si>
     <t>MultiCellDS Digital Cell Line</t>
   </si>
   <si>
@@ -1861,6 +1849,18 @@
   </si>
   <si>
     <t>/finish/phenotype_dataset_collection_ID</t>
+  </si>
+  <si>
+    <t>release</t>
+  </si>
+  <si>
+    <t>factor type</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Script Variable?</t>
   </si>
 </sst>
 </file>
@@ -2967,8 +2967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FA11B-2D6D-4A50-A5F1-7D079DCC0D36}">
   <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="C101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3052,7 +3052,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A17" si="0">A3+1</f>
+        <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -3238,8 +3238,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B12" s="104" t="s">
         <v>15</v>
@@ -3249,12 +3248,6 @@
       </c>
       <c r="D12" s="104" t="s">
         <v>3</v>
-      </c>
-      <c r="E12" s="104" t="s">
-        <v>496</v>
-      </c>
-      <c r="F12" s="103" t="s">
-        <v>499</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>111</v>
@@ -3263,7 +3256,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>122</v>
@@ -3287,7 +3280,7 @@
     <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>125</v>
@@ -3310,8 +3303,12 @@
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="B15" s="4" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -3332,11 +3329,11 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f>A14+1</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -3348,7 +3345,7 @@
         <v>120</v>
       </c>
       <c r="F16" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>111</v>
@@ -3358,7 +3355,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>123</v>
@@ -3382,8 +3379,8 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f>A17+1</f>
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>124</v>
@@ -3407,8 +3404,8 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" ref="A19:A96" si="1">A18+1</f>
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>492</v>
@@ -3431,18 +3428,24 @@
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="103">
-        <f t="shared" si="1"/>
-        <v>18</v>
+      <c r="A20" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="B20" s="104" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="E20" s="104" t="s">
+        <v>496</v>
+      </c>
+      <c r="F20" s="103" t="s">
+        <v>499</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>111</v>
@@ -3451,8 +3454,8 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B21" s="91" t="s">
         <v>495</v>
@@ -3476,8 +3479,8 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B22" s="91" t="s">
         <v>500</v>
@@ -3492,7 +3495,7 @@
         <v>505</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>111</v>
@@ -3501,8 +3504,8 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="B23" s="91" t="s">
         <v>502</v>
@@ -3517,7 +3520,7 @@
         <v>507</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>111</v>
@@ -3526,8 +3529,8 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="B24" s="91" t="s">
         <v>501</v>
@@ -3542,7 +3545,7 @@
         <v>508</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>111</v>
@@ -3551,8 +3554,8 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="B25" s="91" t="s">
         <v>504</v>
@@ -3567,7 +3570,7 @@
         <v>509</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>111</v>
@@ -3576,8 +3579,8 @@
     </row>
     <row r="26" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="B26" s="91" t="s">
         <v>503</v>
@@ -3592,7 +3595,7 @@
         <v>510</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>111</v>
@@ -3601,8 +3604,8 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>16</v>
@@ -3622,8 +3625,8 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>17</v>
@@ -3645,8 +3648,8 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>18</v>
@@ -3668,8 +3671,8 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="B30" s="104" t="s">
         <v>19</v>
@@ -3681,10 +3684,10 @@
         <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>111</v>
@@ -3693,8 +3696,8 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="1"/>
-        <v>29</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B31" s="104" t="s">
         <v>20</v>
@@ -3706,10 +3709,10 @@
         <v>3</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>111</v>
@@ -3718,8 +3721,8 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="B32" s="104" t="s">
         <v>21</v>
@@ -3731,10 +3734,10 @@
         <v>3</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>111</v>
@@ -3743,8 +3746,8 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>22</v>
@@ -3766,8 +3769,8 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>23</v>
@@ -3789,11 +3792,11 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <f t="shared" si="1"/>
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -3805,7 +3808,7 @@
         <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>112</v>
@@ -3814,11 +3817,11 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="B36" s="91" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -3830,7 +3833,7 @@
         <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>112</v>
@@ -3839,11 +3842,11 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <f t="shared" si="1"/>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="B37" s="91" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -3852,10 +3855,10 @@
         <v>3</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F37" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>112</v>
@@ -3864,11 +3867,11 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="B38" s="91" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -3880,7 +3883,7 @@
         <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>112</v>
@@ -3889,11 +3892,11 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <f t="shared" si="1"/>
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="B39" s="91" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -3905,7 +3908,7 @@
         <v>109</v>
       </c>
       <c r="F39" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>112</v>
@@ -3914,11 +3917,11 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <f t="shared" si="1"/>
-        <v>38</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="B40" s="91" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -3927,10 +3930,10 @@
         <v>3</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="F40" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>112</v>
@@ -3939,11 +3942,11 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="B41" s="91" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -3952,10 +3955,10 @@
         <v>3</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="F41" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>112</v>
@@ -3964,11 +3967,11 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
       <c r="B42" s="91" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>4</v>
@@ -3980,7 +3983,7 @@
         <v>105</v>
       </c>
       <c r="F42" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>112</v>
@@ -3989,11 +3992,11 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="B43" s="91" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -4002,10 +4005,10 @@
         <v>3</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F43" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>112</v>
@@ -4014,11 +4017,11 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <f t="shared" si="1"/>
-        <v>42</v>
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
       <c r="B44" s="91" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -4030,7 +4033,7 @@
         <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>112</v>
@@ -4039,11 +4042,11 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <f t="shared" si="1"/>
-        <v>43</v>
+        <f t="shared" si="0"/>
+        <v>38</v>
       </c>
       <c r="B45" s="91" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -4055,7 +4058,7 @@
         <v>121</v>
       </c>
       <c r="F45" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>112</v>
@@ -4064,11 +4067,11 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="B46" s="91" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -4080,7 +4083,7 @@
         <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>112</v>
@@ -4089,11 +4092,11 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <f t="shared" si="1"/>
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="B47" s="91" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>4</v>
@@ -4105,7 +4108,7 @@
         <v>118</v>
       </c>
       <c r="F47" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>112</v>
@@ -4114,11 +4117,11 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <f t="shared" si="1"/>
-        <v>46</v>
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
       <c r="B48" s="91" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>4</v>
@@ -4130,7 +4133,7 @@
         <v>109</v>
       </c>
       <c r="F48" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>112</v>
@@ -4139,8 +4142,8 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <f t="shared" si="1"/>
-        <v>47</v>
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>24</v>
@@ -4160,8 +4163,8 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <f t="shared" si="1"/>
-        <v>48</v>
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>25</v>
@@ -4185,8 +4188,8 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <f t="shared" si="1"/>
-        <v>49</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>26</v>
@@ -4210,8 +4213,8 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>27</v>
@@ -4222,7 +4225,9 @@
       <c r="D52" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="4" t="s">
+        <v>514</v>
+      </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6" t="s">
         <v>111</v>
@@ -4231,8 +4236,8 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <f t="shared" si="1"/>
-        <v>51</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>28</v>
@@ -4256,8 +4261,8 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <f t="shared" si="1"/>
-        <v>52</v>
+        <f t="shared" si="0"/>
+        <v>47</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>29</v>
@@ -4279,8 +4284,8 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <f t="shared" si="1"/>
-        <v>53</v>
+        <f t="shared" si="0"/>
+        <v>48</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>30</v>
@@ -4302,8 +4307,8 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <f t="shared" si="1"/>
-        <v>54</v>
+        <f t="shared" si="0"/>
+        <v>49</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>31</v>
@@ -4325,8 +4330,8 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <f t="shared" si="1"/>
-        <v>55</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>32</v>
@@ -4351,8 +4356,8 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <f t="shared" si="1"/>
-        <v>56</v>
+        <f t="shared" si="0"/>
+        <v>51</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>33</v>
@@ -4376,8 +4381,8 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <f t="shared" si="1"/>
-        <v>57</v>
+        <f t="shared" si="0"/>
+        <v>52</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>34</v>
@@ -4399,8 +4404,8 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <f t="shared" si="1"/>
-        <v>58</v>
+        <f t="shared" si="0"/>
+        <v>53</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>35</v>
@@ -4422,8 +4427,8 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <f t="shared" si="1"/>
-        <v>59</v>
+        <f t="shared" si="0"/>
+        <v>54</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>481</v>
@@ -4447,8 +4452,8 @@
     </row>
     <row r="62" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>55</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>36</v>
@@ -4472,8 +4477,8 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <f t="shared" si="1"/>
-        <v>61</v>
+        <f t="shared" si="0"/>
+        <v>56</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>37</v>
@@ -4491,8 +4496,8 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <f t="shared" si="1"/>
-        <v>62</v>
+        <f t="shared" si="0"/>
+        <v>57</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>38</v>
@@ -4516,8 +4521,8 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <f t="shared" si="1"/>
-        <v>63</v>
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>39</v>
@@ -4541,8 +4546,8 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <f t="shared" si="1"/>
-        <v>64</v>
+        <f t="shared" si="0"/>
+        <v>59</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>40</v>
@@ -4566,8 +4571,8 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <f t="shared" si="1"/>
-        <v>65</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>43</v>
@@ -4579,7 +4584,7 @@
         <v>3</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>517</v>
+        <v>600</v>
       </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6" t="s">
@@ -4589,8 +4594,8 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <f t="shared" si="1"/>
-        <v>66</v>
+        <f t="shared" ref="A68:A128" si="1">A67+1</f>
+        <v>61</v>
       </c>
       <c r="B68" s="91" t="s">
         <v>44</v>
@@ -4601,12 +4606,8 @@
       <c r="D68" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E68" s="91" t="s">
-        <v>496</v>
-      </c>
-      <c r="F68" s="92" t="s">
-        <v>499</v>
-      </c>
+      <c r="E68" s="91"/>
+      <c r="F68" s="92"/>
       <c r="G68" s="6" t="s">
         <v>111</v>
       </c>
@@ -4615,7 +4616,7 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>45</v>
@@ -4627,10 +4628,10 @@
         <v>3</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G69" s="6" t="s">
         <v>111</v>
@@ -4640,7 +4641,7 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>41</v>
@@ -4651,9 +4652,7 @@
       <c r="D70" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="4" t="s">
-        <v>518</v>
-      </c>
+      <c r="E70" s="4"/>
       <c r="F70" s="6"/>
       <c r="G70" s="6" t="s">
         <v>111</v>
@@ -4663,7 +4662,7 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>42</v>
@@ -4674,9 +4673,7 @@
       <c r="D71" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>519</v>
-      </c>
+      <c r="E71" s="4"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6" t="s">
         <v>111</v>
@@ -4686,7 +4683,7 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>46</v>
@@ -4698,7 +4695,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
@@ -4707,7 +4704,7 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B73" s="105" t="s">
         <v>47</v>
@@ -4719,7 +4716,7 @@
         <v>3</v>
       </c>
       <c r="E73" s="105" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="F73" s="107" t="s">
         <v>110</v>
@@ -4732,7 +4729,7 @@
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>48</v>
@@ -4755,7 +4752,7 @@
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>49</v>
@@ -4778,7 +4775,7 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>50</v>
@@ -4799,7 +4796,7 @@
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>51</v>
@@ -4811,7 +4808,7 @@
         <v>3</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F77" s="6"/>
       <c r="G77" s="6" t="s">
@@ -4822,7 +4819,7 @@
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>52</v>
@@ -4845,7 +4842,7 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B79" s="108" t="s">
         <v>53</v>
@@ -4857,10 +4854,10 @@
         <v>3</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>111</v>
@@ -4869,7 +4866,7 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B80" s="108" t="s">
         <v>54</v>
@@ -4881,10 +4878,10 @@
         <v>3</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>111</v>
@@ -4894,7 +4891,7 @@
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B81" s="108" t="s">
         <v>55</v>
@@ -4906,10 +4903,10 @@
         <v>3</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>111</v>
@@ -4919,7 +4916,7 @@
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>56</v>
@@ -4942,7 +4939,7 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <f t="shared" si="1"/>
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>57</v>
@@ -4965,7 +4962,7 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>126</v>
@@ -4988,7 +4985,7 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>127</v>
@@ -5000,7 +4997,7 @@
         <v>3</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F85" s="16"/>
       <c r="G85" s="6" t="s">
@@ -5011,7 +5008,7 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>58</v>
@@ -5032,7 +5029,7 @@
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B87" s="109" t="s">
         <v>59</v>
@@ -5044,10 +5041,10 @@
         <v>3</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>112</v>
@@ -5057,7 +5054,7 @@
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B88" s="109" t="s">
         <v>60</v>
@@ -5069,20 +5066,18 @@
         <v>3</v>
       </c>
       <c r="E88" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6" t="s">
         <v>535</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="H88" s="6"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>61</v>
@@ -5097,13 +5092,13 @@
         <v>515</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>62</v>
@@ -5119,14 +5114,14 @@
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="6" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="H90" s="6"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>63</v>
@@ -5147,7 +5142,7 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B92" s="109" t="s">
         <v>71</v>
@@ -5159,10 +5154,10 @@
         <v>3</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>112</v>
@@ -5171,7 +5166,7 @@
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <f t="shared" si="1"/>
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B93" s="109" t="s">
         <v>64</v>
@@ -5183,10 +5178,10 @@
         <v>3</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>112</v>
@@ -5195,7 +5190,7 @@
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>65</v>
@@ -5211,13 +5206,13 @@
       </c>
       <c r="F94" s="6"/>
       <c r="G94" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>66</v>
@@ -5233,13 +5228,13 @@
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <f t="shared" si="1"/>
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>67</v>
@@ -5252,13 +5247,13 @@
       </c>
       <c r="E96" s="4"/>
       <c r="G96" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <f t="shared" ref="A97:A129" si="2">A96+1</f>
-        <v>95</v>
+        <f t="shared" si="1"/>
+        <v>90</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>68</v>
@@ -5274,13 +5269,13 @@
       </c>
       <c r="F97" s="6"/>
       <c r="G97" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <f t="shared" si="2"/>
-        <v>96</v>
+        <f t="shared" si="1"/>
+        <v>91</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>69</v>
@@ -5296,13 +5291,13 @@
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <f t="shared" si="2"/>
-        <v>97</v>
+        <f t="shared" si="1"/>
+        <v>92</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>70</v>
@@ -5318,13 +5313,13 @@
       </c>
       <c r="F99" s="16"/>
       <c r="G99" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <f t="shared" si="2"/>
-        <v>98</v>
+        <f t="shared" si="1"/>
+        <v>93</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>72</v>
@@ -5344,8 +5339,8 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <f t="shared" si="2"/>
-        <v>99</v>
+        <f t="shared" si="1"/>
+        <v>94</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>73</v>
@@ -5357,18 +5352,20 @@
         <v>3</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="F101" s="6"/>
+        <v>520</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>527</v>
+      </c>
       <c r="G101" s="6" t="s">
-        <v>538</v>
+        <v>112</v>
       </c>
       <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>95</v>
       </c>
       <c r="B102" s="4" t="s">
         <v>74</v>
@@ -5380,18 +5377,20 @@
         <v>3</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="F102" s="6"/>
+        <v>516</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>527</v>
+      </c>
       <c r="G102" s="6" t="s">
-        <v>538</v>
+        <v>112</v>
       </c>
       <c r="H102" s="6"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <f t="shared" si="2"/>
-        <v>101</v>
+        <f t="shared" si="1"/>
+        <v>96</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>75</v>
@@ -5407,14 +5406,14 @@
       </c>
       <c r="F103" s="6"/>
       <c r="G103" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H103" s="6"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <f t="shared" si="2"/>
-        <v>102</v>
+        <f t="shared" si="1"/>
+        <v>97</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>76</v>
@@ -5430,14 +5429,14 @@
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H104" s="6"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <f t="shared" si="2"/>
-        <v>103</v>
+        <f t="shared" si="1"/>
+        <v>98</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>77</v>
@@ -5448,19 +5447,19 @@
       <c r="D105" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E105" s="4" t="s">
-        <v>523</v>
+      <c r="E105" s="6" t="s">
+        <v>603</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H105" s="6"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <f t="shared" si="2"/>
-        <v>104</v>
+        <f t="shared" si="1"/>
+        <v>99</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>78</v>
@@ -5472,18 +5471,18 @@
         <v>3</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H106" s="6"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <f t="shared" si="2"/>
-        <v>105</v>
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>79</v>
@@ -5495,18 +5494,18 @@
         <v>3</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H107" s="6"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <f t="shared" si="2"/>
-        <v>106</v>
+        <f t="shared" si="1"/>
+        <v>101</v>
       </c>
       <c r="B108" s="109" t="s">
         <v>80</v>
@@ -5518,10 +5517,10 @@
         <v>3</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="G108" s="5" t="s">
         <v>112</v>
@@ -5530,8 +5529,8 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <f t="shared" si="2"/>
-        <v>107</v>
+        <f t="shared" si="1"/>
+        <v>102</v>
       </c>
       <c r="B109" s="4" t="s">
         <v>81</v>
@@ -5547,14 +5546,14 @@
       </c>
       <c r="F109" s="6"/>
       <c r="G109" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H109" s="6"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <f t="shared" si="2"/>
-        <v>108</v>
+        <f t="shared" si="1"/>
+        <v>103</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>82</v>
@@ -5569,14 +5568,14 @@
         <v>513</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H110" s="6"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <f t="shared" si="2"/>
-        <v>109</v>
+        <f t="shared" si="1"/>
+        <v>104</v>
       </c>
       <c r="B111" s="4" t="s">
         <v>83</v>
@@ -5588,16 +5587,18 @@
         <v>3</v>
       </c>
       <c r="E111" s="4"/>
-      <c r="F111" s="6"/>
+      <c r="F111" s="6" t="s">
+        <v>527</v>
+      </c>
       <c r="G111" s="6" t="s">
-        <v>538</v>
+        <v>112</v>
       </c>
       <c r="H111" s="6"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <f t="shared" si="2"/>
-        <v>110</v>
+        <f t="shared" si="1"/>
+        <v>105</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>84</v>
@@ -5611,14 +5612,14 @@
       <c r="E112" s="4"/>
       <c r="F112" s="6"/>
       <c r="G112" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H112" s="6"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <f t="shared" si="2"/>
-        <v>111</v>
+        <f t="shared" si="1"/>
+        <v>106</v>
       </c>
       <c r="B113" s="4" t="s">
         <v>85</v>
@@ -5634,14 +5635,14 @@
       </c>
       <c r="F113" s="6"/>
       <c r="G113" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H113" s="6"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <f t="shared" si="2"/>
-        <v>112</v>
+        <f t="shared" si="1"/>
+        <v>107</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>86</v>
@@ -5656,14 +5657,14 @@
         <v>513</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="H114" s="6"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <f t="shared" si="2"/>
-        <v>113</v>
+        <f t="shared" si="1"/>
+        <v>108</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>87</v>
@@ -5682,8 +5683,8 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <f t="shared" si="2"/>
-        <v>114</v>
+        <f t="shared" si="1"/>
+        <v>109</v>
       </c>
       <c r="B116" s="4" t="s">
         <v>88</v>
@@ -5694,7 +5695,9 @@
       <c r="D116" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E116" s="4"/>
+      <c r="E116" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F116" s="6" t="s">
         <v>142</v>
       </c>
@@ -5705,8 +5708,8 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <f t="shared" si="2"/>
-        <v>115</v>
+        <f t="shared" si="1"/>
+        <v>110</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>89</v>
@@ -5717,7 +5720,9 @@
       <c r="D117" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E117" s="4"/>
+      <c r="E117" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="F117" s="6" t="s">
         <v>143</v>
       </c>
@@ -5728,8 +5733,8 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <f t="shared" si="2"/>
-        <v>116</v>
+        <f t="shared" si="1"/>
+        <v>111</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>90</v>
@@ -5740,7 +5745,9 @@
       <c r="D118" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E118" s="4"/>
+      <c r="E118" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="F118" s="6"/>
       <c r="G118" s="5" t="s">
         <v>148</v>
@@ -5749,8 +5756,8 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <f t="shared" si="2"/>
-        <v>117</v>
+        <f t="shared" si="1"/>
+        <v>112</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>91</v>
@@ -5774,8 +5781,8 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <f t="shared" si="2"/>
-        <v>118</v>
+        <f t="shared" si="1"/>
+        <v>113</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>92</v>
@@ -5797,8 +5804,8 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <f t="shared" si="2"/>
-        <v>119</v>
+        <f t="shared" si="1"/>
+        <v>114</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>93</v>
@@ -5818,8 +5825,8 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <f t="shared" si="2"/>
-        <v>120</v>
+        <f t="shared" si="1"/>
+        <v>115</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>94</v>
@@ -5840,8 +5847,8 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <f t="shared" si="2"/>
-        <v>121</v>
+        <f t="shared" si="1"/>
+        <v>116</v>
       </c>
       <c r="B123" s="4" t="s">
         <v>95</v>
@@ -5853,7 +5860,7 @@
         <v>3</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>514</v>
+        <v>116</v>
       </c>
       <c r="F123" s="6" t="s">
         <v>147</v>
@@ -5865,8 +5872,8 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <f t="shared" si="2"/>
-        <v>122</v>
+        <f t="shared" si="1"/>
+        <v>117</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>96</v>
@@ -5878,7 +5885,7 @@
         <v>3</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>514</v>
+        <v>602</v>
       </c>
       <c r="F124" s="6" t="s">
         <v>146</v>
@@ -5889,8 +5896,8 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <f t="shared" si="2"/>
-        <v>123</v>
+        <f t="shared" si="1"/>
+        <v>118</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>97</v>
@@ -5910,8 +5917,8 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <f t="shared" si="2"/>
-        <v>124</v>
+        <f t="shared" si="1"/>
+        <v>119</v>
       </c>
       <c r="B126" s="4" t="s">
         <v>98</v>
@@ -5931,8 +5938,8 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <f t="shared" si="2"/>
-        <v>125</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="B127" s="4" t="s">
         <v>482</v>
@@ -5944,7 +5951,7 @@
         <v>3</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>514</v>
+        <v>120</v>
       </c>
       <c r="F127" s="6" t="s">
         <v>145</v>
@@ -5955,8 +5962,8 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <f t="shared" si="2"/>
-        <v>126</v>
+        <f t="shared" si="1"/>
+        <v>121</v>
       </c>
       <c r="B128" s="7" t="s">
         <v>99</v>
@@ -5987,7 +5994,7 @@
       <c r="B131" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:G1 E122 G3:G5 E3:E5 F6:G6 H1:H18 E19 G19 E123:G1048576 G122 E67:G121 E7:G18 H27:H1048576 E21:E26 G21:G26 E27:G55">
+  <conditionalFormatting sqref="E1:G1 E122 G3:G5 E3:E5 F6:G6 H1:H18 E19 G19 E123:G1048576 G122 H27:H1048576 E21:E26 G21:G26 E27:G55 E7:G11 E13:G18 G12 E20:F20 E67:G101 E103:G121 G102 E102">
     <cfRule type="expression" dxfId="13" priority="20">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
@@ -6067,7 +6074,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6225,7 +6232,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6624,8 +6631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E22B35-2D1E-461B-B9C7-98553FB27C66}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6644,93 +6651,93 @@
         <v>443</v>
       </c>
       <c r="B1" s="110" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C1" s="111" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="97"/>
       <c r="B3" s="48" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C3" s="112" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="97"/>
       <c r="D4" s="37" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="97"/>
       <c r="D5" s="37" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="97"/>
       <c r="D6" s="37" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="97"/>
       <c r="D7" s="37" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="97"/>
       <c r="D8" s="39" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E8" s="63" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6763,17 +6770,17 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
@@ -6782,7 +6789,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
@@ -7276,7 +7283,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7481,7 +7488,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7797,7 +7804,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7885,7 +7892,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8056,7 +8063,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8382,8 +8389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D15C30-4CE2-4FE6-8ED7-DB2C8418632F}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8532,7 +8539,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minor fixes for MCDS2ISA script (issue using .title() for headers), ISA2MCDS script works for I and S file entity conversions
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEB323B-8E29-4D46-8EB5-91CE415A9594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AADD40-C1D6-44DD-A38D-5A5F59992E08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="608">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -1263,9 +1263,6 @@
     <t>Parameter Value[Patient Age at Diagnosis]</t>
   </si>
   <si>
-    <t>Patient Age at Diagnosis - Units</t>
-  </si>
-  <si>
     <t>Characteristic[Patient Age at Diagnosis Measurement Type]</t>
   </si>
   <si>
@@ -1278,27 +1275,18 @@
     <t>Parameter Value[Overall Survival]</t>
   </si>
   <si>
-    <t>Overall Survival - Units</t>
-  </si>
-  <si>
     <t>Characteristic[Overall Survival - Measurement Type]</t>
   </si>
   <si>
     <t>Characteristic[D/Rho - Measurement Type]</t>
   </si>
   <si>
-    <t>D/Rho - Units</t>
-  </si>
-  <si>
     <t>Parameter Value[D/Rho]</t>
   </si>
   <si>
     <t>Parameter Value[Rho/D]</t>
   </si>
   <si>
-    <t>Rho/D - Units</t>
-  </si>
-  <si>
     <t>Characteristic[Rho/D - Measurement Type]</t>
   </si>
   <si>
@@ -1734,9 +1722,6 @@
     <t>Comment[Data Origins PMCID]</t>
   </si>
   <si>
-    <t>Comment[Data Origin PMID]</t>
-  </si>
-  <si>
     <t>Comment[Data Origins URL]</t>
   </si>
   <si>
@@ -1864,6 +1849,30 @@
   </si>
   <si>
     <t>Multiple - Study Protocol Name</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Mult-join</t>
+  </si>
+  <si>
+    <t>Comment[Data Origins PMID]</t>
+  </si>
+  <si>
+    <t>Comment[Investigation Person ORCID iD]</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/path</t>
+  </si>
+  <si>
+    <t>Comment[Study Person ORCID iD]</t>
+  </si>
+  <si>
+    <t>cell_line/metadata/curation/current_contact/orcid-identifier/path, cell_line/metadata/curation/curator/orcid-identifier/path, cell_line/metadata/curation/creator/orcid-identifier/path,  cell_line/metadata/curation/last_modified_by/orcid-identifier/path</t>
   </si>
 </sst>
 </file>
@@ -2559,7 +2568,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -2655,6 +2664,13 @@
       <fill>
         <patternFill>
           <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2968,10 +2984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FA11B-2D6D-4A50-A5F1-7D079DCC0D36}">
-  <dimension ref="A1:J131"/>
+  <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="B91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3044,7 +3060,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>110</v>
@@ -3055,7 +3071,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A67" si="0">A3+1</f>
+        <f t="shared" ref="A4:A68" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -3068,7 +3084,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>110</v>
@@ -3092,7 +3108,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>110</v>
@@ -3116,7 +3132,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>110</v>
@@ -3311,7 +3327,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -3336,7 +3352,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -3348,7 +3364,7 @@
         <v>120</v>
       </c>
       <c r="F16" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>111</v>
@@ -3411,7 +3427,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -3420,10 +3436,10 @@
         <v>3</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>111</v>
@@ -3436,7 +3452,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="104" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -3445,10 +3461,10 @@
         <v>3</v>
       </c>
       <c r="E20" s="104" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F20" s="103" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>111</v>
@@ -3461,7 +3477,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="91" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -3470,10 +3486,10 @@
         <v>3</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>111</v>
@@ -3486,7 +3502,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="91" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -3495,10 +3511,10 @@
         <v>3</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>111</v>
@@ -3511,7 +3527,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="91" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -3520,10 +3536,10 @@
         <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>111</v>
@@ -3536,7 +3552,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="91" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -3545,10 +3561,10 @@
         <v>3</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>111</v>
@@ -3561,7 +3577,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="91" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -3570,10 +3586,10 @@
         <v>3</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>111</v>
@@ -3586,7 +3602,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -3595,10 +3611,10 @@
         <v>3</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>111</v>
@@ -3620,7 +3636,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -3687,10 +3703,10 @@
         <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>111</v>
@@ -3712,10 +3728,10 @@
         <v>3</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>111</v>
@@ -3737,10 +3753,10 @@
         <v>3</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>111</v>
@@ -3762,7 +3778,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
@@ -3785,7 +3801,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6" t="s">
@@ -3799,7 +3815,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -3811,7 +3827,7 @@
         <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>112</v>
@@ -3824,7 +3840,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="91" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -3836,7 +3852,7 @@
         <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>112</v>
@@ -3849,7 +3865,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="91" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -3858,10 +3874,10 @@
         <v>3</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="F37" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>112</v>
@@ -3874,7 +3890,7 @@
         <v>31</v>
       </c>
       <c r="B38" s="91" t="s">
-        <v>561</v>
+        <v>602</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -3886,7 +3902,7 @@
         <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>112</v>
@@ -3899,7 +3915,7 @@
         <v>32</v>
       </c>
       <c r="B39" s="91" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -3911,10 +3927,10 @@
         <v>109</v>
       </c>
       <c r="F39" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>112</v>
+        <v>601</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -3924,7 +3940,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="91" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -3933,10 +3949,10 @@
         <v>3</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="F40" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>112</v>
@@ -3949,7 +3965,7 @@
         <v>34</v>
       </c>
       <c r="B41" s="91" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -3958,10 +3974,10 @@
         <v>3</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="F41" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>112</v>
@@ -3974,7 +3990,7 @@
         <v>35</v>
       </c>
       <c r="B42" s="91" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>4</v>
@@ -3986,7 +4002,7 @@
         <v>105</v>
       </c>
       <c r="F42" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>112</v>
@@ -3999,7 +4015,7 @@
         <v>36</v>
       </c>
       <c r="B43" s="91" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -4008,10 +4024,10 @@
         <v>3</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="F43" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>112</v>
@@ -4024,7 +4040,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="91" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -4036,7 +4052,7 @@
         <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>112</v>
@@ -4049,7 +4065,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="91" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -4061,7 +4077,7 @@
         <v>121</v>
       </c>
       <c r="F45" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>112</v>
@@ -4074,7 +4090,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="91" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -4086,10 +4102,10 @@
         <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>112</v>
+        <v>601</v>
       </c>
       <c r="H46" s="2"/>
     </row>
@@ -4099,7 +4115,7 @@
         <v>40</v>
       </c>
       <c r="B47" s="91" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>4</v>
@@ -4111,7 +4127,7 @@
         <v>118</v>
       </c>
       <c r="F47" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>112</v>
@@ -4124,7 +4140,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="91" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>4</v>
@@ -4136,7 +4152,7 @@
         <v>109</v>
       </c>
       <c r="F48" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>112</v>
@@ -4158,7 +4174,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
@@ -4229,7 +4245,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6" t="s">
@@ -4277,7 +4293,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6" t="s">
@@ -4300,7 +4316,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6" t="s">
@@ -4323,7 +4339,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>111</v>
@@ -4349,7 +4365,7 @@
         <v>116</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>111</v>
@@ -4397,7 +4413,7 @@
         <v>3</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6" t="s">
@@ -4420,7 +4436,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6" t="s">
@@ -4434,7 +4450,7 @@
         <v>54</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>4</v>
@@ -4453,82 +4469,78 @@
       </c>
       <c r="H61" s="6"/>
     </row>
-    <row r="62" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="7" t="s">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="F62" s="8"/>
+        <v>604</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>605</v>
+      </c>
       <c r="G62" s="6" t="s">
         <v>111</v>
       </c>
       <c r="H62" s="6"/>
-      <c r="I62"/>
-      <c r="J62"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>37</v>
+        <f>A61+1</f>
+        <v>55</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E63" s="13"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
+      <c r="D63" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="F63" s="8"/>
+      <c r="G63" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="H63" s="6"/>
+      <c r="I63"/>
+      <c r="J63"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E64" s="13"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
       <c r="H64" s="6"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>4</v>
@@ -4537,10 +4549,10 @@
         <v>3</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>111</v>
@@ -4550,10 +4562,10 @@
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C66" s="7" t="s">
         <v>4</v>
@@ -4562,10 +4574,10 @@
         <v>3</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>111</v>
@@ -4575,10 +4587,10 @@
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>4</v>
@@ -4587,9 +4599,11 @@
         <v>3</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="F67" s="6"/>
+        <v>512</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="G67" s="6" t="s">
         <v>111</v>
       </c>
@@ -4597,11 +4611,11 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <f t="shared" ref="A68:A128" si="1">A67+1</f>
-        <v>61</v>
-      </c>
-      <c r="B68" s="91" t="s">
-        <v>44</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>4</v>
@@ -4609,8 +4623,10 @@
       <c r="D68" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E68" s="91"/>
-      <c r="F68" s="92"/>
+      <c r="E68" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="F68" s="6"/>
       <c r="G68" s="6" t="s">
         <v>111</v>
       </c>
@@ -4618,11 +4634,11 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>45</v>
+        <f t="shared" ref="A69:A128" si="1">A68+1</f>
+        <v>61</v>
+      </c>
+      <c r="B69" s="91" t="s">
+        <v>44</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>4</v>
@@ -4630,12 +4646,8 @@
       <c r="D69" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="4" t="s">
-        <v>528</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>527</v>
-      </c>
+      <c r="E69" s="91"/>
+      <c r="F69" s="92"/>
       <c r="G69" s="6" t="s">
         <v>111</v>
       </c>
@@ -4644,10 +4656,10 @@
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <f t="shared" si="1"/>
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>4</v>
@@ -4655,8 +4667,12 @@
       <c r="D70" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="4"/>
-      <c r="F70" s="6"/>
+      <c r="E70" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>523</v>
+      </c>
       <c r="G70" s="6" t="s">
         <v>111</v>
       </c>
@@ -4665,10 +4681,10 @@
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>4</v>
@@ -4686,79 +4702,77 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>46</v>
+        <v>64</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>517</v>
-      </c>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="E72" s="4"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="H72" s="6"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <f t="shared" si="1"/>
-        <v>66</v>
-      </c>
-      <c r="B73" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="C73" s="106" t="s">
-        <v>4</v>
-      </c>
-      <c r="D73" s="105" t="s">
-        <v>3</v>
-      </c>
-      <c r="E73" s="105" t="s">
-        <v>532</v>
-      </c>
-      <c r="F73" s="107" t="s">
-        <v>110</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>491</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>513</v>
+      </c>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
       <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="F74" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="B74" s="105" t="s">
+        <v>47</v>
+      </c>
+      <c r="C74" s="106" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="105" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="105" t="s">
+        <v>528</v>
+      </c>
+      <c r="F74" s="107" t="s">
+        <v>110</v>
+      </c>
       <c r="G74" s="6" t="s">
-        <v>111</v>
+        <v>487</v>
       </c>
       <c r="H74" s="6"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>4</v>
@@ -4767,7 +4781,7 @@
         <v>3</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F75" s="6"/>
       <c r="G75" s="6" t="s">
@@ -4778,54 +4792,54 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>50</v>
+        <v>68</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E76" s="13" t="s">
-        <v>516</v>
-      </c>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="H76" s="6"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>51</v>
+        <v>69</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="F77" s="6"/>
-      <c r="G77" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
       <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>4</v>
@@ -4834,7 +4848,7 @@
         <v>3</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6" t="s">
@@ -4845,10 +4859,10 @@
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="B79" s="108" t="s">
-        <v>53</v>
+        <v>71</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>4</v>
@@ -4857,22 +4871,21 @@
         <v>3</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>537</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>527</v>
-      </c>
+        <v>508</v>
+      </c>
+      <c r="F79" s="6"/>
       <c r="G79" s="6" t="s">
         <v>111</v>
       </c>
+      <c r="H79" s="6"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B80" s="108" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>4</v>
@@ -4881,23 +4894,22 @@
         <v>3</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="H80" s="6"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B81" s="108" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>4</v>
@@ -4906,10 +4918,10 @@
         <v>3</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>111</v>
@@ -4919,10 +4931,10 @@
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>56</v>
+        <v>74</v>
+      </c>
+      <c r="B82" s="108" t="s">
+        <v>55</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>4</v>
@@ -4931,9 +4943,11 @@
         <v>3</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="F82" s="6"/>
+        <v>535</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>523</v>
+      </c>
       <c r="G82" s="6" t="s">
         <v>111</v>
       </c>
@@ -4942,10 +4956,10 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>4</v>
@@ -4954,7 +4968,7 @@
         <v>3</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="6" t="s">
@@ -4965,10 +4979,10 @@
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>4</v>
@@ -4977,9 +4991,9 @@
         <v>3</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="F84"/>
+        <v>509</v>
+      </c>
+      <c r="F84" s="6"/>
       <c r="G84" s="6" t="s">
         <v>111</v>
       </c>
@@ -4988,10 +5002,10 @@
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>4</v>
@@ -5000,9 +5014,9 @@
         <v>3</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="F85" s="16"/>
+        <v>512</v>
+      </c>
+      <c r="F85"/>
       <c r="G85" s="6" t="s">
         <v>111</v>
       </c>
@@ -5011,56 +5025,54 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>58</v>
+        <v>78</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E86" s="13" t="s">
-        <v>516</v>
-      </c>
-      <c r="F86" s="15"/>
-      <c r="G86" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="F86" s="16"/>
+      <c r="G86" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="H86" s="6"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <f t="shared" si="1"/>
-        <v>80</v>
-      </c>
-      <c r="B87" s="109" t="s">
-        <v>59</v>
+        <v>79</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="F87" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="G87" s="5" t="s">
-        <v>112</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
       <c r="H87" s="6"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <f t="shared" si="1"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B88" s="109" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>4</v>
@@ -5069,21 +5081,23 @@
         <v>3</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="F88" s="6"/>
-      <c r="G88" s="6" t="s">
-        <v>535</v>
+        <v>527</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="H88" s="6"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <f t="shared" si="1"/>
-        <v>82</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>61</v>
+        <v>81</v>
+      </c>
+      <c r="B89" s="109" t="s">
+        <v>60</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>4</v>
@@ -5092,19 +5106,21 @@
         <v>3</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>515</v>
-      </c>
+        <v>596</v>
+      </c>
+      <c r="F89" s="6"/>
       <c r="G89" s="6" t="s">
-        <v>535</v>
-      </c>
+        <v>531</v>
+      </c>
+      <c r="H89" s="6"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>4</v>
@@ -5113,66 +5129,63 @@
         <v>3</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="F90" s="6"/>
+        <v>511</v>
+      </c>
       <c r="G90" s="6" t="s">
-        <v>535</v>
-      </c>
-      <c r="H90" s="6"/>
+        <v>531</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <f t="shared" si="1"/>
-        <v>84</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>63</v>
+        <v>83</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>516</v>
-      </c>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6" t="s">
+        <v>531</v>
+      </c>
       <c r="H91" s="6"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <f t="shared" si="1"/>
-        <v>85</v>
-      </c>
-      <c r="B92" s="109" t="s">
-        <v>71</v>
+        <v>84</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>529</v>
-      </c>
-      <c r="F92" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="G92" s="5" t="s">
-        <v>112</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="6"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B93" s="109" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>4</v>
@@ -5181,10 +5194,10 @@
         <v>3</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>523</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>112</v>
@@ -5193,10 +5206,10 @@
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>65</v>
+        <v>86</v>
+      </c>
+      <c r="B94" s="109" t="s">
+        <v>64</v>
       </c>
       <c r="C94" s="7" t="s">
         <v>4</v>
@@ -5205,20 +5218,22 @@
         <v>3</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="F94" s="6"/>
-      <c r="G94" s="6" t="s">
-        <v>534</v>
+        <v>526</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="G94" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>4</v>
@@ -5227,20 +5242,20 @@
         <v>3</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C96" s="7" t="s">
         <v>4</v>
@@ -5248,18 +5263,21 @@
       <c r="D96" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E96" s="4"/>
+      <c r="E96" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="F96" s="6"/>
       <c r="G96" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C97" s="7" t="s">
         <v>4</v>
@@ -5267,21 +5285,18 @@
       <c r="D97" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E97" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="F97" s="6"/>
+      <c r="E97" s="4"/>
       <c r="G97" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <f t="shared" si="1"/>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>4</v>
@@ -5290,20 +5305,20 @@
         <v>3</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>4</v>
@@ -5312,66 +5327,63 @@
         <v>3</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F99" s="16"/>
+        <v>509</v>
+      </c>
+      <c r="F99" s="6"/>
       <c r="G99" s="6" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <f t="shared" si="1"/>
-        <v>93</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>72</v>
+        <v>92</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C100" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E100" s="13" t="s">
-        <v>516</v>
-      </c>
-      <c r="F100" s="15"/>
-      <c r="G100" s="15"/>
-      <c r="H100" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F100" s="16"/>
+      <c r="G100" s="6" t="s">
+        <v>530</v>
+      </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <f t="shared" si="1"/>
-        <v>94</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>73</v>
+        <v>93</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>520</v>
-      </c>
-      <c r="F101" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="G101" s="6" t="s">
-        <v>112</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="F101" s="15"/>
+      <c r="G101" s="15"/>
       <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>4</v>
@@ -5382,8 +5394,8 @@
       <c r="E102" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="F102" s="5" t="s">
-        <v>527</v>
+      <c r="F102" s="6" t="s">
+        <v>523</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>112</v>
@@ -5393,10 +5405,10 @@
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>4</v>
@@ -5405,21 +5417,23 @@
         <v>3</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="F103" s="6"/>
+        <v>512</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>523</v>
+      </c>
       <c r="G103" s="6" t="s">
-        <v>604</v>
+        <v>112</v>
       </c>
       <c r="H103" s="6"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <f t="shared" si="1"/>
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>4</v>
@@ -5428,21 +5442,21 @@
         <v>3</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="H104" s="6"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>4</v>
@@ -5450,22 +5464,22 @@
       <c r="D105" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E105" s="6" t="s">
-        <v>603</v>
+      <c r="E105" s="4" t="s">
+        <v>509</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="H105" s="6"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>4</v>
@@ -5473,22 +5487,22 @@
       <c r="D106" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E106" s="4" t="s">
-        <v>520</v>
+      <c r="E106" s="6" t="s">
+        <v>598</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="H106" s="6"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>4</v>
@@ -5497,21 +5511,21 @@
         <v>3</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="H107" s="6"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <f t="shared" si="1"/>
-        <v>101</v>
-      </c>
-      <c r="B108" s="109" t="s">
-        <v>80</v>
+        <v>100</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="C108" s="7" t="s">
         <v>4</v>
@@ -5520,23 +5534,21 @@
         <v>3</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="G108" s="5" t="s">
-        <v>112</v>
+        <v>516</v>
+      </c>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6" t="s">
+        <v>599</v>
       </c>
       <c r="H108" s="6"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <f t="shared" si="1"/>
-        <v>102</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>81</v>
+        <v>101</v>
+      </c>
+      <c r="B109" s="109" t="s">
+        <v>80</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>4</v>
@@ -5545,21 +5557,23 @@
         <v>3</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="F109" s="6"/>
-      <c r="G109" s="6" t="s">
-        <v>604</v>
+        <v>529</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="G109" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="H109" s="6"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>4</v>
@@ -5568,20 +5582,21 @@
         <v>3</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>513</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="F110" s="6"/>
       <c r="G110" s="6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="H110" s="6"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <f t="shared" si="1"/>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>4</v>
@@ -5589,22 +5604,21 @@
       <c r="D111" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E111" s="4"/>
-      <c r="F111" s="6" t="s">
-        <v>527</v>
+      <c r="E111" s="4" t="s">
+        <v>509</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>112</v>
+        <v>599</v>
       </c>
       <c r="H111" s="6"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>4</v>
@@ -5613,19 +5627,21 @@
         <v>3</v>
       </c>
       <c r="E112" s="4"/>
-      <c r="F112" s="6"/>
+      <c r="F112" s="6" t="s">
+        <v>523</v>
+      </c>
       <c r="G112" s="6" t="s">
-        <v>604</v>
+        <v>112</v>
       </c>
       <c r="H112" s="6"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <f t="shared" si="1"/>
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C113" s="7" t="s">
         <v>4</v>
@@ -5633,22 +5649,20 @@
       <c r="D113" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E113" s="4" t="s">
-        <v>515</v>
-      </c>
+      <c r="E113" s="4"/>
       <c r="F113" s="6"/>
       <c r="G113" s="6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="H113" s="6"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C114" s="7" t="s">
         <v>4</v>
@@ -5657,65 +5671,63 @@
         <v>3</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>513</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="F114" s="6"/>
       <c r="G114" s="6" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="H114" s="6"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <f t="shared" si="1"/>
-        <v>108</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>87</v>
+        <v>107</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C115" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E115" s="13" t="s">
-        <v>516</v>
-      </c>
-      <c r="F115" s="14"/>
-      <c r="G115" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="G115" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="H115" s="6"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <f t="shared" si="1"/>
-        <v>109</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>88</v>
+        <v>108</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="C116" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E116" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G116" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H116" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="E116" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C117" s="7" t="s">
         <v>4</v>
@@ -5724,10 +5736,10 @@
         <v>3</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>112</v>
@@ -5737,10 +5749,10 @@
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C118" s="7" t="s">
         <v>4</v>
@@ -5751,19 +5763,21 @@
       <c r="E118" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F118" s="6"/>
+      <c r="F118" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="G118" s="5" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="H118" s="6"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C119" s="7" t="s">
         <v>4</v>
@@ -5772,23 +5786,21 @@
         <v>3</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>144</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="F119" s="6"/>
       <c r="G119" s="5" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="H119" s="6"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <f t="shared" si="1"/>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C120" s="7" t="s">
         <v>4</v>
@@ -5797,21 +5809,23 @@
         <v>3</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="F120" s="6"/>
+        <v>510</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="G120" s="5" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="H120" s="6"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C121" s="7" t="s">
         <v>4</v>
@@ -5820,19 +5834,21 @@
         <v>3</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>514</v>
-      </c>
+        <v>510</v>
+      </c>
+      <c r="F121" s="6"/>
       <c r="G121" s="5" t="s">
         <v>148</v>
       </c>
+      <c r="H121" s="6"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C122" s="7" t="s">
         <v>4</v>
@@ -5841,9 +5857,8 @@
         <v>3</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="F122" s="2"/>
+        <v>510</v>
+      </c>
       <c r="G122" s="5" t="s">
         <v>148</v>
       </c>
@@ -5851,10 +5866,10 @@
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C123" s="7" t="s">
         <v>4</v>
@@ -5863,23 +5878,20 @@
         <v>3</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F123" s="6" t="s">
-        <v>147</v>
-      </c>
+        <v>510</v>
+      </c>
+      <c r="F123" s="2"/>
       <c r="G123" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H123" s="6"/>
+        <v>148</v>
+      </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C124" s="7" t="s">
         <v>4</v>
@@ -5888,22 +5900,23 @@
         <v>3</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>602</v>
+        <v>116</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G124" s="5" t="s">
         <v>112</v>
       </c>
+      <c r="H124" s="6"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C125" s="7" t="s">
         <v>4</v>
@@ -5912,19 +5925,22 @@
         <v>3</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>515</v>
+        <v>597</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C126" s="7" t="s">
         <v>4</v>
@@ -5933,7 +5949,7 @@
         <v>3</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G126" s="5" t="s">
         <v>148</v>
@@ -5942,10 +5958,10 @@
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>482</v>
+        <v>98</v>
       </c>
       <c r="C127" s="7" t="s">
         <v>4</v>
@@ -5954,116 +5970,163 @@
         <v>3</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F127" s="6" t="s">
-        <v>145</v>
+        <v>509</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F128" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="G129" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <f>A128+1</f>
         <v>121</v>
       </c>
-      <c r="B128" s="7" t="s">
+      <c r="B130" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C128" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D128" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E128" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="F128" s="10"/>
-      <c r="G128" s="5" t="s">
+      <c r="C130" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D130" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="F130" s="10"/>
+      <c r="G130" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="H128" s="12"/>
-    </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C129" s="11"/>
-      <c r="D129" s="11"/>
-    </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="18"/>
-    </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="18"/>
+      <c r="H130" s="12"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C131" s="11"/>
+      <c r="D131" s="11"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:G1 E122 G3:G5 E3:E5 F6:G6 H1:H18 E19 G19 E123:G1048576 G122 H27:H1048576 E21:E26 G21:G26 E27:G55 E7:G11 E13:G18 G12 E20:F20 E67:G101 G102 E102 E103:G121">
-    <cfRule type="expression" dxfId="0" priority="20">
+  <conditionalFormatting sqref="E1:G1 E123 G3:G5 E3:E5 F6:G6 H1:H18 E19 G19 G123 H27:H1048576 E21:E26 G21:G26 E7:G11 E13:G18 G12 E20:F20 E68:G102 G103 E103 E104:G122 E27:G55 E133:G1048576 F132:G132 E124:G131">
+    <cfRule type="expression" dxfId="14" priority="23">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G2">
-    <cfRule type="expression" dxfId="13" priority="17">
+    <cfRule type="expression" dxfId="13" priority="20">
       <formula>"$C2 = 'Header'"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:G2 I57 E57:G59 E61:G61 E60:F60 E63:G66 E62:F62">
-    <cfRule type="expression" dxfId="12" priority="16">
+  <conditionalFormatting sqref="E2:G2 I57 E57:G59 E60:F60 E64:G67 E63:F63 E61:G62">
+    <cfRule type="expression" dxfId="12" priority="19">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61:F61">
-    <cfRule type="expression" dxfId="11" priority="15">
+  <conditionalFormatting sqref="E61:F62">
+    <cfRule type="expression" dxfId="11" priority="18">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="10" priority="14">
+    <cfRule type="expression" dxfId="10" priority="17">
       <formula>"$C2 = 'Header'"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56">
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G61">
-    <cfRule type="expression" dxfId="8" priority="10">
+  <conditionalFormatting sqref="G61:G62">
+    <cfRule type="expression" dxfId="8" priority="13">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G60">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G62">
-    <cfRule type="expression" dxfId="2" priority="2">
+  <conditionalFormatting sqref="G63">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G56">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>"$C2 = ""Header"""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G132">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>"$C2 = ""Header"""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6077,7 +6140,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6091,7 +6154,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>368</v>
@@ -6109,10 +6172,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>117</v>
@@ -6127,7 +6190,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="97"/>
       <c r="B3" s="43" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>341</v>
@@ -6142,7 +6205,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="97"/>
       <c r="B4" s="43" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>367</v>
@@ -6157,7 +6220,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="97"/>
       <c r="B5" s="43" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>342</v>
@@ -6193,32 +6256,32 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="50" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -6252,7 +6315,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>357</v>
@@ -6278,7 +6341,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>350</v>
@@ -6392,12 +6455,12 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -6651,96 +6714,96 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="110" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="C1" s="111" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="97"/>
       <c r="B3" s="48" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="C3" s="112" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="97"/>
       <c r="D4" s="37" t="s">
+        <v>578</v>
+      </c>
+      <c r="E4" s="62" t="s">
         <v>583</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="97"/>
       <c r="D5" s="37" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="97"/>
       <c r="D6" s="37" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="97"/>
       <c r="D7" s="37" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="97"/>
       <c r="D8" s="39" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="E8" s="63" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6773,17 +6836,17 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
@@ -6792,7 +6855,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
@@ -6923,8 +6986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF94A00-A6D2-49B1-9C65-88878417CF76}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6938,7 +7001,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B1" s="72" t="s">
         <v>385</v>
@@ -6949,7 +7012,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="93" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>384</v>
@@ -7092,7 +7155,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="37" t="s">
-        <v>404</v>
+        <v>600</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>325</v>
@@ -7102,7 +7165,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="37" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C17" s="62" t="s">
         <v>324</v>
@@ -7111,7 +7174,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="37" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C18" s="62" t="s">
         <v>339</v>
@@ -7121,7 +7184,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="37" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C19" s="62" t="s">
         <v>338</v>
@@ -7131,7 +7194,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="37" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C20" s="62" t="s">
         <v>329</v>
@@ -7141,7 +7204,7 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="37" t="s">
-        <v>409</v>
+        <v>600</v>
       </c>
       <c r="C21" s="62" t="s">
         <v>331</v>
@@ -7151,7 +7214,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="37" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C22" s="62" t="s">
         <v>330</v>
@@ -7161,7 +7224,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="37" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C23" s="62" t="s">
         <v>326</v>
@@ -7171,7 +7234,7 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="37" t="s">
-        <v>412</v>
+        <v>600</v>
       </c>
       <c r="C24" s="62" t="s">
         <v>328</v>
@@ -7181,7 +7244,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="37" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C25" s="62" t="s">
         <v>327</v>
@@ -7191,7 +7254,7 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="37" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C26" s="62" t="s">
         <v>332</v>
@@ -7201,7 +7264,7 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="37" t="s">
-        <v>415</v>
+        <v>600</v>
       </c>
       <c r="C27" s="62" t="s">
         <v>337</v>
@@ -7211,7 +7274,7 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="94"/>
       <c r="B28" s="37" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C28" s="62" t="s">
         <v>334</v>
@@ -7221,7 +7284,7 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="37" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C29" s="62" t="s">
         <v>333</v>
@@ -7231,7 +7294,7 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="94"/>
       <c r="B30" s="37" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C30" s="62" t="s">
         <v>335</v>
@@ -7241,7 +7304,7 @@
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="94"/>
       <c r="B31" s="39" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C31" s="63" t="s">
         <v>336</v>
@@ -7300,7 +7363,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>179</v>
@@ -7315,7 +7378,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="93" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>176</v>
@@ -7458,22 +7521,22 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7506,7 +7569,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="85" t="s">
         <v>203</v>
@@ -7523,7 +7586,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="94" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>200</v>
@@ -7775,22 +7838,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -7819,7 +7882,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>233</v>
@@ -7830,7 +7893,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>202</v>
@@ -7868,12 +7931,12 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7907,7 +7970,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="71" t="s">
         <v>235</v>
@@ -7919,7 +7982,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B2" s="69" t="s">
         <v>258</v>
@@ -8034,22 +8097,22 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B18" s="70"/>
     </row>
@@ -8081,7 +8144,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>279</v>
@@ -8111,7 +8174,7 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="99" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>282</v>
@@ -8321,7 +8384,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -8408,7 +8471,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>302</v>
@@ -8428,7 +8491,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>306</v>
@@ -8516,17 +8579,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -8556,66 +8619,66 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E1" s="76" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>389</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="97"/>
       <c r="B3" s="43" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="97"/>
       <c r="B4" s="43" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -8624,7 +8687,7 @@
         <v>391</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="62"/>
@@ -8635,29 +8698,29 @@
         <v>390</v>
       </c>
       <c r="C6" s="64" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="63"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ISA2MCDS script works for StateTransitions, TransportProcesses, Microenvironment, ClinicalStain, CellDeath, and CellCycle assays
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AADD40-C1D6-44DD-A38D-5A5F59992E08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EB430B-E427-4DF5-9A6F-91C82886B968}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="613">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -1263,6 +1263,9 @@
     <t>Parameter Value[Patient Age at Diagnosis]</t>
   </si>
   <si>
+    <t>Patient Age at Diagnosis - Units</t>
+  </si>
+  <si>
     <t>Characteristic[Patient Age at Diagnosis Measurement Type]</t>
   </si>
   <si>
@@ -1275,18 +1278,27 @@
     <t>Parameter Value[Overall Survival]</t>
   </si>
   <si>
+    <t>Overall Survival - Units</t>
+  </si>
+  <si>
     <t>Characteristic[Overall Survival - Measurement Type]</t>
   </si>
   <si>
     <t>Characteristic[D/Rho - Measurement Type]</t>
   </si>
   <si>
+    <t>D/Rho - Units</t>
+  </si>
+  <si>
     <t>Parameter Value[D/Rho]</t>
   </si>
   <si>
     <t>Parameter Value[Rho/D]</t>
   </si>
   <si>
+    <t>Rho/D - Units</t>
+  </si>
+  <si>
     <t>Characteristic[Rho/D - Measurement Type]</t>
   </si>
   <si>
@@ -1851,9 +1863,6 @@
     <t>Multiple - Study Protocol Name</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>Mult-join</t>
   </si>
   <si>
@@ -1873,6 +1882,12 @@
   </si>
   <si>
     <t>cell_line/metadata/curation/current_contact/orcid-identifier/path, cell_line/metadata/curation/curator/orcid-identifier/path, cell_line/metadata/curation/creator/orcid-identifier/path,  cell_line/metadata/curation/last_modified_by/orcid-identifier/path</t>
+  </si>
+  <si>
+    <t>domain/experimental_condition/conditions</t>
+  </si>
+  <si>
+    <t>Characteristic[Experiment Condition]</t>
   </si>
 </sst>
 </file>
@@ -2986,7 +3001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FA11B-2D6D-4A50-A5F1-7D079DCC0D36}">
   <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
@@ -3060,7 +3075,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>110</v>
@@ -3084,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>110</v>
@@ -3108,7 +3123,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>110</v>
@@ -3132,7 +3147,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>110</v>
@@ -3327,7 +3342,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -3352,7 +3367,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -3364,7 +3379,7 @@
         <v>120</v>
       </c>
       <c r="F16" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>111</v>
@@ -3427,7 +3442,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -3436,10 +3451,10 @@
         <v>3</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>111</v>
@@ -3452,7 +3467,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="104" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -3461,10 +3476,10 @@
         <v>3</v>
       </c>
       <c r="E20" s="104" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="F20" s="103" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>111</v>
@@ -3477,7 +3492,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="91" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -3486,10 +3501,10 @@
         <v>3</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>111</v>
@@ -3502,7 +3517,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="91" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -3511,10 +3526,10 @@
         <v>3</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>111</v>
@@ -3527,7 +3542,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="91" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -3536,10 +3551,10 @@
         <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>111</v>
@@ -3552,7 +3567,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="91" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -3561,10 +3576,10 @@
         <v>3</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>111</v>
@@ -3577,7 +3592,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="91" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -3586,10 +3601,10 @@
         <v>3</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>111</v>
@@ -3602,7 +3617,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -3611,10 +3626,10 @@
         <v>3</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>111</v>
@@ -3636,7 +3651,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -3703,10 +3718,10 @@
         <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>111</v>
@@ -3728,10 +3743,10 @@
         <v>3</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>111</v>
@@ -3753,10 +3768,10 @@
         <v>3</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>111</v>
@@ -3778,7 +3793,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
@@ -3801,7 +3816,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6" t="s">
@@ -3815,7 +3830,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>554</v>
+        <v>558</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -3827,7 +3842,7 @@
         <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>544</v>
+        <v>548</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>112</v>
@@ -3840,7 +3855,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="91" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -3852,7 +3867,7 @@
         <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>112</v>
@@ -3865,7 +3880,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="91" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -3874,10 +3889,10 @@
         <v>3</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="F37" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>112</v>
@@ -3890,7 +3905,7 @@
         <v>31</v>
       </c>
       <c r="B38" s="91" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -3902,7 +3917,7 @@
         <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>112</v>
@@ -3915,7 +3930,7 @@
         <v>32</v>
       </c>
       <c r="B39" s="91" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -3927,10 +3942,10 @@
         <v>109</v>
       </c>
       <c r="F39" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -3940,7 +3955,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="91" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -3949,10 +3964,10 @@
         <v>3</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="F40" t="s">
-        <v>549</v>
+        <v>553</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>112</v>
@@ -3965,7 +3980,7 @@
         <v>34</v>
       </c>
       <c r="B41" s="91" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -3974,10 +3989,10 @@
         <v>3</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>553</v>
+        <v>557</v>
       </c>
       <c r="F41" t="s">
-        <v>550</v>
+        <v>554</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>112</v>
@@ -3990,7 +4005,7 @@
         <v>35</v>
       </c>
       <c r="B42" s="91" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>4</v>
@@ -4002,7 +4017,7 @@
         <v>105</v>
       </c>
       <c r="F42" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>112</v>
@@ -4015,7 +4030,7 @@
         <v>36</v>
       </c>
       <c r="B43" s="91" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -4024,10 +4039,10 @@
         <v>3</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="F43" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>112</v>
@@ -4040,7 +4055,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="91" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -4052,7 +4067,7 @@
         <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>112</v>
@@ -4065,7 +4080,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="91" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -4077,7 +4092,7 @@
         <v>121</v>
       </c>
       <c r="F45" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>112</v>
@@ -4090,7 +4105,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="91" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -4102,10 +4117,10 @@
         <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="H46" s="2"/>
     </row>
@@ -4115,7 +4130,7 @@
         <v>40</v>
       </c>
       <c r="B47" s="91" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>4</v>
@@ -4127,7 +4142,7 @@
         <v>118</v>
       </c>
       <c r="F47" t="s">
-        <v>542</v>
+        <v>546</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>112</v>
@@ -4140,7 +4155,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="91" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>4</v>
@@ -4152,7 +4167,7 @@
         <v>109</v>
       </c>
       <c r="F48" t="s">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>112</v>
@@ -4174,7 +4189,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
@@ -4245,7 +4260,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6" t="s">
@@ -4293,7 +4308,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6" t="s">
@@ -4316,7 +4331,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6" t="s">
@@ -4339,7 +4354,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>111</v>
@@ -4365,7 +4380,7 @@
         <v>116</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>111</v>
@@ -4413,7 +4428,7 @@
         <v>3</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6" t="s">
@@ -4436,7 +4451,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6" t="s">
@@ -4450,7 +4465,7 @@
         <v>54</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>4</v>
@@ -4471,7 +4486,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>4</v>
@@ -4480,10 +4495,10 @@
         <v>3</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>111</v>
@@ -4505,7 +4520,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="6" t="s">
@@ -4549,7 +4564,7 @@
         <v>3</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>128</v>
@@ -4574,7 +4589,7 @@
         <v>3</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>129</v>
@@ -4599,7 +4614,7 @@
         <v>3</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>131</v>
@@ -4624,7 +4639,7 @@
         <v>3</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6" t="s">
@@ -4668,10 +4683,10 @@
         <v>3</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G70" s="6" t="s">
         <v>111</v>
@@ -4735,7 +4750,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
@@ -4756,13 +4771,13 @@
         <v>3</v>
       </c>
       <c r="E74" s="105" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="F74" s="107" t="s">
         <v>110</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="H74" s="6"/>
     </row>
@@ -4781,7 +4796,7 @@
         <v>3</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="F75" s="6"/>
       <c r="G75" s="6" t="s">
@@ -4804,7 +4819,7 @@
         <v>3</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="6" t="s">
@@ -4827,7 +4842,7 @@
         <v>2</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
@@ -4848,7 +4863,7 @@
         <v>3</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6" t="s">
@@ -4871,7 +4886,7 @@
         <v>3</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="6" t="s">
@@ -4894,10 +4909,10 @@
         <v>3</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>111</v>
@@ -4918,10 +4933,10 @@
         <v>3</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>111</v>
@@ -4943,10 +4958,10 @@
         <v>3</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G82" s="6" t="s">
         <v>111</v>
@@ -4968,7 +4983,7 @@
         <v>3</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="6" t="s">
@@ -4991,7 +5006,7 @@
         <v>3</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="6" t="s">
@@ -5014,7 +5029,7 @@
         <v>3</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F85"/>
       <c r="G85" s="6" t="s">
@@ -5037,7 +5052,7 @@
         <v>3</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="F86" s="16"/>
       <c r="G86" s="6" t="s">
@@ -5060,7 +5075,7 @@
         <v>2</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F87" s="15"/>
       <c r="G87" s="15"/>
@@ -5081,10 +5096,10 @@
         <v>3</v>
       </c>
       <c r="E88" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="F88" s="6" t="s">
         <v>527</v>
-      </c>
-      <c r="F88" s="6" t="s">
-        <v>523</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>112</v>
@@ -5106,11 +5121,11 @@
         <v>3</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="H89" s="6"/>
     </row>
@@ -5129,10 +5144,10 @@
         <v>3</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -5150,11 +5165,11 @@
         <v>3</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="H91" s="6"/>
     </row>
@@ -5173,7 +5188,7 @@
         <v>2</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F92" s="14"/>
       <c r="G92" s="14"/>
@@ -5194,10 +5209,10 @@
         <v>3</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>112</v>
@@ -5218,10 +5233,10 @@
         <v>3</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>112</v>
@@ -5242,11 +5257,11 @@
         <v>3</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="6" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -5264,11 +5279,11 @@
         <v>3</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="6" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -5287,7 +5302,7 @@
       </c>
       <c r="E97" s="4"/>
       <c r="G97" s="6" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -5305,11 +5320,11 @@
         <v>3</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="6" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -5327,11 +5342,11 @@
         <v>3</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="F99" s="6"/>
       <c r="G99" s="6" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -5353,7 +5368,7 @@
       </c>
       <c r="F100" s="16"/>
       <c r="G100" s="6" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -5371,7 +5386,7 @@
         <v>2</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F101" s="15"/>
       <c r="G101" s="15"/>
@@ -5392,10 +5407,10 @@
         <v>3</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>112</v>
@@ -5417,10 +5432,10 @@
         <v>3</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>112</v>
@@ -5442,11 +5457,11 @@
         <v>3</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H104" s="6"/>
     </row>
@@ -5465,11 +5480,11 @@
         <v>3</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H105" s="6"/>
     </row>
@@ -5488,11 +5503,11 @@
         <v>3</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H106" s="6"/>
     </row>
@@ -5511,11 +5526,11 @@
         <v>3</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H107" s="6"/>
     </row>
@@ -5534,11 +5549,11 @@
         <v>3</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H108" s="6"/>
     </row>
@@ -5557,10 +5572,10 @@
         <v>3</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>112</v>
@@ -5582,11 +5597,11 @@
         <v>3</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H110" s="6"/>
     </row>
@@ -5605,10 +5620,10 @@
         <v>3</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H111" s="6"/>
     </row>
@@ -5628,7 +5643,7 @@
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="6" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="G112" s="6" t="s">
         <v>112</v>
@@ -5652,7 +5667,7 @@
       <c r="E113" s="4"/>
       <c r="F113" s="6"/>
       <c r="G113" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H113" s="6"/>
     </row>
@@ -5671,11 +5686,11 @@
         <v>3</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H114" s="6"/>
     </row>
@@ -5694,10 +5709,10 @@
         <v>3</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="H115" s="6"/>
     </row>
@@ -5716,7 +5731,7 @@
         <v>2</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -5809,7 +5824,7 @@
         <v>3</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F120" s="6" t="s">
         <v>144</v>
@@ -5834,7 +5849,7 @@
         <v>3</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F121" s="6"/>
       <c r="G121" s="5" t="s">
@@ -5857,7 +5872,7 @@
         <v>3</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="G122" s="5" t="s">
         <v>148</v>
@@ -5878,7 +5893,7 @@
         <v>3</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="5" t="s">
@@ -5925,7 +5940,7 @@
         <v>3</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>146</v>
@@ -5949,7 +5964,7 @@
         <v>3</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="G126" s="5" t="s">
         <v>148</v>
@@ -5970,7 +5985,7 @@
         <v>3</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="G127" s="5" t="s">
         <v>148</v>
@@ -5982,7 +5997,7 @@
         <v>120</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>4</v>
@@ -6002,7 +6017,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" s="4" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>4</v>
@@ -6011,10 +6026,10 @@
         <v>3</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="G129" s="5" t="s">
         <v>112</v>
@@ -6035,7 +6050,7 @@
         <v>3</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F130" s="10"/>
       <c r="G130" s="5" t="s">
@@ -6154,7 +6169,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>368</v>
@@ -6172,10 +6187,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>117</v>
@@ -6190,7 +6205,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="97"/>
       <c r="B3" s="43" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>341</v>
@@ -6205,7 +6220,7 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="97"/>
       <c r="B4" s="43" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>367</v>
@@ -6220,7 +6235,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="97"/>
       <c r="B5" s="43" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>342</v>
@@ -6256,32 +6271,32 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="50" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
   </sheetData>
@@ -6298,7 +6313,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6315,7 +6330,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>357</v>
@@ -6341,7 +6356,7 @@
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>350</v>
@@ -6455,12 +6470,12 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -6714,96 +6729,96 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="110" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="C1" s="111" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="E1" s="73" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="97"/>
       <c r="B3" s="48" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="C3" s="112" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="E3" s="62" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="97"/>
       <c r="D4" s="37" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="97"/>
       <c r="D5" s="37" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="97"/>
       <c r="D6" s="37" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="E6" s="62" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="97"/>
       <c r="D7" s="37" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="E7" s="62" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="97"/>
       <c r="D8" s="39" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="E8" s="63" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6836,17 +6851,17 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
@@ -6855,7 +6870,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
@@ -6986,8 +7001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF94A00-A6D2-49B1-9C65-88878417CF76}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7001,7 +7016,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="B1" s="72" t="s">
         <v>385</v>
@@ -7012,7 +7027,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="93" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>384</v>
@@ -7155,7 +7170,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="94"/>
       <c r="B16" s="37" t="s">
-        <v>600</v>
+        <v>404</v>
       </c>
       <c r="C16" s="62" t="s">
         <v>325</v>
@@ -7165,7 +7180,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="94"/>
       <c r="B17" s="37" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C17" s="62" t="s">
         <v>324</v>
@@ -7174,7 +7189,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="94"/>
       <c r="B18" s="37" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C18" s="62" t="s">
         <v>339</v>
@@ -7184,7 +7199,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="94"/>
       <c r="B19" s="37" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C19" s="62" t="s">
         <v>338</v>
@@ -7194,7 +7209,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="37" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C20" s="62" t="s">
         <v>329</v>
@@ -7204,7 +7219,7 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="94"/>
       <c r="B21" s="37" t="s">
-        <v>600</v>
+        <v>409</v>
       </c>
       <c r="C21" s="62" t="s">
         <v>331</v>
@@ -7214,7 +7229,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="94"/>
       <c r="B22" s="37" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C22" s="62" t="s">
         <v>330</v>
@@ -7224,7 +7239,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="94"/>
       <c r="B23" s="37" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="C23" s="62" t="s">
         <v>326</v>
@@ -7234,7 +7249,7 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="94"/>
       <c r="B24" s="37" t="s">
-        <v>600</v>
+        <v>412</v>
       </c>
       <c r="C24" s="62" t="s">
         <v>328</v>
@@ -7244,7 +7259,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="94"/>
       <c r="B25" s="37" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C25" s="62" t="s">
         <v>327</v>
@@ -7254,7 +7269,7 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="94"/>
       <c r="B26" s="37" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C26" s="62" t="s">
         <v>332</v>
@@ -7264,7 +7279,7 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="94"/>
       <c r="B27" s="37" t="s">
-        <v>600</v>
+        <v>415</v>
       </c>
       <c r="C27" s="62" t="s">
         <v>337</v>
@@ -7274,7 +7289,7 @@
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="94"/>
       <c r="B28" s="37" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="C28" s="62" t="s">
         <v>334</v>
@@ -7284,7 +7299,7 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="94"/>
       <c r="B29" s="37" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C29" s="62" t="s">
         <v>333</v>
@@ -7294,7 +7309,7 @@
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="94"/>
       <c r="B30" s="37" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="C30" s="62" t="s">
         <v>335</v>
@@ -7304,7 +7319,7 @@
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="94"/>
       <c r="B31" s="39" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C31" s="63" t="s">
         <v>336</v>
@@ -7349,7 +7364,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7363,7 +7378,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>179</v>
@@ -7378,7 +7393,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="93" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>176</v>
@@ -7420,10 +7435,10 @@
         <v>167</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>166</v>
+        <v>611</v>
       </c>
       <c r="D5" s="90" t="s">
-        <v>165</v>
+        <v>612</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7432,10 +7447,10 @@
         <v>164</v>
       </c>
       <c r="C6" s="89" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D6" s="90" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -7444,10 +7459,10 @@
         <v>161</v>
       </c>
       <c r="C7" s="89" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D7" s="90" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -7456,10 +7471,10 @@
         <v>158</v>
       </c>
       <c r="C8" s="89" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D8" s="90" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -7467,8 +7482,12 @@
       <c r="B9" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="89" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="90" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="94"/>
@@ -7516,27 +7535,29 @@
       <c r="B15" s="88" t="s">
         <v>149</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="40"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="83"/>
+      <c r="D15" s="38"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
-        <v>434</v>
-      </c>
+        <v>438</v>
+      </c>
+      <c r="C16" s="84"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7553,8 +7574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACDCEEC-2455-41F7-B48E-7900618A1490}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7569,7 +7590,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="85" t="s">
         <v>203</v>
@@ -7586,7 +7607,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="94" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="B2" s="86" t="s">
         <v>200</v>
@@ -7838,22 +7859,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -7870,7 +7891,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7882,7 +7903,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>233</v>
@@ -7893,7 +7914,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>202</v>
@@ -7931,12 +7952,12 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7970,7 +7991,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="71" t="s">
         <v>235</v>
@@ -7982,7 +8003,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B2" s="69" t="s">
         <v>258</v>
@@ -8097,22 +8118,22 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B18" s="70"/>
     </row>
@@ -8144,7 +8165,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>279</v>
@@ -8174,7 +8195,7 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="99" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>282</v>
@@ -8384,7 +8405,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -8471,7 +8492,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>302</v>
@@ -8491,7 +8512,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>306</v>
@@ -8579,17 +8600,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -8604,8 +8625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A97BD1D-99EF-49BC-B0C5-86FC67BB4019}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8619,66 +8640,66 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="E1" s="76" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B2" s="43" t="s">
         <v>389</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="97"/>
       <c r="B3" s="43" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="D3" s="37" t="s">
+        <v>434</v>
+      </c>
+      <c r="E3" s="62" t="s">
         <v>430</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="97"/>
       <c r="B4" s="43" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="E4" s="62" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -8687,7 +8708,7 @@
         <v>391</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="62"/>
@@ -8698,29 +8719,29 @@
         <v>390</v>
       </c>
       <c r="C6" s="64" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="63"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ISA2MCDS DCL conversion script v0.1 is finished
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EB430B-E427-4DF5-9A6F-91C82886B968}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D80A532-3593-4D47-AFCB-C3858420366F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
@@ -6155,7 +6155,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7978,8 +7978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098C817-F491-46B8-ACCD-892895410AE2}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8149,8 +8149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9108F335-02AF-4487-9ECF-FF27706B5F2B}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8476,8 +8476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D15C30-4CE2-4FE6-8ED7-DB2C8418632F}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8586,27 +8586,27 @@
       <c r="A6" s="97"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="98"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>461</v>
       </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
         <v>462</v>
       </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
@@ -8625,8 +8625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A97BD1D-99EF-49BC-B0C5-86FC67BB4019}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed tab and newline formatting issues in xml writing, updated comparison to skip 'update text "nan" '
</commit_message>
<xml_diff>
--- a/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
+++ b/Burns_Thesis_DatabaseConversion/ISA_MCDS_Relationships_Py_CB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\PycharmProjects\MCDS_2_ISATab\Burns_Thesis_DatabaseConversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D80A532-3593-4D47-AFCB-C3858420366F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F11B87-F133-41E2-83CB-CA3415A56ADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
+    <workbookView xWindow="-28920" yWindow="-3765" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2CD61F54-19AE-432F-B1AD-B38F5E2014D6}"/>
   </bookViews>
   <sheets>
     <sheet name="MCDS-DCL to ISA-Tab" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="614">
   <si>
     <t>ISA-Tab Entity</t>
   </si>
@@ -564,9 +564,6 @@
     <t>/material_amount[@measurement_type]</t>
   </si>
   <si>
-    <t>Temperature Units</t>
-  </si>
-  <si>
     <t>domain/variables/physical_parameter_set/conditions/temperature[@units]</t>
   </si>
   <si>
@@ -1888,6 +1885,12 @@
   </si>
   <si>
     <t>Characteristic[Experiment Condition]</t>
+  </si>
+  <si>
+    <t>Temperature units</t>
+  </si>
+  <si>
+    <t>Note: leave units as lower case, else it won't be found by MicroenvironmentAssay function in ISA2DCL.py</t>
   </si>
 </sst>
 </file>
@@ -2535,6 +2538,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2565,20 +2582,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3001,8 +3004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C89FA11B-2D6D-4A50-A5F1-7D079DCC0D36}">
   <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView topLeftCell="B91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F129" sqref="F129"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3075,7 +3078,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>110</v>
@@ -3099,7 +3102,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>110</v>
@@ -3123,7 +3126,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>110</v>
@@ -3147,7 +3150,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>110</v>
@@ -3274,13 +3277,13 @@
       <c r="A12" s="2">
         <v>5</v>
       </c>
-      <c r="B12" s="104" t="s">
+      <c r="B12" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="104" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="104" t="s">
+      <c r="C12" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="94" t="s">
         <v>3</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -3342,7 +3345,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -3367,7 +3370,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -3379,7 +3382,7 @@
         <v>120</v>
       </c>
       <c r="F16" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>111</v>
@@ -3442,19 +3445,19 @@
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>494</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>493</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>111</v>
@@ -3466,8 +3469,8 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B20" s="104" t="s">
-        <v>571</v>
+      <c r="B20" s="94" t="s">
+        <v>570</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -3475,11 +3478,11 @@
       <c r="D20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="104" t="s">
-        <v>496</v>
-      </c>
-      <c r="F20" s="103" t="s">
-        <v>499</v>
+      <c r="E20" s="94" t="s">
+        <v>495</v>
+      </c>
+      <c r="F20" s="93" t="s">
+        <v>498</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>111</v>
@@ -3492,7 +3495,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="91" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -3501,10 +3504,10 @@
         <v>3</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>498</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>111</v>
@@ -3517,7 +3520,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="91" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -3526,10 +3529,10 @@
         <v>3</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>111</v>
@@ -3542,7 +3545,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="91" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -3551,10 +3554,10 @@
         <v>3</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>111</v>
@@ -3567,7 +3570,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="91" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -3576,10 +3579,10 @@
         <v>3</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>111</v>
@@ -3592,7 +3595,7 @@
         <v>18</v>
       </c>
       <c r="B25" s="91" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -3601,10 +3604,10 @@
         <v>3</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>111</v>
@@ -3617,7 +3620,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="91" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -3626,10 +3629,10 @@
         <v>3</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>111</v>
@@ -3651,7 +3654,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
@@ -3708,7 +3711,7 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B30" s="104" t="s">
+      <c r="B30" s="94" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -3718,10 +3721,10 @@
         <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>111</v>
@@ -3733,7 +3736,7 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B31" s="104" t="s">
+      <c r="B31" s="94" t="s">
         <v>20</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -3743,10 +3746,10 @@
         <v>3</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>111</v>
@@ -3758,7 +3761,7 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B32" s="104" t="s">
+      <c r="B32" s="94" t="s">
         <v>21</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -3768,10 +3771,10 @@
         <v>3</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>111</v>
@@ -3793,7 +3796,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
@@ -3816,7 +3819,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6" t="s">
@@ -3830,7 +3833,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="91" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -3842,7 +3845,7 @@
         <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G35" s="5" t="s">
         <v>112</v>
@@ -3855,7 +3858,7 @@
         <v>29</v>
       </c>
       <c r="B36" s="91" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -3867,7 +3870,7 @@
         <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>112</v>
@@ -3880,7 +3883,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="91" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -3889,10 +3892,10 @@
         <v>3</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F37" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="G37" s="5" t="s">
         <v>112</v>
@@ -3905,7 +3908,7 @@
         <v>31</v>
       </c>
       <c r="B38" s="91" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -3917,7 +3920,7 @@
         <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>112</v>
@@ -3930,7 +3933,7 @@
         <v>32</v>
       </c>
       <c r="B39" s="91" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -3942,10 +3945,10 @@
         <v>109</v>
       </c>
       <c r="F39" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -3955,7 +3958,7 @@
         <v>33</v>
       </c>
       <c r="B40" s="91" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -3964,10 +3967,10 @@
         <v>3</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F40" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>112</v>
@@ -3980,7 +3983,7 @@
         <v>34</v>
       </c>
       <c r="B41" s="91" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -3989,10 +3992,10 @@
         <v>3</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F41" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>112</v>
@@ -4005,7 +4008,7 @@
         <v>35</v>
       </c>
       <c r="B42" s="91" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>4</v>
@@ -4017,7 +4020,7 @@
         <v>105</v>
       </c>
       <c r="F42" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>112</v>
@@ -4030,7 +4033,7 @@
         <v>36</v>
       </c>
       <c r="B43" s="91" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -4039,10 +4042,10 @@
         <v>3</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F43" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>112</v>
@@ -4055,7 +4058,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="91" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -4067,7 +4070,7 @@
         <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>112</v>
@@ -4080,7 +4083,7 @@
         <v>38</v>
       </c>
       <c r="B45" s="91" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -4092,7 +4095,7 @@
         <v>121</v>
       </c>
       <c r="F45" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>112</v>
@@ -4105,7 +4108,7 @@
         <v>39</v>
       </c>
       <c r="B46" s="91" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -4117,10 +4120,10 @@
         <v>109</v>
       </c>
       <c r="F46" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H46" s="2"/>
     </row>
@@ -4130,7 +4133,7 @@
         <v>40</v>
       </c>
       <c r="B47" s="91" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>4</v>
@@ -4142,7 +4145,7 @@
         <v>118</v>
       </c>
       <c r="F47" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>112</v>
@@ -4155,7 +4158,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="91" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>4</v>
@@ -4167,7 +4170,7 @@
         <v>109</v>
       </c>
       <c r="F48" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>112</v>
@@ -4189,7 +4192,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
@@ -4260,7 +4263,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6" t="s">
@@ -4308,7 +4311,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6" t="s">
@@ -4331,7 +4334,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6" t="s">
@@ -4354,7 +4357,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G56" s="6" t="s">
         <v>111</v>
@@ -4380,7 +4383,7 @@
         <v>116</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G57" s="6" t="s">
         <v>111</v>
@@ -4428,7 +4431,7 @@
         <v>3</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6" t="s">
@@ -4451,7 +4454,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6" t="s">
@@ -4465,7 +4468,7 @@
         <v>54</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>4</v>
@@ -4486,19 +4489,19 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E62" s="4" t="s">
+      <c r="F62" s="6" t="s">
         <v>607</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>608</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>111</v>
@@ -4520,7 +4523,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F63" s="8"/>
       <c r="G63" s="6" t="s">
@@ -4564,7 +4567,7 @@
         <v>3</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>128</v>
@@ -4589,7 +4592,7 @@
         <v>3</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>129</v>
@@ -4614,7 +4617,7 @@
         <v>3</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>131</v>
@@ -4639,7 +4642,7 @@
         <v>3</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6" t="s">
@@ -4683,10 +4686,10 @@
         <v>3</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G70" s="6" t="s">
         <v>111</v>
@@ -4750,7 +4753,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
@@ -4761,23 +4764,23 @@
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="B74" s="105" t="s">
+      <c r="B74" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="C74" s="106" t="s">
-        <v>4</v>
-      </c>
-      <c r="D74" s="105" t="s">
-        <v>3</v>
-      </c>
-      <c r="E74" s="105" t="s">
-        <v>532</v>
-      </c>
-      <c r="F74" s="107" t="s">
+      <c r="C74" s="96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="95" t="s">
+        <v>531</v>
+      </c>
+      <c r="F74" s="97" t="s">
         <v>110</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H74" s="6"/>
     </row>
@@ -4796,7 +4799,7 @@
         <v>3</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F75" s="6"/>
       <c r="G75" s="6" t="s">
@@ -4819,7 +4822,7 @@
         <v>3</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="6" t="s">
@@ -4842,7 +4845,7 @@
         <v>2</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
@@ -4863,7 +4866,7 @@
         <v>3</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="6" t="s">
@@ -4886,7 +4889,7 @@
         <v>3</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F79" s="6"/>
       <c r="G79" s="6" t="s">
@@ -4899,7 +4902,7 @@
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B80" s="108" t="s">
+      <c r="B80" s="98" t="s">
         <v>53</v>
       </c>
       <c r="C80" s="7" t="s">
@@ -4909,10 +4912,10 @@
         <v>3</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>111</v>
@@ -4923,7 +4926,7 @@
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="B81" s="108" t="s">
+      <c r="B81" s="98" t="s">
         <v>54</v>
       </c>
       <c r="C81" s="7" t="s">
@@ -4933,10 +4936,10 @@
         <v>3</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>111</v>
@@ -4948,7 +4951,7 @@
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B82" s="108" t="s">
+      <c r="B82" s="98" t="s">
         <v>55</v>
       </c>
       <c r="C82" s="7" t="s">
@@ -4958,10 +4961,10 @@
         <v>3</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G82" s="6" t="s">
         <v>111</v>
@@ -4983,7 +4986,7 @@
         <v>3</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F83" s="6"/>
       <c r="G83" s="6" t="s">
@@ -5006,7 +5009,7 @@
         <v>3</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="6" t="s">
@@ -5029,7 +5032,7 @@
         <v>3</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F85"/>
       <c r="G85" s="6" t="s">
@@ -5052,7 +5055,7 @@
         <v>3</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F86" s="16"/>
       <c r="G86" s="6" t="s">
@@ -5075,7 +5078,7 @@
         <v>2</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F87" s="15"/>
       <c r="G87" s="15"/>
@@ -5086,7 +5089,7 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B88" s="109" t="s">
+      <c r="B88" s="99" t="s">
         <v>59</v>
       </c>
       <c r="C88" s="7" t="s">
@@ -5096,10 +5099,10 @@
         <v>3</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>112</v>
@@ -5111,7 +5114,7 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B89" s="109" t="s">
+      <c r="B89" s="99" t="s">
         <v>60</v>
       </c>
       <c r="C89" s="7" t="s">
@@ -5121,11 +5124,11 @@
         <v>3</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H89" s="6"/>
     </row>
@@ -5144,10 +5147,10 @@
         <v>3</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -5165,11 +5168,11 @@
         <v>3</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F91" s="6"/>
       <c r="G91" s="6" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H91" s="6"/>
     </row>
@@ -5188,7 +5191,7 @@
         <v>2</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F92" s="14"/>
       <c r="G92" s="14"/>
@@ -5199,7 +5202,7 @@
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="B93" s="109" t="s">
+      <c r="B93" s="99" t="s">
         <v>71</v>
       </c>
       <c r="C93" s="7" t="s">
@@ -5209,10 +5212,10 @@
         <v>3</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>112</v>
@@ -5223,7 +5226,7 @@
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="B94" s="109" t="s">
+      <c r="B94" s="99" t="s">
         <v>64</v>
       </c>
       <c r="C94" s="7" t="s">
@@ -5233,10 +5236,10 @@
         <v>3</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>112</v>
@@ -5257,11 +5260,11 @@
         <v>3</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F95" s="6"/>
       <c r="G95" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -5279,11 +5282,11 @@
         <v>3</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -5302,7 +5305,7 @@
       </c>
       <c r="E97" s="4"/>
       <c r="G97" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -5320,11 +5323,11 @@
         <v>3</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F98" s="6"/>
       <c r="G98" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -5342,11 +5345,11 @@
         <v>3</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F99" s="6"/>
       <c r="G99" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -5368,7 +5371,7 @@
       </c>
       <c r="F100" s="16"/>
       <c r="G100" s="6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -5386,7 +5389,7 @@
         <v>2</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F101" s="15"/>
       <c r="G101" s="15"/>
@@ -5407,10 +5410,10 @@
         <v>3</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>112</v>
@@ -5432,10 +5435,10 @@
         <v>3</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>112</v>
@@ -5457,11 +5460,11 @@
         <v>3</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H104" s="6"/>
     </row>
@@ -5480,11 +5483,11 @@
         <v>3</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H105" s="6"/>
     </row>
@@ -5503,11 +5506,11 @@
         <v>3</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H106" s="6"/>
     </row>
@@ -5526,11 +5529,11 @@
         <v>3</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F107" s="6"/>
       <c r="G107" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H107" s="6"/>
     </row>
@@ -5549,11 +5552,11 @@
         <v>3</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H108" s="6"/>
     </row>
@@ -5562,7 +5565,7 @@
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="B109" s="109" t="s">
+      <c r="B109" s="99" t="s">
         <v>80</v>
       </c>
       <c r="C109" s="7" t="s">
@@ -5572,10 +5575,10 @@
         <v>3</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>112</v>
@@ -5597,11 +5600,11 @@
         <v>3</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H110" s="6"/>
     </row>
@@ -5620,10 +5623,10 @@
         <v>3</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H111" s="6"/>
     </row>
@@ -5643,7 +5646,7 @@
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G112" s="6" t="s">
         <v>112</v>
@@ -5667,7 +5670,7 @@
       <c r="E113" s="4"/>
       <c r="F113" s="6"/>
       <c r="G113" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H113" s="6"/>
     </row>
@@ -5686,11 +5689,11 @@
         <v>3</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F114" s="6"/>
       <c r="G114" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H114" s="6"/>
     </row>
@@ -5709,10 +5712,10 @@
         <v>3</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H115" s="6"/>
     </row>
@@ -5731,7 +5734,7 @@
         <v>2</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F116" s="14"/>
       <c r="G116" s="14"/>
@@ -5824,7 +5827,7 @@
         <v>3</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F120" s="6" t="s">
         <v>144</v>
@@ -5849,7 +5852,7 @@
         <v>3</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F121" s="6"/>
       <c r="G121" s="5" t="s">
@@ -5872,7 +5875,7 @@
         <v>3</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G122" s="5" t="s">
         <v>148</v>
@@ -5893,7 +5896,7 @@
         <v>3</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="5" t="s">
@@ -5940,7 +5943,7 @@
         <v>3</v>
       </c>
       <c r="E125" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F125" s="6" t="s">
         <v>146</v>
@@ -5964,7 +5967,7 @@
         <v>3</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G126" s="5" t="s">
         <v>148</v>
@@ -5985,7 +5988,7 @@
         <v>3</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G127" s="5" t="s">
         <v>148</v>
@@ -5997,7 +6000,7 @@
         <v>120</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C128" s="7" t="s">
         <v>4</v>
@@ -6017,19 +6020,19 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="F129" s="6" t="s">
         <v>609</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D129" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E129" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="F129" s="6" t="s">
-        <v>610</v>
       </c>
       <c r="G129" s="5" t="s">
         <v>112</v>
@@ -6050,7 +6053,7 @@
         <v>3</v>
       </c>
       <c r="E130" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F130" s="10"/>
       <c r="G130" s="5" t="s">
@@ -6169,134 +6172,134 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B1" s="55" t="s">
+        <v>367</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>368</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="74" t="s">
         <v>369</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="E1" s="76" t="s">
         <v>370</v>
       </c>
-      <c r="E1" s="76" t="s">
-        <v>371</v>
-      </c>
       <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
-        <v>477</v>
+      <c r="A2" s="106" t="s">
+        <v>476</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>117</v>
       </c>
       <c r="D2" s="37" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="107"/>
+      <c r="B3" s="43" t="s">
+        <v>483</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
+      <c r="B4" s="43" t="s">
+        <v>484</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="D4" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E4" s="62" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="107"/>
+      <c r="B5" s="43" t="s">
+        <v>485</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>374</v>
+      </c>
+      <c r="E5" s="60" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
-      <c r="B3" s="43" t="s">
-        <v>484</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>341</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>372</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="43" t="s">
-        <v>485</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>367</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>374</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
-      <c r="B5" s="43" t="s">
-        <v>486</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>375</v>
-      </c>
-      <c r="E5" s="60" t="s">
-        <v>381</v>
-      </c>
-    </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="43"/>
       <c r="C6" s="22"/>
       <c r="D6" s="51" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="44"/>
       <c r="C7" s="64"/>
       <c r="D7" s="52" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E7" s="61" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="50" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -6330,152 +6333,152 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B1" s="55" t="s">
+        <v>356</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>357</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="74" t="s">
         <v>358</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="E1" s="76" t="s">
         <v>359</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="F1" s="80" t="s">
         <v>360</v>
       </c>
-      <c r="F1" s="80" t="s">
-        <v>361</v>
-      </c>
       <c r="G1" s="56" t="s">
+        <v>354</v>
+      </c>
+      <c r="H1" s="59" t="s">
         <v>355</v>
       </c>
-      <c r="H1" s="59" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
-        <v>480</v>
+      <c r="A2" s="106" t="s">
+        <v>479</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>117</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F2" s="57" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G2" s="53"/>
       <c r="H2" s="60" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="107"/>
       <c r="B3" s="43" t="s">
+        <v>350</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>347</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>362</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>268</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>288</v>
+      </c>
+      <c r="H3" s="60" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
+      <c r="B4" s="43" t="s">
         <v>351</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C4" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>348</v>
-      </c>
-      <c r="E3" s="62" t="s">
+      <c r="D4" s="37" t="s">
+        <v>345</v>
+      </c>
+      <c r="E4" s="62" t="s">
         <v>363</v>
-      </c>
-      <c r="F3" s="57" t="s">
-        <v>269</v>
-      </c>
-      <c r="G3" s="53" t="s">
-        <v>289</v>
-      </c>
-      <c r="H3" s="60" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="43" t="s">
-        <v>352</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>346</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>364</v>
       </c>
       <c r="F4" s="57"/>
       <c r="G4" s="53"/>
       <c r="H4" s="60"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="43" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E5" s="62" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F5" s="57"/>
       <c r="G5" s="53"/>
       <c r="H5" s="60"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="97"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="44" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C6" s="64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E6" s="63" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="54"/>
       <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="97"/>
+      <c r="A7" s="107"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="97"/>
+      <c r="A8" s="107"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="97"/>
+      <c r="A9" s="107"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="98"/>
+      <c r="A10" s="108"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -6569,7 +6572,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
-      <c r="B22" s="102"/>
+      <c r="B22" s="112"/>
       <c r="C22" s="27"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
@@ -6582,7 +6585,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
-      <c r="B23" s="102"/>
+      <c r="B23" s="112"/>
       <c r="C23" s="27"/>
       <c r="D23" s="29"/>
       <c r="E23" s="29"/>
@@ -6595,7 +6598,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
-      <c r="B24" s="102"/>
+      <c r="B24" s="112"/>
       <c r="C24" s="27"/>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
@@ -6608,7 +6611,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
-      <c r="B25" s="102"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="27"/>
       <c r="D25" s="29"/>
       <c r="E25" s="29"/>
@@ -6621,7 +6624,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
-      <c r="B26" s="102"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="27"/>
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
@@ -6634,7 +6637,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
-      <c r="B27" s="102"/>
+      <c r="B27" s="112"/>
       <c r="C27" s="27"/>
       <c r="D27" s="29"/>
       <c r="E27" s="29"/>
@@ -6729,139 +6732,139 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>443</v>
-      </c>
-      <c r="B1" s="110" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="100" t="s">
+        <v>573</v>
+      </c>
+      <c r="C1" s="101" t="s">
         <v>574</v>
       </c>
-      <c r="C1" s="111" t="s">
+      <c r="D1" s="72" t="s">
         <v>575</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="E1" s="73" t="s">
         <v>576</v>
       </c>
-      <c r="E1" s="73" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="106" t="s">
+        <v>592</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>572</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>579</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="107"/>
+      <c r="B3" s="48" t="s">
+        <v>571</v>
+      </c>
+      <c r="C3" s="102" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
-        <v>593</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>579</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>573</v>
-      </c>
-      <c r="D2" s="37" t="s">
+      <c r="D3" s="37" t="s">
         <v>580</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E3" s="62" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
+      <c r="D4" s="37" t="s">
+        <v>581</v>
+      </c>
+      <c r="E4" s="62" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="107"/>
+      <c r="D5" s="37" t="s">
+        <v>582</v>
+      </c>
+      <c r="E5" s="62" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="97"/>
-      <c r="B3" s="48" t="s">
-        <v>572</v>
-      </c>
-      <c r="C3" s="112" t="s">
-        <v>578</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>581</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="D4" s="37" t="s">
-        <v>582</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
-      <c r="D5" s="37" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="107"/>
+      <c r="D6" s="37" t="s">
         <v>583</v>
       </c>
-      <c r="E5" s="62" t="s">
+      <c r="E6" s="62" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
-      <c r="D6" s="37" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="107"/>
+      <c r="D7" s="37" t="s">
         <v>584</v>
       </c>
-      <c r="E6" s="62" t="s">
+      <c r="E7" s="62" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="97"/>
-      <c r="D7" s="37" t="s">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="107"/>
+      <c r="D8" s="39" t="s">
         <v>585</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E8" s="63" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="97"/>
-      <c r="D8" s="39" t="s">
-        <v>586</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>592</v>
-      </c>
-    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="97"/>
+      <c r="A9" s="107"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="97"/>
+      <c r="A10" s="107"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="97"/>
+      <c r="A11" s="107"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="97"/>
+      <c r="A12" s="107"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="97"/>
+      <c r="A13" s="107"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="97"/>
+      <c r="A14" s="107"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="97"/>
+      <c r="A15" s="107"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
+      <c r="A16" s="107"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="98"/>
+      <c r="A17" s="108"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
@@ -6870,7 +6873,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="34" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
@@ -6908,37 +6911,37 @@
       <c r="L26" s="29"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I27" s="102"/>
+      <c r="I27" s="112"/>
       <c r="J27" s="29"/>
       <c r="K27" s="29"/>
       <c r="L27" s="29"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I28" s="102"/>
+      <c r="I28" s="112"/>
       <c r="J28" s="29"/>
       <c r="K28" s="29"/>
       <c r="L28" s="29"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I29" s="102"/>
+      <c r="I29" s="112"/>
       <c r="J29" s="29"/>
       <c r="K29" s="29"/>
       <c r="L29" s="29"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I30" s="102"/>
+      <c r="I30" s="112"/>
       <c r="J30" s="29"/>
       <c r="K30" s="29"/>
       <c r="L30" s="29"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I31" s="102"/>
+      <c r="I31" s="112"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I32" s="102"/>
+      <c r="I32" s="112"/>
       <c r="J32" s="29"/>
       <c r="K32" s="29"/>
       <c r="L32" s="29"/>
@@ -7016,111 +7019,111 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B1" s="72" t="s">
+        <v>384</v>
+      </c>
+      <c r="C1" s="73" t="s">
         <v>385</v>
       </c>
-      <c r="C1" s="73" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
+        <v>449</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>383</v>
+      </c>
+      <c r="C2" s="62" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
-        <v>450</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>384</v>
-      </c>
-      <c r="C2" s="62" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="104"/>
+      <c r="B3" s="37" t="s">
         <v>387</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="37" t="s">
-        <v>388</v>
       </c>
       <c r="C3" s="62" t="s">
         <v>129</v>
       </c>
       <c r="F3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
+      <c r="A4" s="104"/>
       <c r="B4" s="37" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="104"/>
+      <c r="B5" s="37" t="s">
         <v>394</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C5" s="62" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="94"/>
-      <c r="B5" s="37" t="s">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="104"/>
+      <c r="B6" s="37" t="s">
         <v>395</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C6" s="62" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="104"/>
+      <c r="B7" s="37" t="s">
+        <v>397</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>319</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="104"/>
+      <c r="B8" s="37" t="s">
+        <v>398</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>320</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="104"/>
+      <c r="B9" s="37" t="s">
+        <v>396</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="104"/>
+      <c r="B10" s="37" t="s">
+        <v>392</v>
+      </c>
+      <c r="C10" s="62" t="s">
         <v>314</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="94"/>
-      <c r="B6" s="37" t="s">
-        <v>396</v>
-      </c>
-      <c r="C6" s="62" t="s">
-        <v>316</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="94"/>
-      <c r="B7" s="37" t="s">
-        <v>398</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>320</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="94"/>
-      <c r="B8" s="37" t="s">
-        <v>399</v>
-      </c>
-      <c r="C8" s="62" t="s">
-        <v>321</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
-      <c r="B9" s="37" t="s">
-        <v>397</v>
-      </c>
-      <c r="C9" s="62" t="s">
-        <v>317</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="94"/>
-      <c r="B10" s="37" t="s">
-        <v>393</v>
-      </c>
-      <c r="C10" s="62" t="s">
-        <v>315</v>
-      </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="37" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C11" s="62" t="s">
         <v>141</v>
@@ -7128,218 +7131,218 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="37" t="s">
+        <v>399</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>317</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="104"/>
+      <c r="B13" s="37" t="s">
         <v>400</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C13" s="62" t="s">
         <v>318</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
-      <c r="B13" s="37" t="s">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="104"/>
+      <c r="B14" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="C13" s="62" t="s">
-        <v>319</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="94"/>
-      <c r="B14" s="37" t="s">
+      <c r="C14" s="62" t="s">
+        <v>321</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="104"/>
+      <c r="B15" s="37" t="s">
         <v>402</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C15" s="62" t="s">
         <v>322</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="94"/>
-      <c r="B15" s="37" t="s">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="104"/>
+      <c r="B16" s="37" t="s">
         <v>403</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C16" s="62" t="s">
+        <v>324</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="104"/>
+      <c r="B17" s="37" t="s">
+        <v>404</v>
+      </c>
+      <c r="C17" s="62" t="s">
         <v>323</v>
       </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="94"/>
-      <c r="B16" s="37" t="s">
-        <v>404</v>
-      </c>
-      <c r="C16" s="62" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="104"/>
+      <c r="B18" s="37" t="s">
+        <v>405</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>338</v>
+      </c>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="104"/>
+      <c r="B19" s="37" t="s">
+        <v>406</v>
+      </c>
+      <c r="C19" s="62" t="s">
+        <v>337</v>
+      </c>
+      <c r="D19" s="28"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="104"/>
+      <c r="B20" s="37" t="s">
+        <v>407</v>
+      </c>
+      <c r="C20" s="62" t="s">
+        <v>328</v>
+      </c>
+      <c r="D20" s="28"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="104"/>
+      <c r="B21" s="37" t="s">
+        <v>408</v>
+      </c>
+      <c r="C21" s="62" t="s">
+        <v>330</v>
+      </c>
+      <c r="D21" s="29"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="104"/>
+      <c r="B22" s="37" t="s">
+        <v>409</v>
+      </c>
+      <c r="C22" s="62" t="s">
+        <v>329</v>
+      </c>
+      <c r="D22" s="29"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="104"/>
+      <c r="B23" s="37" t="s">
+        <v>412</v>
+      </c>
+      <c r="C23" s="62" t="s">
         <v>325</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="94"/>
-      <c r="B17" s="37" t="s">
-        <v>405</v>
-      </c>
-      <c r="C17" s="62" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
-      <c r="B18" s="37" t="s">
-        <v>406</v>
-      </c>
-      <c r="C18" s="62" t="s">
-        <v>339</v>
-      </c>
-      <c r="D18" s="28"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
-      <c r="B19" s="37" t="s">
-        <v>407</v>
-      </c>
-      <c r="C19" s="62" t="s">
-        <v>338</v>
-      </c>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="94"/>
-      <c r="B20" s="37" t="s">
-        <v>408</v>
-      </c>
-      <c r="C20" s="62" t="s">
-        <v>329</v>
-      </c>
-      <c r="D20" s="28"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="94"/>
-      <c r="B21" s="37" t="s">
-        <v>409</v>
-      </c>
-      <c r="C21" s="62" t="s">
+      <c r="D23" s="29"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="104"/>
+      <c r="B24" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="C24" s="62" t="s">
+        <v>327</v>
+      </c>
+      <c r="D24" s="29"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="104"/>
+      <c r="B25" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="C25" s="62" t="s">
+        <v>326</v>
+      </c>
+      <c r="D25" s="29"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="104"/>
+      <c r="B26" s="37" t="s">
+        <v>413</v>
+      </c>
+      <c r="C26" s="62" t="s">
         <v>331</v>
       </c>
-      <c r="D21" s="29"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="94"/>
-      <c r="B22" s="37" t="s">
-        <v>410</v>
-      </c>
-      <c r="C22" s="62" t="s">
-        <v>330</v>
-      </c>
-      <c r="D22" s="29"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="94"/>
-      <c r="B23" s="37" t="s">
-        <v>413</v>
-      </c>
-      <c r="C23" s="62" t="s">
-        <v>326</v>
-      </c>
-      <c r="D23" s="29"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="94"/>
-      <c r="B24" s="37" t="s">
-        <v>412</v>
-      </c>
-      <c r="C24" s="62" t="s">
-        <v>328</v>
-      </c>
-      <c r="D24" s="29"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="94"/>
-      <c r="B25" s="37" t="s">
-        <v>411</v>
-      </c>
-      <c r="C25" s="62" t="s">
-        <v>327</v>
-      </c>
-      <c r="D25" s="29"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="94"/>
-      <c r="B26" s="37" t="s">
+      <c r="D26" s="29"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="104"/>
+      <c r="B27" s="37" t="s">
         <v>414</v>
       </c>
-      <c r="C26" s="62" t="s">
+      <c r="C27" s="62" t="s">
+        <v>336</v>
+      </c>
+      <c r="D27" s="29"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="104"/>
+      <c r="B28" s="37" t="s">
+        <v>415</v>
+      </c>
+      <c r="C28" s="62" t="s">
+        <v>333</v>
+      </c>
+      <c r="D28" s="29"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="104"/>
+      <c r="B29" s="37" t="s">
+        <v>416</v>
+      </c>
+      <c r="C29" s="62" t="s">
         <v>332</v>
       </c>
-      <c r="D26" s="29"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="94"/>
-      <c r="B27" s="37" t="s">
-        <v>415</v>
-      </c>
-      <c r="C27" s="62" t="s">
-        <v>337</v>
-      </c>
-      <c r="D27" s="29"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="94"/>
-      <c r="B28" s="37" t="s">
-        <v>416</v>
-      </c>
-      <c r="C28" s="62" t="s">
+      <c r="D29" s="29"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="104"/>
+      <c r="B30" s="37" t="s">
+        <v>417</v>
+      </c>
+      <c r="C30" s="62" t="s">
         <v>334</v>
       </c>
-      <c r="D28" s="29"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="94"/>
-      <c r="B29" s="37" t="s">
-        <v>417</v>
-      </c>
-      <c r="C29" s="62" t="s">
-        <v>333</v>
-      </c>
-      <c r="D29" s="29"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="94"/>
-      <c r="B30" s="37" t="s">
+      <c r="D30" s="29"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="104"/>
+      <c r="B31" s="39" t="s">
         <v>418</v>
       </c>
-      <c r="C30" s="62" t="s">
+      <c r="C31" s="63" t="s">
         <v>335</v>
       </c>
-      <c r="D30" s="29"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="94"/>
-      <c r="B31" s="39" t="s">
-        <v>419</v>
-      </c>
-      <c r="C31" s="63" t="s">
-        <v>336</v>
-      </c>
       <c r="D31" s="29"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="94"/>
+      <c r="A32" s="104"/>
       <c r="D32" s="29"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
+      <c r="A33" s="104"/>
       <c r="D33" s="29"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="94"/>
+      <c r="A34" s="104"/>
       <c r="D34" s="29"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="95"/>
+      <c r="A35" s="105"/>
       <c r="D35" s="28"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -7363,8 +7366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27473039-7BF5-41BD-AAFA-F14B86FDFC50}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7378,47 +7381,50 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="81" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
         <v>443</v>
       </c>
-      <c r="B1" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="81" t="s">
-        <v>178</v>
-      </c>
-      <c r="D1" s="79" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" s="20"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
-        <v>444</v>
-      </c>
       <c r="B2" s="25" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C2" s="89" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
+      <c r="A3" s="104"/>
       <c r="B3" s="25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C3" s="89" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" s="90" t="s">
-        <v>171</v>
+        <v>612</v>
+      </c>
+      <c r="E3" t="s">
+        <v>613</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
+      <c r="A4" s="104"/>
       <c r="B4" s="25" t="s">
         <v>170</v>
       </c>
@@ -7430,19 +7436,19 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="94"/>
+      <c r="A5" s="104"/>
       <c r="B5" s="25" t="s">
         <v>167</v>
       </c>
       <c r="C5" s="89" t="s">
+        <v>610</v>
+      </c>
+      <c r="D5" s="90" t="s">
         <v>611</v>
       </c>
-      <c r="D5" s="90" t="s">
-        <v>612</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="94"/>
+      <c r="A6" s="104"/>
       <c r="B6" s="25" t="s">
         <v>164</v>
       </c>
@@ -7454,7 +7460,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="94"/>
+      <c r="A7" s="104"/>
       <c r="B7" s="25" t="s">
         <v>161</v>
       </c>
@@ -7466,7 +7472,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="94"/>
+      <c r="A8" s="104"/>
       <c r="B8" s="25" t="s">
         <v>158</v>
       </c>
@@ -7478,7 +7484,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="25" t="s">
         <v>155</v>
       </c>
@@ -7490,7 +7496,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="94"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="25" t="s">
         <v>154</v>
       </c>
@@ -7499,7 +7505,7 @@
       <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="25" t="s">
         <v>153</v>
       </c>
@@ -7507,7 +7513,7 @@
       <c r="D11" s="38"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="25" t="s">
         <v>152</v>
       </c>
@@ -7515,7 +7521,7 @@
       <c r="D12" s="38"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="25" t="s">
         <v>151</v>
       </c>
@@ -7523,7 +7529,7 @@
       <c r="D13" s="38"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="94"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="25" t="s">
         <v>150</v>
       </c>
@@ -7531,7 +7537,7 @@
       <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="95"/>
+      <c r="A15" s="105"/>
       <c r="B15" s="88" t="s">
         <v>149</v>
       </c>
@@ -7540,24 +7546,24 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C16" s="84"/>
       <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7590,205 +7596,205 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B1" s="85" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="104" t="s">
+        <v>448</v>
+      </c>
+      <c r="B2" s="86" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="104"/>
+      <c r="B3" s="86" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="104"/>
+      <c r="B4" s="86" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D4" s="83" t="s">
+        <v>227</v>
+      </c>
+      <c r="E4" s="62" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="104"/>
+      <c r="B5" s="86" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="D1" s="81" t="s">
-        <v>231</v>
-      </c>
-      <c r="E1" s="76" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
-        <v>449</v>
-      </c>
-      <c r="B2" s="86" t="s">
-        <v>200</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="D2" s="82" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="62" t="s">
-        <v>221</v>
-      </c>
-      <c r="G2" s="17"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="86" t="s">
-        <v>216</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="C5" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="D3" s="83" t="s">
-        <v>227</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="94"/>
-      <c r="B4" s="86" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="D4" s="83" t="s">
+      <c r="D5" s="83" t="s">
         <v>228</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E5" s="62" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="104"/>
+      <c r="B6" s="86" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="83" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="62" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="94"/>
-      <c r="B5" s="86" t="s">
-        <v>204</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="83" t="s">
-        <v>229</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="94"/>
-      <c r="B6" s="86" t="s">
-        <v>209</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" s="83" t="s">
-        <v>230</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>224</v>
-      </c>
-    </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="94"/>
+      <c r="A7" s="104"/>
       <c r="B7" s="86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="83"/>
       <c r="E7" s="62"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="94"/>
+      <c r="A8" s="104"/>
       <c r="B8" s="86" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D8" s="83"/>
       <c r="E8" s="62"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="86" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D9" s="83"/>
       <c r="E9" s="62"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="94"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10" s="83"/>
       <c r="E10" s="62"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="86" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D11" s="83"/>
       <c r="E11" s="62"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="86" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D12" s="83"/>
       <c r="E12" s="62"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="86" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="62"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="94"/>
+      <c r="A14" s="104"/>
       <c r="B14" s="86" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D14" s="83"/>
       <c r="E14" s="62"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="94"/>
+      <c r="A15" s="104"/>
       <c r="B15" s="86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D15" s="83"/>
       <c r="E15" s="62"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="94"/>
+      <c r="A16" s="104"/>
       <c r="B16" s="86" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D16" s="83"/>
       <c r="E16" s="62"/>
@@ -7798,12 +7804,12 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="94"/>
+      <c r="A17" s="104"/>
       <c r="B17" s="86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D17" s="83"/>
       <c r="E17" s="62"/>
@@ -7813,12 +7819,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
+      <c r="A18" s="104"/>
       <c r="B18" s="86" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D18" s="83"/>
       <c r="E18" s="62"/>
@@ -7828,12 +7834,12 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
+      <c r="A19" s="104"/>
       <c r="B19" s="86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19" s="83"/>
       <c r="E19" s="62"/>
@@ -7843,12 +7849,12 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="95"/>
+      <c r="A20" s="105"/>
       <c r="B20" s="87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D20" s="84"/>
       <c r="E20" s="63"/>
@@ -7859,22 +7865,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="34" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>
@@ -7903,61 +7909,61 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B1" s="55" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>234</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
-        <v>452</v>
+      <c r="A2" s="106" t="s">
+        <v>451</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="107"/>
       <c r="B3" s="43" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" s="22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
+      <c r="B4" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="108"/>
+      <c r="B5" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="64" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="43" t="s">
-        <v>210</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="98"/>
-      <c r="B5" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7978,7 +7984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098C817-F491-46B8-ACCD-892895410AE2}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -7991,149 +7997,149 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B1" s="71" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="106" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
-        <v>458</v>
-      </c>
-      <c r="B2" s="69" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="107"/>
+      <c r="B3" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
+      <c r="B4" s="43" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="107"/>
+      <c r="B5" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="107"/>
+      <c r="B6" s="43" t="s">
         <v>258</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
-      <c r="B3" s="43" t="s">
-        <v>249</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="43" t="s">
-        <v>251</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
-      <c r="B5" s="43" t="s">
+      <c r="C6" s="22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="107"/>
+      <c r="B7" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="107"/>
+      <c r="B8" s="43" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="107"/>
+      <c r="B9" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
-      <c r="B6" s="43" t="s">
-        <v>259</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="97"/>
-      <c r="B7" s="43" t="s">
-        <v>260</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="97"/>
-      <c r="B8" s="43" t="s">
-        <v>261</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="C9" s="22" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="97"/>
-      <c r="B9" s="43" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="107"/>
+      <c r="B10" s="43" t="s">
         <v>253</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C10" s="22" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="97"/>
-      <c r="B10" s="43" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="107"/>
+      <c r="B11" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C11" s="22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="97"/>
-      <c r="B11" s="43" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="107"/>
+      <c r="B12" s="43" t="s">
         <v>255</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C12" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="97"/>
-      <c r="B12" s="43" t="s">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="107"/>
+      <c r="B13" s="44" t="s">
         <v>256</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C13" s="64" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="97"/>
-      <c r="B13" s="44" t="s">
-        <v>257</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>248</v>
-      </c>
-    </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="98"/>
+      <c r="A14" s="108"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B18" s="70"/>
     </row>
@@ -8165,22 +8171,22 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B1" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" s="75" t="s">
         <v>279</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>277</v>
-      </c>
-      <c r="D1" s="74" t="s">
-        <v>278</v>
-      </c>
-      <c r="E1" s="75" t="s">
+      <c r="F1" s="76" t="s">
         <v>280</v>
-      </c>
-      <c r="F1" s="76" t="s">
-        <v>281</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -8194,21 +8200,21 @@
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
-        <v>460</v>
+      <c r="A2" s="109" t="s">
+        <v>459</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E2" s="66"/>
       <c r="F2" s="62" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -8222,21 +8228,21 @@
       <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
+      <c r="A3" s="110"/>
       <c r="B3" s="47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E3" s="66" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F3" s="62" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -8250,21 +8256,21 @@
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="100"/>
+      <c r="A4" s="110"/>
       <c r="B4" s="47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E4" s="66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F4" s="62" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -8278,21 +8284,21 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="100"/>
+      <c r="A5" s="110"/>
       <c r="B5" s="47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E5" s="66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F5" s="62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -8306,21 +8312,21 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="100"/>
+      <c r="A6" s="110"/>
       <c r="B6" s="47" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E6" s="66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F6" s="62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -8334,21 +8340,21 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="48" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>267</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>272</v>
+      </c>
+      <c r="E7" s="67" t="s">
         <v>287</v>
       </c>
-      <c r="C7" s="64" t="s">
-        <v>268</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>273</v>
-      </c>
-      <c r="E7" s="67" t="s">
-        <v>288</v>
-      </c>
       <c r="F7" s="63" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -8362,7 +8368,7 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="100"/>
+      <c r="A8" s="110"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -8378,7 +8384,7 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="100"/>
+      <c r="A9" s="110"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -8391,7 +8397,7 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="101"/>
+      <c r="A10" s="111"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -8405,7 +8411,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -8420,7 +8426,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -8435,7 +8441,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -8450,7 +8456,7 @@
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -8492,109 +8498,109 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B1" s="55" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="74" t="s">
         <v>303</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="E1" s="77" t="s">
         <v>304</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="F1" s="76" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="106" t="s">
+        <v>463</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>305</v>
       </c>
-      <c r="F1" s="76" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
-        <v>464</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>306</v>
-      </c>
       <c r="C2" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E2" s="23"/>
       <c r="F2" s="62" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
+      <c r="A3" s="107"/>
       <c r="B3" s="47" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>268</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
+      <c r="B4" s="47" t="s">
         <v>307</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C4" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>289</v>
-      </c>
-      <c r="F3" s="62" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="47" t="s">
+      <c r="D4" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="107"/>
+      <c r="B5" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C5" s="64" t="s">
         <v>298</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D5" s="39" t="s">
         <v>300</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>288</v>
-      </c>
-      <c r="F4" s="62" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="97"/>
-      <c r="B5" s="48" t="s">
-        <v>309</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>299</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>301</v>
-      </c>
       <c r="E5" s="65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F5" s="63" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -8602,7 +8608,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="45" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -8610,7 +8616,7 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -8640,108 +8646,108 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="36" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B1" s="55" t="s">
+        <v>420</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>419</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>426</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="106" t="s">
+        <v>468</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>388</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>421</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>420</v>
-      </c>
-      <c r="D1" s="74" t="s">
+      <c r="D2" s="37" t="s">
+        <v>432</v>
+      </c>
+      <c r="E2" s="62" t="s">
         <v>427</v>
       </c>
-      <c r="E1" s="76" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
-        <v>469</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>389</v>
-      </c>
-      <c r="C2" s="22" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="107"/>
+      <c r="B3" s="43" t="s">
+        <v>430</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>422</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D3" s="37" t="s">
         <v>433</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E3" s="62" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
+      <c r="B4" s="43" t="s">
+        <v>431</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>423</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>434</v>
+      </c>
+      <c r="E4" s="62" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
-      <c r="B3" s="43" t="s">
-        <v>431</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>423</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>434</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="43" t="s">
-        <v>432</v>
-      </c>
-      <c r="C4" s="22" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="107"/>
+      <c r="B5" s="43" t="s">
+        <v>390</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>424</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>435</v>
-      </c>
-      <c r="E4" s="62" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
-      <c r="B5" s="43" t="s">
-        <v>391</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>425</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="62"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="98"/>
+      <c r="A6" s="108"/>
       <c r="B6" s="44" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C6" s="64" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="63"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="78" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -8886,18 +8892,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8919,6 +8925,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61B3F181-E7E1-4FBA-8814-FA691E66D479}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0C5842A-C8ED-4FB1-AB1C-EB0747C5F625}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -8932,12 +8946,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61B3F181-E7E1-4FBA-8814-FA691E66D479}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>